<commit_message>
Add evaluation script and server notification functionality
- Created `evaluate_model.py` to evaluate model performance using DeepEval, including loading configurations, processing questions, and saving evaluation results to Excel.
- Updated `request_LLM.py` to remove excessive output from a specific section.
- Added `serverchan.py` for sending notifications via Server酱, including dynamic URL construction based on SENDKEY format.
</commit_message>
<xml_diff>
--- a/QA/deepseek/deepseek-r1_answers.xlsx
+++ b/QA/deepseek/deepseek-r1_answers.xlsx
@@ -483,7 +483,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -509,15 +509,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>嗯，用户问的是如何从单粒子运动轨迹理论出发，推导并解释磁镜约束的基本原理，以及对聚变装置设计的意义，同时讨论绝热不变量的作用和失效条件。作为聚变等离子体物理专家，我得先理清这些概念。
-首先，磁镜约束是一种利用磁场来限制等离子体的方法。单粒子轨迹理论是研究带电粒子在磁场中运动的基础，所以我要从这里入手。单粒子的运动方程包括洛伦兹力的影响，我记得磁场的梯度变化会影响粒子的轨迹。
-接下来，用户提到了绝热不变量，这在磁镜约束中起关键作用。绝热不变量意味着在缓慢变化的磁场中，某些物理量保持不变，比如磁通量。这在维持粒子约束方面非常重要。不过，当磁场变化过快或者粒子能量过高时，绝热近似就会失效，导致粒子逃逸。
-用户可能还希望了解磁镜在聚变装置中的设计意义。比如说，设计磁镜装置时需要考虑磁场梯度、镜比等因素，以优化约束性能。同时，选择合适的材料和诊断手段也是确保装置高效运行的重要方面。
-再考虑用户可能的深层需求，他们可能正在研究磁镜装置的设计或优化，想了解其中的物理原理和工程实现。因此，我在回答时需要结合理论推导和工程应用，提供具体的建议和参数分析。
-在思考过程中，我还需要确保回答结构清晰，遵循用户提供的答题规范，逐步展开背景、原理推导、定量估算、工程意义、比较拓展和要点总结。同时，语言要严谨，避免猜测，必要时指出需要进一步的信息或假设。
-最后，我需要确保各部分内容连贯，从单粒子轨迹理论引出磁镜约束，再讨论绝热不变量及其失效条件，最后总结对装置设计的意义，帮助用户全面理解这一主题。
-&lt;/think&gt;
-### **核心结论**  
+          <t>### **核心结论**  
 磁镜约束通过磁场梯度变化引导粒子运动，利用绝热不变量限制粒子逃逸，从而实现等离子体的约束；然而，当粒子能量过高或磁场变化过快时，绝热不变量失效，导致粒子逃逸。
 ---
 ### **背景与概念**  
@@ -581,7 +573,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -607,47 +599,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>嗯，我现在得仔细想一下这个问题。首先，用户想推导均匀磁化冷等离子体中平行传播的右旋和左旋圆偏振电磁波的色散关系。然后，用托卡马克的典型参数估算电子和离子的回旋频率，最后讨论ECRH和ICRH用了哪种波的共振特性。
-首先，关于色散关系。均匀磁化等离子体中的波传播，通常会考虑波矢k与磁场B0平行的情况。这种情况下，波可以分为右旋（R波）和左旋（L波）。记得等离子体的色散关系涉及到波的频率和波矢的关系，通常使用波的电场分解为平行和垂直于磁场的分量来分析。
-公式的话，应该从波动方程出发，假设磁场均匀且静态，电场满足一定的波动方程。对于冷等离子体，忽略热运动的影响，所以可以用冷等离子体的近似。磁化等离子体的响应可以用介电张量来描述，其中介电常数分为平行和垂直于磁场的分量。
-然后，当波平行传播时，电场会有两个极化方向，一个平行于磁场，另一个垂直。这种情况下，R波和L波分别对应不同的极化模式。我记得，R波的频率会高于电子回旋频率，而L波则会低于。这可能跟波的传播方向和极化方向有关。
-接下来，得具体写出色散方程。假设波矢k与B0平行，那么波的频率ω满足色散关系：
-对于R波，色散关系是：
-ω² = ω_e² + ω_c² + k²c² + ... ？或者是不是更简单的情况，因为平行传播可能有特定的解。
-抱歉，可能有点迷糊。那正确的色散方程应该是怎样的呢？我记得在均匀磁化等离子体中，沿磁力线传播的波有两种模式：快波和慢波。快波的频率较高，而慢波较低。不过这里用户提到了右旋和左旋圆偏振波，可能这两种波对应不同的极化模式。
-或者是这样：沿磁传播的圆偏振波，其色散关系涉及到电子回旋频率和光速等因素。色散方程应该是：
-(ω² - v_B^2 k²)(ω² - v_B^2 k² - ω_c²) = 0
-其中v_B是磁速，等于c / sqrt(μ_0 ε_0)，但更准确地说，应该是v_B = c / sqrt(μ_r μ_0 ε_0)，但这里等离子体是冷的，所以μ_r=1，所以v_B=c。这可能不对，因为冷等离子体的波速可能不是这样。
-或者，另一种方法，使用等离子体的介电常数张量。对于平行传播的波，介电张量在垂直平面和传播方向上会有不同的表达式。然后，色散方程是从介电张量的行列式等于零得到的。
-假设电场的分量为E_z和E_perp（垂直于B的方向）。在平行传播的情况下，E_z对应的是L波，而E_perp对应的是R波或者相反？可能需要再理清楚。
-或者，正确的色散关系是：
-对于R波，ω² = ω_c² + k² c²
-而L波的情况呢？可能L波的色散关系不同，或者是否要考虑静磁近似？
-抱歉，可能需要重新梳理一下。冷磁化等离子体中，电磁波沿磁场传播，分为快波和慢波两种模式。快波的频率较高，与电子回旋频率有关，慢波频率较低。这两种模式对应的极化可能与波的旋转方向有关。
-哦，对了，右旋圆偏振波和左旋圆偏振波可能对应于快波和慢波。因此，它们的色散关系应该是：
-快波（R波）：ω² = ω_c² + (k c)^2 + (k c_e)^2？ 这可能不正确。或者，更准确地说，快波的色散关系是ω² = (ω_c² + (k c)^2)，而慢波则是ω² = (k c_e)^2，其中c_e是等离子体频率对应的波速。这可能更合理。
-那等离子体频率ω_p的平方是n e² / (ε_0 m_e)，而电子回旋频率ω_c是 e B / (m_e c)。然后，色散关系可以写成：
-(ω² - k² c²)(ω² - ω_c²) = ω_p^4 / (4 c² k²)
-或者，另一种形式，具体得再仔细计算一下。
-或者，考虑波的电场分为两个分量，一个平行于B，另一个垂直。在平行传播的情况下，当电场平行于B时，对应的是低频模式，而电场垂直于B则对应高频模式。
-快波的色散关系是ω² = ω_c² + (k c)^2，而慢波的色散关系则是ω² = (k c_e)^2，其中c_e是等离子体的声速或者其他？ 这可能需要更详细的计算。
-哦，对了，等离子体的波通常满足：
-(ω^2 - (k c)^2)(ω^2 - k^2 v_A^2) = ω_p^4
-其中v_A是磁声速，v_A² = B²/(μ_0 ρ)，而ρ是等离子体的密度。这可能适用于等离子体中的磁压缩波和磁剪切波的情况，但具体在冷等离子体中，可能有所不同。
-但用户的问题是关于电磁波，特别是右旋和左旋圆偏振波，所以可能需要用更详细的方式来推导。
-另外，我需要记住，当波沿着B传播时，电场和磁场的极化情况如何。右旋和左旋可能对应于特定的相位关系，从而影响色散关系。
-或许，更简便的方法是考虑R波和L波分别对应于快波和慢波，其色散关系分别为：
-ω = sqrt(ω_c² + k² c²) 和 ω = k v_e，其中v_e是等离子体频率对应的波速。
-不过，可能需要重新计算，从波动方程出发，建立色散关系。
-总之，可能需要通过建立介电张量，求解行列式，得到色散方程，然后解出两种模式的频率表达式。
-接下来，估算电子和离子的回旋频率。给定的参数是B0=2 T，ne=5e19 m^-3。
-电子回旋频率ω_ce = e B0/(m_e c)，计算其值。离子回旋频率ω_ci = e B0/(m_i c)，其中m_i假设为质子的质量，即m_p≈1.67e-27 kg。计算两者的频率，并将它们转换为GHz或其他常用单位，以便比较。
-然后，讨论ECRH和ICRH使用的波的类型。ECRH通常利用电子回旋共振，可能需要在高频率下，比如与电子回旋频率相匹配，而ICRH则利用离子的回旋共振，频率相对较低。
-回到色散关系，ECRH和ICRH分别对应不同波的共振条件。比如，ECRH可能利用快波（R波）的共振，因为快波的频率更高，接近电子回旋频率，而ICRH则可能利用慢波（L波）的共振，频率接近离子回旋频率。
-不过，这可能需要更详细的分析，特别是考虑波的类型和它们如何与回旋频率匹配。
-综上所述，我需要先推导出R波和L波的色散关系，然后使用给定参数计算回旋频率，并讨论ECRH和ICRH的应用情况。
-&lt;/think&gt;
-### 推导均匀磁化冷等离子体中平行传播的R波和L波的色散关系
+          <t>### 推导均匀磁化冷等离子体中平行传播的R波和L波的色散关系
 #### 背景与概念
 在均匀磁化冷等离子体中，电磁波沿磁场方向传播时，会出现两种极化的模式：右旋圆偏振波（R波）和左旋圆偏振波（L波）。这些波的传播特性由等离子体的磁化性质决定，可以通过波动方程推导出它们的色散关系。
 #### 原理与推导
@@ -708,7 +660,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -734,14 +686,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>嗯，用户让我估算Spitzer电阻率在典型托卡马克参数下的值，还要讨论经典电阻占环电压的比例，以及引出反常电阻的概念。首先，我需要回忆一下Spitzer电阻率的公式。记得Spitzer模型是基于等离子体中电子-离子碰撞的电阻率，公式应该是ρ = (m_e c² Z_eff n_e)^{-1}，其中m_e是电子质量，c是光速，n_e是电子密度，Z_eff是有效电荷数。对吧？
-然后，代入给定的参数：Te=5 keV，ne=1e20 m^-3，Zeff=2。计算的时候要注意单位，Te虽然给了，但在Spitzer公式里可能不需要用到，因为它是假设热力学极限的情况。那是不是可以直接代入参数计算呢？
-接下来，计算的时候，m_e c²是电子的静止能量，大约0.511 MeV。Z_eff是2，ne是1e20，单位要转换一下，比如转成m^-3。然后用公式代入，计算电阻率。计算结果应该是大约1e-4 Ohm·m，这似乎和典型的等离子体电阻率相符。
-然后，讨论经典电阻占环电压的比例。环电压V环大约在托卡马克中是几伏特左右，比如 ITER 设计的环电压是约1伏。经典电阻产生的电压降V_classic可以用V=IR，其中I是环向电流，比如5 MA，R是托卡马克的半径，比如R=5米。那电阻率ρ乘以电流I，再除以半径R，得到电压降。比如ρ=1e-4，I=5e6 A，R=5，得到V=1e-4 *5e6 /5 =0.1伏。这样，经典电阻贡献的电压只有0.1伏，而实际环电压是1伏，说明还有其他因素，比如反常电阻，导致了大部分电压降。
-所以，反常电阻的概念是由于等离子体中的微湍流或其他非经典效应，使得电阻率比Spitzer模型预测的要高得多。这通常出现在托卡马克的高约束模式（H-mode）中，边缘区域的反常电阻显著增加，导致大部分环电压用于驱动电流。
-总结一下，步骤是先计算Spitzer电阻率，然后估算经典电阻贡献的电压，发现与实验不符，进而引出反常电阻。这样用户的需求就得到了满足。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 在典型托卡马克等离子体参数下，Spitzer电阻率的值约为 $10^{-4} \, \Omega \cdot \text{m}$。经典电阻的贡献通常仅占环电压的约 $10\%$，其余 $90\%$ 由反常电阻贡献，这引出了反常电阻的概念。
 ---
 ### 背景与概念  
@@ -801,7 +746,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -827,17 +772,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>好，我现在需要回答关于反常输运以及离子温度梯度模（ITG）的问题。首先，我得理解什么是反常输运，它在聚变等离子体中的重要性。反常输运指的是超出经典扩散范围的输运现象，这意味着它不是由简单的粒子碰撞引起的，而是更复杂的微扰动导致的。这在托卡马克装置中非常重要，因为它直接影响到等离子体的约束性能，进而影响聚变反应的效率和持续性。
-接下来，用户详细讨论了ITG作为主要的微观不稳定性如何驱动反常输运。我需要详细阐述ITG的线性增长和非线性饱和机制。首先，线性增长部分，我应该介绍ITG的性质，比如它是在什么条件下激发的，涉及的等离子体参数，如温度梯度、密度梯度、磁场梯度等。然后，给出相关的波动方程，说明驱动这种不稳定的物理机制。
-在推导过程中，我需要列出关键的假设条件，例如磁流体力学的近似、忽略某些高阶效应等。这些假设能够简化方程，使其更易于分析，同时保持主要的物理现象。在推导波动方程时，我需要明确各个符号的含义，如波动电场、磁场、等离子体的响应函数等。
-接下来，讨论不稳定的增长率。通过对方程进行线性分析，可以得到增长率为γ，这个增长率为正数时，意味着ITG不稳定性被激发。增长率为γ与温度梯度的平方成正比，说明温度梯度越大，不稳定性越强，输运也越严重。同时，增长率与磁场梯度、离子迁移率等参数相关，需要给出具体的表达式和符号定义。
-然后，进入非线性饱和机制。在线性阶段，不稳定性不断增长，但当达到一定程度时，非线性效应开始发挥作用，导致饱和。非线性饱和机制通常涉及波动与等离子体之间的相互作用，可能包括自洽的改变等离子体参数，如温度梯度，从而减缓进一步的增长。在分析中，我需要介绍常见的饱和机制，比如ITG的非线性级联和相位空间隔离，并解释这些机制如何导致输运的饱和。
-定量估算部分，我需要插入典型的参数，比如在JT-60U装置中的参数，计算出增长率为大约500/s。这说明ITG的不稳定性发展非常迅速，对输运的影响显著。同时，指出这些参数可能随装置条件的不同而变化，强调在设计和优化聚变装置时需要考虑这些因素。
-在工程或实验意义方面，我需要说明如何通过调整装置参数来抑制ITG，比如控制温度梯度、优化磁场配置等。这可能涉及到反馈控制、磁场形状设计等工程技术手段，以提高等离子体的约束性能，减少热量和粒子的损失，从而改善聚变反应的条件。
-最后，比较与拓展部分，可以讨论其他类型的微观不稳定性，如电子温度梯度模（ETG）和 ballooning 模，说明它们的驱动条件和饱和机制。这不仅拓宽了讨论的范围，也帮助读者更好地理解不同不稳定性在反常输运中的角色。
-总结整个思考过程，我需要确保回答结构清晰，逻辑严谨，每个部分都涵盖必要的细节，同时避免过于复杂的数学推导，使读者能够理解反常输运和ITG不稳定性在聚变物理中的重要性及其实际应用。
-&lt;/think&gt;
-### 反常输运的定义
+          <t>### 反常输运的定义
 反常输运，又称 anomalous transport，是指在等离子体中，粒子、能量和动量的输运速率超出经典（Fickian或diffusive）输运理论的预测的现象。这种输运主要由微观不稳定性（如漂移波、温度梯度驱动的不稳定性）和宏观不稳定性（如磁流体力学（MHD）不稳定性）驱动。
 ---
 ### 离子温度梯度模（ITG）及其驱动的反常输运
@@ -904,7 +839,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -930,17 +865,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>嗯，我现在要回答关于等离子体鞘层形成过程和主要特征的问题，还有鞘层在等离子体与壁相互作用（PMI）以及朗缪尔探针诊断中的作用。首先，我需要回忆一下等离子体鞘层的基本概念。
-等离子体鞘层，特别是德拜鞘层，我记得它是在等离子体和固体壁之间形成的。这个鞘层的主要作用是屏蔽外部的电场，防止等离子体中的带电粒子直接接触到壁。那么，鞘层的形成过程是怎样的呢？
-首先，等离子体中的电子由于轻且速度快，会迅速响应外部的电场变化，而离子因为质量大、速度慢，响应较慢。当等离子体靠近壁时，电子会先到达壁，导致壁上的电势发生变化，进而吸引离子。这样，电子的积累导致壁带负电，形成鞘层电势。这个过程称为电荷分离。
-接下来，鞘层的主要特征包括德拜长度和鞘层电势。德拜长度λ_D是描述电势衰减的特征长度，由等离子体的温度和密度决定。计算公式是λ_D = sqrt( (ε_0 k_B T_e) / (n_e e^2) )。鞘层电势Φ_s则取决于等离子体的参数，比如电子温度和密度，通常为几伏特。
-然后，关于鞘层在PMI中的作用，它会影响离子的轰击能量。高能量的离子轰击壁会导致壁材料的侵蚀，这对聚变装置的材料选择和寿命有重要影响。因此，控制鞘层电势和离子能量是工程设计中的关键点。
-在朗缪尔探针诊断中，鞘层的作用是让探针能够测量等离子体的参数。探针浸入等离子体时，周围的鞘层会限制电流，通过测量探针的电流-电压特性，可以推断出等离子体的电子温度、密度和离子密度等参数。
-总结一下，我需要分步骤描述鞘层的形成过程，解释其主要特征，然后详细阐述它在PMI和探针诊断中的作用。同时，注意使用规范的符号和单位，确保解释清晰准确。
-现在，我需要确保我没有遗漏任何关键点，比如鞘层的分类（德拜鞘层和预鞘层）、鞘层形成中的假设（比如忽略磁场、离子惯性等）。此外，PMI中的其他效应，如碰撞、中性原子的影响也需要提及。
-最后，整理这些思路，按照规范的答题结构，逐步展开每个部分，确保逻辑清晰，内容全面。
-&lt;/think&gt;
-### 等离子体鞘层的形成过程和主要特征
+          <t>### 等离子体鞘层的形成过程和主要特征
 #### 1. 核心结论
 等离子体鞘层是在等离子体与固体壁界面处形成的一个具有空间电势梯度的区域，其特征包括德拜长度、鞘层电势和空间电荷分布。
 #### 2. 背景与概念
@@ -963,7 +888,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -989,15 +914,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>嗯，我现在要回答关于磁流体力学（MHD）近似的适用条件及其局限性，以及在哪些聚变等离子体研究中必须使用更复杂模型的问题。首先，我得先理解什么是MHD近似。
-MHD是一种将等离子体视为完全导电的流体的模型。它适用于等离子体中电场可以忽略的情况，也就是说，电场由洛伦兹力平衡。这可能发生在较大的尺度和较低的频率下，或者在等离子体参数足够大时，比如温度很高或密度很大。
-适用条件方面，我想到的是当离子和电子的运动趋近于相同的时候。这可能需要满足一些参数条件，比如温度高、磁场强或者特征长度尺度大。这些条件下，等离子体的导电性很好，可以使用MHD模型。
-接下来，MHD的局限性。当等离子体的参数偏离这些条件，比如在高频率、小尺度或者磁场较弱的情况下，MHD就不再适用。这时候，可能需要考虑离子和电子的不同运动，也就是双流体模型。或者在更极端的情况下，甚至需要考虑回旋运动，使用回旋动力学模型。
-然后，哪些聚变等离子体现象需要超越MHD呢？我想到的一些现象包括 Alfven波、磁流体不稳定性（如kink不稳定性）、磁重联等，可能需要更细致的模型来描述。此外，当涉及电场的快速变化或等离子体的非均匀运动时，MHD可能无法准确描述，需要更精细的模型。
-在回答时，我需要结构清晰，分点论述，每个部分都要详细但简明。同时，要按照用户的要求，用中文写，使用小标题，方程用LaTeX，单位规范等。
-总结一下，我会先给出核心结论，然后分点讨论适用条件、局限性、以及需要更复杂模型的现象。最后，给出工程或实验意义，比较不同模型的优缺点，并总结要点。
-&lt;/think&gt;
-### 磁流体力学（MHD）近似的适用条件及其局限性
+          <t>### 磁流体力学（MHD）近似的适用条件及其局限性
 #### 1. **核心结论**
 磁流体力学（MHD）近似适用于等离子体的宏观尺度和低频动力学行为，当等离子体参数满足离子和电子运动趋近于同一速度时。其局限性在于无法描述小尺度、高频现象以及电荷分离效应，这些情况下需采用双流体或回旋动力学模型。
 ---
@@ -1040,7 +957,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -1066,14 +983,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>好的，我现在需要解释等离子体中的朗道阻尼机制，以及它在无碰撞等离子体中波阻尼的原因，同时分析它对等离子体加热和电流驱动的影响。
-首先，我应该回忆一下朗道阻尼的基本概念。朗道阻尼是由苏联物理学家 Lev Landau 提出的一种机制，它描述了等离子体中波的衰减现象。等离子体由大量带电粒子组成，这些粒子会与电磁波相互作用，导致波能量转化为热能。
-接下来，我需要思考为什么在无碰撞等离子体中会出现波阻尼。通常，等离子体中的波阻尼可能源于粒子之间的碰撞，但朗道阻尼发生在无碰撞的情况下。这是因为即使粒子不直接碰撞，它们的集体行为也会导致能量转移。具体来说，当波传播时，某些粒子的速度与波相位速度匹配，导致这些粒子获得能量，从而改变它们的速度分布，使波逐渐衰减。
-然后，我需要解释朗道阻尼的机制。这涉及波与粒子之间的相互作用。当波的频率接近粒子的共振频率时，粒子会吸收波的能量。在动量空间中，这种相互作用会导致粒子的分布发生变化，使波的能量被粒子带走，形成阻尼。
-在分析对等离子体加热和电流驱动的影响时，我需要考虑几个方面。首先，朗道阻尼会导致波能量转化为等离子体的热能，从而实现等离子体加热。其次，波的吸收可以产生电流，特别是在磁场存在的情况下，这可能用于电流驱动。此外，朗道阻尼的选择性吸收特性可能会影响加热和驱动的效率，例如不同离子种类吸收不同频率的波，导致加热的不均匀性。
-最后，我需要总结这些点，强调朗道阻尼在等离子体中的重要作用，特别是在聚变装置中的应用。同时，指出其潜在的挑战，如非线性效应和多维效应，这些可能需要更复杂的理论来处理。
-&lt;/think&gt;
-### 朗道阻尼机制解释
+          <t>### 朗道阻尼机制解释
 #### 核心结论
 朗道阻尼机制描述了等离子体中的无碰撞波阻尼现象，是由于波与粒子之间的能量交换导致波能量转化为热能。
 ---
@@ -1138,7 +1048,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -1164,16 +1074,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，我现在要讨论E×B漂移在等离子体约束和输运中的双重作用。首先，我记得E×B漂移是等离子体中的一个基本现象，涉及到电场和磁场的相互作用。用户提到的例子有霍尔推进器和磁控溅射，这些都是等离子体应用的实例，所以需要从这些具体装置出发来分析。
-首先，我需要明确E×B漂移的定义和物理机制。E×B漂移是指在磁场和电场的共同作用下，等离子体的带电粒子获得的一种平均漂移运动。这个漂移速度由公式v = (E × B)/B²给出，其中E是电场，B是磁感应强度。这个速度使得粒子在等离子体中整体移动，形成一种输运现象。
-接下来，讨论E×B漂移在约束中的作用。在磁约束聚变装置中，例如托卡马克，E×B漂移有助于限制等离子体的扩散，提高约束性能。这是因为E×B漂移会形成一个闭合的环流，阻止粒子的径向逃逸，从而延长等离子体的寿命。这种效应通常被称为“等离子体约束”。
-然后是输运的作用。虽然E×B漂移有助于约束，但它同时也可能导致粒子的输运，尤其是在电场和磁场梯度较大时。这种输运现象可能包括玻姆扩散和近壁电导等反常输运机制。玻姆扩散是由等离子体波动引起的粒子输运，其扩散系数与温度梯度有关；而近壁电导则涉及到等离子体与装置壁之间的相互作用，可能导致电子的大量损失。
-接下来，我需要以霍尔推进器为例，分析其中的反常电子输运机制。霍尔推进器是一种空间推进装置，利用等离子体在强磁场中的E×B漂移效应来产生推力。在这种装置中，电子的E×B漂移会导致电子的输运，从而影响等离子体的电导率和推进效率。特别是在近壁区域，电子与器壁的相互作用可能引发近壁电导，这种现象会导致电子的大量损失，从而影响推进器的性能。
-再以磁控溅射为例，这种技术利用等离子体在靶材上的溅射效应来沉积薄膜。在磁控溅射中，E×B漂移帮助形成一个环形等离子体流，从而增强溅射效率。然而，如果等离子体中的电场梯度较大，可能会引发玻姆扩散，导致离子输运增加，从而影响薄膜的质量和沉积速率。
-在分析这些现象时，我还需要考虑相关的物理参数，如电场强度、磁场强度、等离子体密度和温度等。这些参数会影响E×B漂移的速度和输运机制的强度。例如，较强的磁场会减小E×B漂移速度，但同时也会增强对等离子体的约束；而较高的电场梯度则会促进玻姆扩散。
-总结一下，E×B漂移在等离子体约束中起到积极的稳定作用，而在输运中则可能导致反常现象，如玻姆扩散和近壁电导。这两种作用在不同的应用中表现不同，需要根据具体装置的参数和需求来平衡和优化。
-&lt;/think&gt;
-### E×B漂移在等离子体约束和输运中的双重作用
+          <t>### E×B漂移在等离子体约束和输运中的双重作用
 #### 核心结论
 E×B漂移在等离子体中具有双重作用：一方面有助于约束等离子体，另一方面导致反常电子输运。这两种作用在霍尔推进器和磁控溅射中均有体现，分别涉及玻姆扩散和近壁电导机制。
 #### 背景与概念
@@ -1208,7 +1109,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -1234,19 +1135,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>好，我现在需要回答如何通过实验手段测量等离子体的基本参数，包括电子温度Te、离子温度Ti、电子密度ne和等离子体电流Ip。至少要列举三种不同的诊断技术，并说明它们的原理。
-首先，我得回忆一下常见的等离子体诊断方法。记得常用的有光谱诊断、微波诊断和磁测量等。光谱诊断可能涉及X射线和极紫外光谱，微波诊断可能包括反射计和干涉计，磁测量可能涉及托卡马克的磁探针或者平衡磁测量系统。
-让我详细想一下每种方法的原理。首先是光谱诊断。电子温度可以通过X射线或极紫外谱线的宽度来确定，根据多普勒效应，谱线宽度和温度相关。离子温度可能需要观察离子的谱线。电子密度则可以通过等离子体吸收连续谱来确定，这可能涉及到吸收光谱中的变化，比如等离子体的吸收边。这种方法需要有特定的光谱仪设备，能够捕捉到不同波长的光谱线。
-接下来是微波诊断，主要有反射计和干涉计。微波反射计可以测量等离子体的电子密度分布。因为当微波穿过等离子体时，其反射特性取决于等离子体的频率和电子密度，由此可以推导出电子密度的分布。微波干涉计则是利用等离子体对微波的相位调制来测量整体电子密度，因为等离子体对微波会产生相位变化，相位变化的量与电子密度积分有关。
-第三种是磁测量，特别是用于托卡马克装置的磁探针。磁探针可以直接测量等离子体内部的磁场，进而通过等离子体的磁流体力学关系，确定等离子体电流Ip。此外，平衡磁测量系统可以通过环形磁探针测量等离子体中的不同位置的磁感强度，结合托卡马克的结构，计算出等离子体电流的分布和总量。
-现在，我需要考虑每种方法的具体步骤和理论基础。对于光谱诊断，涉及的公式可能包括使用波尔兹曼分布来确定电子温度，因为谱线的强度比例与温度有关。离子温度可能通过离子的谱线宽度来确定。电子密度则可能通过斯托克斯位移或其他吸收特性来确定。
-微波反射计的原理可能涉及到等离子体的反射特性，比如反射频率与电子密度的关系，即反射频率等于等离子体频率。等离子体频率ωp=√(n_e e²/(ε₀ m_e))，所以通过测量反射频率，可以得到n_e。干涉计方面，相位变化Δφ与积分电子密度n_e * L成正比，Δφ=2π (n_e e^2)/(ε₀ m_e ω^2) * L，因此通过测量相位变化，可以得到n_e。
-磁探针测量等离子体电流则涉及到法拉第电磁感应定律。托卡马克中的等离子体电流会产生环形磁场，环形磁探针测量不同位置的磁感强度，通过积分可以得到等离子体电流Ip。具体的，Ip等于1/(μ₀ R)乘以积分环路的磁感强度B·dl，即Ip=(1/(μ₀ R)) ∫ B dl。
-我还需要考虑这些方法的优缺点。例如，光谱诊断需要高分辨率的光谱仪，且可能需要特定的谱线覆盖范围，对于某些等离子体可能不容易获取。微波诊断则对等离子体中的微波传播条件有要求，可能需要处理高密度或高温等离子体中的衰减或折射问题。磁探针测量在托卡马克装置中是标准的方法，但需要良好的磁测量系统和信号处理能力，才能精确测量微小的磁场变化。
-最后，我要确保回答涵盖所有要求的参数，即Te、Ti、ne和Ip，每种诊断方法是否能测量这些参数中的部分或全部。例如，光谱诊断可以测量Te、Ti和ne，但可能不直接测量Ip。微波反射计和干涉计则主要测量ne。磁探针则测量Ip，可能结合其他方法来确定其他参数。
-总的来说，我需要组织这三种方法，详细说明每种方法的原理、测量参数、相关公式，并简要提到它们的适用性和局限性。这样就能全面回答用户的问题了。
-&lt;/think&gt;
-### 如何通过实验手段测量等离子体的基本参数
+          <t>### 如何通过实验手段测量等离子体的基本参数
 通过实验手段测量等离子体的基本参数，如电子温度（Te）、离子温度（Ti）、电子密度（ne）和等离子体电流（Ip），是聚变等离子体物理研究中的核心任务。以下是三种常见的诊断技术及其原理：
 ---
 ### 1. 光谱诊断（Spectroscopy）
@@ -1307,7 +1196,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -1333,16 +1222,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，我现在得回答一个关于托卡马克放电过程的问题。问题是要简述在击穿、电流爬升、平顶和破裂这四个阶段，哪些基本的等离子体物理过程占主导地位。我需要仔细回忆一下托卡马克的基本工作原理和每个阶段的特点。
-首先，击穿阶段，这是等离子体开始形成的过程。我记得击穿通常涉及到电离，所以这里的主导过程应该是电离。可能需要考虑气体放电机制，比如初始的电子被加速到足够高能量去撞击气体分子，导致电离。
-接下来是电流爬升阶段。这个阶段主要是等离子体电流迅速增加。这里涉及到电流生成机制，可能与等离子体的欧姆加热有关。同时，可能会有不稳定性开始出现，因为电流密度高了，容易引发像气球模不稳定性这样的问题。另外，加热方式主要是欧姆加热，还有可能产生较大的涡旋，影响输运。
-然后是平顶阶段，这是托卡马克运行的核心阶段，维持高温高压。这里主导过程应该是输运，因为维持高参数需要控制热量和粒子的输运。同时，磁流体力学（MHD）不稳定性可能在这个阶段变得关键，比如锯齿模不稳定性，会影响等离子体的稳定性。还有反馈控制可能被用来稳定等离子体。
-最后是破裂阶段，这是等离子体突然失去稳定的过程。这里的主导过程是不稳定性，特别是MHD不稳定性，导致等离子体失去约束，发生破裂。可能还有磁重联等过程参与其中。
-我还需要考虑每个阶段的具体物理过程和相关因素，比如在击穿阶段，电离主要由气压、磁场和初始电子密度决定；在电流爬升阶段，涉及欧姆加热和相关的输运；平顶阶段可能需要考虑辐射损失和反馈控制；破裂阶段则涉及不稳定性的发展和能量快速释放。
-在总结时，我需要清晰地列出每个阶段的主导过程，并简要说明它们的物理机制和影响因素。这可能涉及到电离、辐射、输运、不稳定性、加热机制等多个方面。
-可能需要进一步查阅相关资料，确保每个阶段的描述准确无误，但根据我的现有知识，大致是这样的结构。
-&lt;/think&gt;
-在托卡马克放电的四个阶段中，每个阶段都由不同的等离子体物理过程主导：
+          <t>在托卡马克放电的四个阶段中，每个阶段都由不同的等离子体物理过程主导：
 ### 1. 等离子体击穿阶段
 - **主导过程**：电离
 - **描述**：在此阶段，外部电源产生的电流引发气体放电，电子被加速至足够高的能量以撞击气体分子，导致电离。这一过程主要受气体压力、初始磁场强度和电子密度的影响。
@@ -1416,7 +1296,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -1442,107 +1322,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>嗯，我现在得仔细分析一下汤姆逊散射诊断测量等离子体电子温度和密度的原理，特别是当电子温度为10keV时的多普勒展宽Δλ，以及这对光谱仪分辨率的要求。
-首先，汤姆逊散射诊断的基本原理是什么？我记得汤姆逊散射是基于自由电子对光的散射现象。当激光束进入等离子体时，电子会散射光，散射光的光谱包含了等离子体参数的信息。具体来说，散射光的光谱形状受到电子热运动速度的影响，这就是多普勒效应。
-那么，散射光的多普勒展宽主要取决于什么因素呢？应该是电子温度，因为温度越高，电子的热运动速度越快，散射光的频率变化范围越大，也就是多普勒展宽Δλ更大。
-接下来，我需要找出多普勒展宽Δλ的计算公式。根据汤姆逊散射理论，多普勒展宽Δλ与电子温度Te和入射激光波长λ0有关。具体公式可能是Δλ ≈ (λ0^2 * c) / (Ry * Te)，其中c是光速，Ry是里德伯常数。不过，我得确认一下这个公式是否正确，或者是否还有其他的系数需要考虑。
-现在，问题中给出的条件是：入射激光波长λ0=1μm，散射角θ=90度，电子温度Te=10keV。我需要计算此时的Δλ，并评估光谱仪的分辨率要求。
-首先，把已知参数代入公式。λ0=1μm=1e-6 m，Te=10keV=1e4 eV。里德伯常数Ry约为13.6 eV，光速c=3e8 m/s。
-计算Δλ：Δλ ≈ (λ0^2 * c) / (Ry * Te) = (1e-6^2 * 3e8) / (13.6 * 1e4)。
-先计算分子：1e-12 * 3e8 = 3e-4 m。
-分母：13.6 * 1e4 = 1.36e5 eV。
-所以Δλ ≈ 3e-4 / 1.36e5 ≈ 2.2e-9 m，也就是2.2纳米。
-不过，这可能吗？我记得多普勒展宽在高温等离子体中通常在几纳米到十几纳米的量级，所以这个结果看起来合理。
-接下来，光谱仪需要能分辨Δλ，否则无法准确测量。因此，光谱仪的分辨率至少需要在Δλ的量级，比如几纳米。
-但是，是否有其他的因素需要考虑，比如散射角θ=90度对多普勒展宽的影响？我是否漏掉了关于散射角的公式？其实，在汤姆逊散射中，多普勒展宽与散射角有关，公式可能需要修正。
-查阅资料，多普勒展宽Δλ的正确公式应该是Δλ = λ0 * (kTe)/(c * sin(θ/2))，其中k是波数，或者更准确地，用电子温度Te来表示，可能涉及电子速度和多普勒效应的公式。
-或者，正确的公式可能是Δλ ≈ (λ0 * c) / (Ry * Te) * (1/(sin(θ/2))) )。不过，我不太确定，可能需要重新推导一下。
-另一种方法，我记得电子速度v_th与温度Te的关系是v_th = sqrt( (8k_B Te) / (π m_e) )，其中k_B是玻尔兹曼常数，m_e是电子质量。
-然后，多普勒频率偏移Δν ≈ v_th * ν0 / c，其中ν0是入射光的频率。波长偏移Δλ = λ0 * v_th / c。
-将v_th代入，Δλ ≈ λ0 * sqrt( (8k_B Te)/(π m_e c^2) )
-或者，另一种表达方式：Δλ ≈ (λ0^2 * c)/(Ry * Te) * 1/(sin(θ/2))。
-现在，我需要确认正确的公式。可能我之前用了错误的公式，导致计算结果不准确。
-重新推导：汤姆逊散射的多普勒展宽来源于电子的热运动速度。散射光的频率变化与电子速度有关，散射角θ会影响这个变化的大小。对于散射角θ，频率变化Δν = (2 v cosθ') / c，其中θ'是电子速度方向与散射方向之间的夹角。因此，平均的Δν会导致多普勒展宽。
-更准确地说，多普勒展宽宽度Δν_Doppler与电子的热运动速度有关，可以表示为Δν_Doppler ≈ (2 v_th / c) * ν0，其中v_th是热速度，ν0是入射光频率。
-而v_th = sqrt( (8 k_B Te) / (π m_e) )，因此Δν_Doppler ≈ (2 * sqrt( (8 k_B Te)/(π m_e) )) / c * ν0。
-转换成波长偏移Δλ_Doppler = (λ0^2 * c)/(2 π m_e k_B Te) ) * (something关于散射角θ)。
-或者，另一个常见的公式是：Δλ = (2 λ0)/(c) * sqrt( (k_B Te)/(2 m_e) )
-这可能与实际的公式更接近。
-现在，我需要使用正确的公式来计算Δλ。假设使用Δλ ≈ (2 λ0)/(c) * sqrt( (k_B Te)/(2 m_e) )
-现在，计算各参数：
-λ0=1e-6 m，
-c=3e8 m/s，
-k_B=1.38e-23 J/K，
-Te=10keV=1e4 eV，
-1 eV=1.6e-19 J，所以Te=1e4 *1.6e-19 =1.6e-15 J，
-m_e=9.1e-31 kg。
-计算sqrt( (k_B Te)/(2 m_e) )：
-分子：k_B Te=1.38e-23 *1.6e-15=2.2e-38 J·K，
-分母：2 m_e=2*9.1e-31=1.82e-30 kg，
-所以内部：2.2e-38 /1.82e-30≈1.2e-8，
-平方根：sqrt(1.2e-8)=约3.46e-4 s^-1。
-然后，Δλ= (2 *1e-6)/(3e8) ) *3.46e-4 ≈ (6.67e-15) *3.46e-4≈2.31e-18 m？这显然不对，因为结果太小了。
-可能我在计算中哪里出了错。
-哦，可能我弄错了公式中的单位转换。Te是10keV，转换成温度应该是Te=10keV / (k_B)，即Te=10e3 eV / (8.617e-5 eV/K)=大约1.16e8 K。但是这可能不是问题所在，因为问题中给出的Te是10keV，而通常在聚变等离子体中，电子温度确实可以达到这样的量级。
-或者，可能我应该使用波长偏移的正确公式。正确的多普勒展宽Δλ公式可能需要重新推导。
-另一种方法，考虑电子的热速度v_th=sqrt( (8k_B Te)/(π m_e) )
-对于Te=10keV=1.6e-15 J，
-v_th= sqrt( (8 * 1.38e-23 *1.6e-15 ) / (π *9.1e-31) )
-计算分子：8*1.38e-23=1.104e-22，
-1.104e-22 *1.6e-15=1.766e-37，
-分母：π *9.1e-31≈2.86e-30，
-所以分子/分母=1.766e-37 /2.86e-30≈6.17e-8，
-平方根：sqrt(6.17e-8)=约7.86e-4 m/s。
-然后，Δλ≈λ0 * v_th / c =1e-6 *7.86e-4 /3e8≈7.86e-10 /3e8≈2.62e-18 m，这明显太小了，肯定是哪里错了。
-看来我在使用公式时出现了错误。正确的多普勒展宽公式应该是Δλ = (λ0 * v_th ) / c，其中v_th是热速度，但需要正确计算。
-或者，可能正确的公式是Δλ=λ0 * sqrt( (k_B Te)/(m_e c^2) ) * sqrt(8/π)。
-让我们重新计算：
-Δλ=λ0 * sqrt( (k_B Te)/(m_e c^2) ) * sqrt(8/π)
-代入数值：
-k_B=1.38e-23 J/K，
-Te=1e4 eV=1.6e-15 J，
-m_e=9.1e-31 kg，
-c=3e8 m/s，
-λ0=1e-6 m。
-计算 (k_B Te)/(m_e c^2)= (1.38e-23 *1.6e-15)/(9.1e-31*(3e8)^2 )= (2.208e-38)/(9.1e-31 *9e16 )= (2.208e-38)/(8.19e-14 )=约2.695e-25。
-平方根：sqrt(2.695e-25)=5.19e-13。
-乘以λ0=1e-6 m，得到：1e-6 *5.19e-13=5.19e-19 m，这还是太小了，显然哪里有问题。
-可能我的公式还是不正确。或许我应该参考汤姆逊散射的多普勒展宽标准公式。
-根据资料，汤姆逊散射的多普勒展宽Δλ可以表示为：
-Δλ = (2 λ0^2 c)/(Ry Te)
-其中Ry是里德伯常数，约为1.097e7 m^-1，Te是电子温度（eV），λ0是入射光波长。
-代入数值：
-Δλ= (2*(1e-6)^2 *3e8)/(1.097e7 *1e4)
-计算分子：2*1e-12 *3e8=6e-4 m。
-分母：1.097e7 *1e4=1.097e11。
-所以Δλ=6e-4 /1.097e11≈5.47e-15 m，这明显不对，因为结果太小。
-可能我搞错了单位。Ry是1.097e7 m^-1，或者Ry的单位是否正确？或者，Te应该以电子伏特为单位，而公式中的单位是否匹配？
-也许正确的公式应该是Δλ= (λ0^2 c)/(Ry h Te)，其中h是普朗克常数，单位要保持一致。
-或者，另一个公式是Δλ= (2 λ0)/(c) * sqrt( (k_B Te)/(2 m_e) )
-重新计算：
-sqrt( (k_B Te)/(2 m_e) )=sqrt( (1.38e-23 *1e4 *1.6e-19 )/(2 *9.1e-31 ) )
-注意：Te=10keV=1e4 eV，所以转换为焦耳时，1e4 eV=1e4 *1.6e-19=1.6e-15 J。
-所以，(1.38e-23 J/K *1.6e-15 J)=2.208e-38 J²/K？
-这可能不对，因为Te是能量单位，不是温度。哦，抱歉，Te在公式中是以能量单位出现的，而k_B Te是能量。
-所以，(k_B Te)=1.38e-23 *1.6e-15=2.208e-38 J。
-除以(2 m_e)=2 *9.1e-31=1.82e-30 kg，
-所以内部是2.208e-38 /1.82e-30≈1.213e-8 m²/s²。
-平方根：sqrt(1.213e-8)=约3.48e-4 m/s。
-然后，Δλ= (2 *1e-6 )/(3e8 ) *3.48e-4 ≈(6.667e-15)*3.48e-4≈2.32e-18 m，还是不对。
-看来我可能需要寻找一个更可靠的公式。查找到汤姆逊散射的多普勒展宽公式，通常表示为：
-Δλ = (λ0 * c) / (Ry * Te )
-其中λ0是入射光波长，c是光速，Ry是里德伯常数（1.097e7 m^-1），Te是电子温度（eV）。
-代入数值：
-Δλ= (1e-6 *3e8 )/(1.097e7 *1e4 )= (3e2 )/(1.097e11 )≈2.734e-9 m=2.734 nm。
-这看起来更合理，而且符合之前估算的2.2纳米左右的结果。
-因此，当Te=10keV，λ0=1μm时，Δλ≈2.7 nm。
-那么，光谱仪需要至少能分辨这个Δλ，否则无法准确测量。通常，光谱仪的分辨率R定义为λ/Δλ，其中Δλ是其能分辨的最小波长间隔。
-例如，若Δλ=2.7nm，而光谱仪的分辨率R必须大于等于Δλ/Δλ=1，但实际上需要更高的分辨率以准确捕捉多普勒展宽的形状。
-例如，假设光谱仪的分辨率Δλ Instrument= Δλ，即分辨率为R=λ0/Δλ=1e-6 /2.7e-9≈370。这意味着光谱仪需要至少在370的分辨率下工作。
-但可能需要更高的分辨率，比如Δλ Instrument= Δλ / N，其中N是信号处理的倍数，如N=2或更高。
-总结，当Te=10keV时，Δλ≈2.7nm，因此光谱仪需要至少在2.7nm的分辨率下工作，或者更高的分辨率以准确测量。
-&lt;/think&gt;
-### 论述汤姆逊散射诊断测量等离子体电子温度（Te）和电子密度（ne）的基本原理，并估算多普勒展宽Δλ及其对光谱仪分辨率的要求。
+          <t>### 论述汤姆逊散射诊断测量等离子体电子温度（Te）和电子密度（ne）的基本原理，并估算多普勒展宽Δλ及其对光谱仪分辨率的要求。
 #### 1. 核心结论
 当入射激光波长λ0=1μm，散射角θ=90∘，电子温度Te=10keV时，散射光谱的特征多普勒展宽Δλ约为2.7nm。因此，光谱仪的分辨率应至少为2.7nm，以准确捕捉多普勒展宽的光谱信息。
 #### 2. 背景与概念
@@ -1571,7 +1351,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -1597,14 +1377,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>嗯，用户是一位资深的聚变等离子体物理与工程专家，现在他想了解激光干涉和偏振测量诊断等离子体密度和磁场的原理。为什么大型装置如ITER常用多弦或远红外激光系统？还有振动补偿和长光程对准的挑战在哪里。
-首先，我得回忆一下激光干涉测量的基本原理。干涉测量利用了光的波长特性，当激光穿过等离子体时，由于等离子体的密度，激光的折射率会发生变化，导致光程差。通过干涉图样的相位变化，可以计算出密度的变化。这样就能实时监测等离子体密度分布了。
-接着是偏振测量，这主要用于测量磁场。等离子体中的磁场会使激光的偏振态发生变化，这种变化可以通过偏振分析来测量。利用法拉第效应，磁场强度与偏振旋转的角度成正比，这样就可以推断出磁场的分布情况。
-然后，为什么ITER会采用多弦或远红外激光系统呢？多弦设计可以让激光从不同的路径穿过等离子体，这样能够更全面地测量三维结构，提高诊断的准确性。远红外激光的波长较长，可以更好地穿透高密度等离子体，减少吸收和散射的影响，确保信号的稳定性和准确性。
-接下来，振动补偿和长光程对准的挑战。等离子体实验中，装置可能会有振动，比如磁性约束中的振动。这会导致激光束的位置偏移，影响测量的稳定性。因此，需要高精度的振动补偿技术，可能需要实时监测和调整激光束的位置。长光程意味着激光需要在装置内传播较远的距离，这增加了光程对准的难度，容易受到环境因素的影响，比如温度变化或结构变形，都需要精密的控制和调整。
-最后，总结一下，激光干涉和偏振测量是重要的诊断手段，能够提供高时空分辨率的等离子体参数。多弦和远红外激光系统的选择是为了适应ITER等大型装置的需求，而振动补偿和长光程对准则是实施过程中需要克服的关键技术挑战。
-&lt;/think&gt;
-### 1. 核心结论  
+          <t>### 1. 核心结论  
 激光干涉测量（Interferometry）用于诊断等离子体密度，偏振测量（Polarimetry）用于诊断磁场或电流密度。大型装置如ITER采用多弦或多波长系统以提高测量精度和覆盖范围，远红外激光用于减少等离子体吸收。振动补偿和长光程对准是这些系统的两项主要技术挑战。
 ---
 ### 2. 背景与概念  
@@ -1664,7 +1437,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -1690,14 +1463,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>好，我现在需要详细思考电子回旋发射（ECE）诊断在聚变等离子体中测量电子温度剖面的物理基础，以及它在不同光学厚度条件下的应用区别。同时，还要探讨在强电子回旋共振加热（ECRH）环境下，尤其是存在超热电子时，ECE系统可能会遇到的问题和相应的解决方案。
-首先，电子回旋发射的基本原理是基于等离子体中的电子在高频电磁波作用下发生回旋共振。当入射的微波频率等于或接近电子回旋频率时，等离子体中的电子会被激发，导致微波被吸收或发射。这种效应在诊断中被用来测量电子温度和密度分布。
-接下来，光学厚度指的是微波在穿过等离子体过程中被吸收的程度。当光学厚度较大时，大部分微波被吸收，只有少部分透射出去；反之，当光学厚度较小时，微波透射较多，吸收较少。不同的光学厚度条件会影响ECE诊断的具体应用方式。例如，在高光学厚度条件下，测量的是局部温度，而在低光学厚度条件下，可能无法有效测量深层等离子体的温度。
-在强ECRH环境下，电子回旋共振加热会导致等离子体中产生超热电子。这些超热电子可能会引起ECE信号的变化，干扰正常测量。具体来说，超热电子的存在会改变等离子体的微波吸收特性，导致测量得到的电子温度不准确。此外，超热电子的分布不均匀也可能影响诊断的准确性。
-为了解决这些问题，可以采用多种方法。首先，优化ECE系统的频率选择，避开超热电子的主要吸收频段，从而减少其对信号的影响。其次，结合其他诊断手段，如多频段ECE或结合其他类型的诊断仪器（如中性束或散射诊断），通过综合分析不同数据，提高测量的准确性。此外，改进数据分析算法，考虑超热电子的影响，对测量结果进行校正，也是解决问题的一种途径。
-在实际应用中，ECE诊断系统的设计需要考虑等离子体的各种参数和状态变化，确保在不同条件下都能有效工作。同时，定期校准和验证系统的性能，也是保证测量准确性的关键。
-&lt;/think&gt;
-### 电子回旋发射（ECE）诊断测量电子温度剖面的物理基础
+          <t>### 电子回旋发射（ECE）诊断测量电子温度剖面的物理基础
 **核心结论**  
 电子回旋发射（ECE）诊断基于等离子体电子的回旋共振特性，通过测量微波发射或吸收来推断电子温度和密度分布。
 **背景与概念**  
@@ -1754,7 +1520,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -1780,33 +1546,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>好，我现在要解决的问题是关于聚变中子诊断在D-T聚变等离子体研究中的重要性，以及列举至少三种不同的中子诊断技术，并说明它们各自提供的关键物理信息。
-首先，我需要理解聚变中子诊断的基本概念和作用。聚变反应中，主要是D-T反应，释放出中子，这些中子携带了等离子体中的关键物理信息，比如聚变反应的剧烈程度、离子的温度、燃料的比例等等。因此，通过检测这些中子，科学家可以间接了解等离子体内的各种物理参数。
-接下来，我需要思考中子诊断技术的重要性。由于聚变反应发生在高温高压的等离子体中，直接测量内部参数非常困难，因此中子诊断成为了一种重要的间接测量手段。中子通量、能谱、时间和空间分布等方面的信息，都可以通过不同的诊断技术来获取。
-现在，我要列举至少三种不同的中子诊断技术，并分析它们各自能提供的关键物理信息。常见的中子诊断技术包括中子通量监测、中子能谱仪和中子相机。
-1. 中子通量监测：
-   这种技术主要是测量中子的总流量，也就是单位时间内通过某个区域的中子数量。聚变反应中释放的中子通量与聚变反应的剧烈程度直接相关，因此通过测量中子通量，可以估算出聚变功率。具体来说，中子通量与反应堆中的燃料浓度和温度有关，通过监测中子通量的变化，可以了解聚变反应的动态过程和聚变功率的变化。
-2. 中子能谱仪：
-   中子能谱仪是用来测量中子的能量分布的。D-T反应释放的中子具有特定的能谱，主要集中在14.7 MeV左右。然而，由于等离子体中的各种物理过程（如中子的热化、散射等），实际测得的中子能谱可能会有所不同。通过分析中子能谱，可以获取关于离子温度的信息。例如，离子温度越高，中子在散射过程中获得的能量越多，能谱的宽度也会相应增大。此外，中子能谱还能提供燃料离子比例的信息，因为不同燃料（如D和T）产生的中子能量不同，通过分析能谱的分布，可以反推出燃料的比例。
-3. 中子相机：
-   中子相机通过测量中子的空间分布来成像，从而获取等离子体的空间结构信息。由于中子具有较强的穿透能力，中子相机可以在不干扰等离子体的情况下，捕捉到等离子体的三维结构和动态变化。例如，中子相机可以用于观察等离子体的对流、磁岛结构等现象。此外，结合中子相机的成像结果，还可以分析α粒子的行为，因为α粒子的运动轨迹会受到等离子体磁场和电场的影响，而这些信息可以通过中子相机的空间分布来间接反映。
-接下来，我需要考虑这些诊断技术的具体实现方法和物理量之间的关系。例如，中子通量监测通常使用中子探测器，如热释光片或裂变室，这些探测器能够记录单位时间内接收到的中子数量。中子通量Φ与聚变反应率R相关，R可以通过Φ和燃料浓度n、反应截面σ等参数来计算。公式为R = n² Φ σ，其中n是燃料离子浓度，σ是反应截面。通过测量Φ，结合已知的n和σ，可以估算出R，从而得到聚变功率P。
-中子能谱仪通常使用闪烁体或飞行时间（TOF）的方法来测量中子的能量。闪烁体材料如塑料闪烁体可以将中子转换为可见光，通过检测光的强度来判断中子的能量。飞行时间方法则是利用中子在不同能量下的速度差异，通过测量中子到达探测器的时间来推断其能量。通过能谱分析，可以得到中子的能量分布函数f(E)，进而计算出离子的平均温度T和燃料比例α。
-中子相机则使用中子敏感的探测器阵列，如中子相机使用的基于CCD的探测器，通过测量中子在不同位置的到达情况，来重建等离子体的空间分布。通过图像处理和反演算法，可以得到等离子体的三维结构和动态变化，从而分析α粒子的行为，如它们的扩散、被困情况等。
-在工程或实验意义方面，这些诊断技术对聚变装置的设计、运行控制、诊断和材料选择具有重要意义。例如，中子通量监测可以帮助优化燃料注入和加热方案，以提高聚变反应的效率。中子能谱仪的数据可以用于验证聚变反应模型，提高理论计算的准确性。中子相机提供的空间信息有助于改进磁 confinement 场的设计，减少等离子体的逃逸，提高聚变装置的稳定性和效率。
-此外，比较不同中子诊断技术的优缺点也很重要。中子通量监测方法简单，成本较低，但只能提供整体的聚变功率信息，缺乏空间和能量分辨能力。中子能谱仪虽然能提供能量信息，但通常需要复杂的探测器和数据处理系统，适用于定点测量。中子相机则具有较高的空间分辨能力，但需要昂贵的探测器和复杂的成像系统，适用于实时监测等离子体的动态变化。
-最后，我需要总结这些诊断技术在聚变等离子体研究中的重要性。中子诊断技术是研究D-T聚变等离子体不可或缺的工具，它们不仅能够提供聚变功率、离子温度、燃料比例等关键参数，还能帮助科学家理解α粒子的行为，为改进聚变装置的设计和运行控制提供重要依据。
-在思考过程中，我需要确保自己对每种诊断技术的工作原理、测量参数以及数据处理方法都有清晰的理解，这样才能准确地回答问题并提供有深度的分析。同时，也要注意结合实际应用，说明这些技术在聚变能研究中的实际意义和价值。
-总结一下，我的思考过程包括：
-1. 理解聚变中子诊断的基本概念和作用。
-2. 分析中子诊断技术在研究中的重要性。
-3. 列举三种中子诊断技术，并详细分析各自的关键物理信息。
-4. 探讨这些技术的具体实现方法和物理量之间的关系。
-5. 评估它们的工程和实验意义。
-6. 比较不同诊断技术的优缺点。
-7. 最后，总结这些技术在聚变等离子体研究中的重要性。
-&lt;/think&gt;
-聚变中子诊断在D-T聚变等离子体研究中具有独特的重要性，因为它提供了关于聚变反应动力学、等离子体状态以及燃料混合比例的直接信息。以下是三种中子诊断技术及其提供的关键物理信息：
+          <t>聚变中子诊断在D-T聚变等离子体研究中具有独特的重要性，因为它提供了关于聚变反应动力学、等离子体状态以及燃料混合比例的直接信息。以下是三种中子诊断技术及其提供的关键物理信息：
 ### 1. 中子通量监测
 - **工作原理**：测量中子在单位时间内通过特定区域的数量。
 - **关键信息**：
@@ -1840,7 +1580,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -1866,34 +1606,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>好，我需要回答用户关于光谱诊断在聚变等离子体研究中应用的问题，特别是测量杂质种类和浓度、离子温度和旋转速度，以及电荷交换复合光谱（CXRS）的原理和应用。我得一步步来分析。
-首先，光谱诊断广泛应用于聚变等离子体研究，特别是在托卡马克装置中。光谱技术能够测量等离子体的温度、密度、杂质含量等参数，这对理解等离子体行为和优化聚变反应至关重要。
-测量杂质种类和浓度是其中一个关键应用。等离子体中的杂质会影响聚变反应的效率和等离子体的稳定性。通过光谱线的波长和强度，可以识别杂质的种类和浓度。比如，使用可见光和紫外光谱技术，观察不同杂质元素发出的特征谱线，结合谱线强度的变化，就可以推断出杂质的含量和分布。
-接下来是离子温度和旋转速度的测量。离子温度是等离子体热力学性质的重要指标，而旋转速度则与等离子体的流动和动力学过程相关。通过分析光谱线的宽度和位移，可以推断出离子的热运动速度和整体旋转速度。例如，宽化的谱线表明离子具有较高的热速度，而谱线的红移或蓝移则反映了离子的旋转运动。
-然后是电荷交换复合光谱（CXRS）的原理和应用。CXRS是一种专门用于测量高能离子分布的技术。当高能离子与中性气体发生电荷交换时，会产生复合辐射。通过分析这些复合辐射的光谱特征，可以推断出高能离子的能量和分布情况。这种方法在研究聚变等离子体中的高能离子对装置壁的侵蚀作用中具有重要作用。
-为了更详细地阐述这些内容，我可以列出每个部分的要点，并解释相关原理和应用。此外，我还需要说明每种测量方法的具体步骤、所使用的光谱范围以及其在聚变研究中的重要性。
-总结一下，我需要在回答中涵盖以下几个方面：
-1. **背景与概念**：
-   - 光谱诊断的基本原理及其在聚变等离子体研究中的重要性。
-   - 不同光谱范围（可见光、紫外、X射线）的特点和应用。
-2. **测量杂质种类和浓度**：
-   - 利用特征谱线识别杂质元素。
-   - 通过谱线强度和拟合方法计算杂质浓度。
-   - 示例：使用可见光谱分析杂质的种类和浓度。
-3. **测量离子温度和旋转速度**：
-   - 利用多普勒效应和谱线宽度计算离子速度分布。
-   - 通过位移谱线测量整体旋转速度。
-   - 示例：使用X射线光谱测量离子温度和旋转。
-4. **电荷交换复合光谱（CXRS）**：
-   - 原理：高能离子与中性气体发生电荷交换，产生复合辐射。
-   - 应用：测量高能离子的能量分布，评估其对装置壁的影响。
-   - 示例：在托卡马克装置中使用CXRS监测高能离子的分布。
-5. **工程和实验意义**：
-   - 说明光谱诊断在聚变装置设计、运行优化和安全性评估中的重要性。
-   - 提出未来发展的可能方向，如更高分辨率光谱技术的应用。
-通过这样的思考和组织，我能够系统地回答用户的问题，并满足其对详细解释的要求。
-&lt;/think&gt;
-### 光谱诊断在聚变等离子体研究中的广泛应用
+          <t>### 光谱诊断在聚变等离子体研究中的广泛应用
 #### 1. 核心结论
 光谱诊断技术通过分析可见光、紫外和X射线等不同波长的光谱特征，能够测量聚变等离子体中的杂质种类与浓度、离子温度与旋转速度，以及利用电荷交换复合光谱（CXRS）研究高能离子的行为。
 #### 2. 背景与概念
@@ -1926,7 +1639,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -1952,14 +1665,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于磁诊断在等离子体物理中的应用，特别是长脉冲运行对积分器的要求。首先，我需要理解磁诊断的基本原理。磁探针、通量环和罗氏线圈各有不同，但都基于法拉第电磁感应定律。等离子体电流变化会产生变化的磁场，通过检测这些磁场的变化，可以推断出电流等参数。
-接下来，用户提到要讨论测量的参数，包括电流、位置、形状、储能以及MHD不稳定性。每种参数的测量都需要特定的诊断方法。例如，电流测量可能需要磁探针或通量环，而位置和形状可能需要多点测量或成像技术。
-然后，问题转向长脉冲运行对积分器的要求。长脉冲意味着等离子体状态可能在较长时间内变化较小，但为了精确测量，积分器的动态范围和分辨率变得非常重要。此外，积分器可能需要处理高频和低频信号，确保在长时间内信号不失真。
-我还需要考虑积分器的带宽、增益和噪声性能。对于长脉冲，积分器可能需要长时间积分，这可能引入低频噪声，影响测量精度。因此，选择合适的积分器参数，如高增益和低噪声，是关键。
-另外，长期运行中的温度和振动变化也可能影响积分器的稳定性，这需要在设计中考虑。可能需要采用温度补偿和高稳定性组件来保证积分器在长时间内的性能。
-最后，我需要总结这些要点，强调积分器在长脉冲运行中的重要性，以及如何选择合适的参数和设计来确保测量的准确性。同时，提到积分器可能带来的问题，如漂移和噪声，以及如何通过技术手段来解决这些挑战。
-&lt;/think&gt;
-### 1. 核心结论  
+          <t>### 1. 核心结论  
 磁诊断通过测量等离子体产生的磁场变化，可用于推断等离子体电流、位置、形状、储能和MHD不稳定性；长脉冲运行要求磁诊断积分器具有宽动态范围、高精度和低漂移特性。
 ---
 ### 2. 背景与概念  
@@ -2017,7 +1723,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -2043,18 +1749,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>嗯，我需要回答关于朗缪尔探针和球形探针的工作原理、测量参数以及在强磁场、高热流密度的聚变边界等离子体中应用时的挑战和局限性。首先，我要回忆一下这两种探针的基本知识。
-朗缪尔探针，我记得它是一种金属探针，用于测量等离子体的参数。工作原理应该是通过施加不同的电压，测量电流，然后利用等离子体的电流-电压特性来推导密度、温度等参数。这可能涉及到朗缪尔的理论，比如探针电流与等离子体参数的关系。
-球形探针呢，它应该是形状更接近球形，这样可以减少边缘效应，特别是在非平衡等离子体中。工作原理可能与朗缪尔探针类似，但设计上有所不同，可能在测量某些特定参数时更有效。
-接下来，测量参数方面，朗缪尔探针通常能测电子温度、密度，可能还有电位和流动速度。球形探针可能还用于测离子参数，如离子温度和密度。但我不太确定，可能需要查证。
-关于在强磁场和高热流条件下的挑战，这可能涉及到等离子体参数的变化，比如温度和密度的剧烈变化，可能会对探针的测量精度产生影响。此外，高热流可能会导致探针材料的损坏，比如熔化或侵蚀。磁场可能会影响等离子体的运动，导致探针测量时的偏移或不准确性。
-局限性方面，朗缪尔探针可能在高密度或高温条件下工作受限，因为探针的电流可能会被限制，导致测量误差。球形探针可能在某些参数上不够灵敏，或者在复杂等离子体环境中表现不佳。
-我还需要考虑这些探针在实际应用中的具体问题，比如诊断系统的复杂性，探针寿命，以及它们在聚变装置中的实际效果。可能还需要比较两者在不同条件下的优缺点，以及它们各自的适用性。
-总结一下，我需要按照用户给的规范来组织回答：核心结论，背景与概念，工作原理，测量参数，挑战和局限性，工程意义，比较与拓展，以及要点总结。我要确保每一步都详细且准确，必要时使用公式来说明原理。
-在写的时候，可能会遇到不确定的地方，比如具体的公式推导是否正确，或者某些参数的具体表现。可能需要做一些假设，比如探针的几何形状、电压施加范围等。同时，还要考虑这些探针在实际实验中的应用情况，比如在 ITER 装置中的使用情况，可能需要查阅相关资料。
-最后，确保回答结构清晰，符合规范，每个部分都有明确的小标题或项目符号，便于阅读。方程使用 LaTeX 语法，单位规范，语言准确严谨。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 朗缪尔探针和球形探针是研究等离子体边界参数的重要工具，分别通过测量电流-电压特性来推导等离子体参数。然而，在强磁场和高热流密度的聚变边界等离子体中，它们面临测量精度受限、探针寿命缩短及复杂环境适应性不足等挑战。
 ---
 ### 背景与概念  
@@ -2136,7 +1831,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -2162,21 +1857,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>好，我现在需要解决的问题是关于未来聚变装置诊断系统中的关键部件在恶劣环境下的辐照损伤效应及应对策略。首先，我要理解问题的具体要求，也就是ITER等聚变装置的诊断系统面临哪些挑战，特别是辐照损伤方面。
-首先，我得明确问题涉及的关键部件：光学窗口、反射镜、光纤、电缆和探测器。接下来，我需要考虑它们所处的环境：强中子/γ辐照、高热负荷、长脉冲、真空和远程维护要求。
-对于每个部件，我需要分析它们可能受到的辐照损伤效应。例如，光学窗口可能会有材料活化和降解，反射镜可能会有镜面退化，光纤可能会有光信号衰减，电缆可能会有绝缘性能下降，探测器可能会有性能衰退。
-然后，我需要针对每种损伤效应，提出相应的应对策略。这可能包括材料选择优化、结构设计改进、表面防护技术、冷却系统加强，以及先进制造技术的应用。
-接下来，我要按照规范的答题结构来组织我的思考。首先是核心结论，然后是背景与概念，接着是原理与推导，然后是定量估算或示例，工程或实验意义，比较与拓展，最后是要点总结。
-在背景部分，我需要详细描述聚变装置的辐照环境，包括中子和γ射线的来源及其能量范围，以及其他极端条件如高热和真空。
-对于原理与推导部分，我需要解释每种辐照损伤的具体机理，如材料活化、结构退化、性能衰退等，并提供相关的物理方程和化学反应式。
-在定量估算或示例部分，我需要给出具体的辐照剂量、温度变化和材料性能参数，以展示损伤效应的程度。例如，中子辐照导致的材料肿胀、变脆和活化，以及γ射线引起的材料降解和光学性能下降。
-工程意义部分，我需要讨论这些损伤效应对于诊断系统设计和运行的影响，强调选择合适材料、优化设计的重要性，并提出具体的防护措施。
-在比较与拓展部分，我可以比较不同材料在辐照环境下的性能，讨论它们的优缺点，并指出在不同辐照条件下的适用性。
-最后，要点总结要简明扼要，重申主要的结论和建议。
-现在，我需要确保我的思考过程中没有遗漏关键点，同时保持逻辑的连贯性。要确保每个部分都紧扣问题，提供全面而深入的分析，同时避免过于技术性的术语，以保持回答的可理解性。
-在完成这些思考后，我就可以按照规定的格式输出答案了，确保每个小标题和项目符号的使用，方便快速阅览。同时，正确使用LaTeX公式，保持单位和符号的规范，确保答案的严谨性和客观性。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 未来聚变装置诊断系统的关键部件在强辐照环境下面临材料活化、性能退化和功能失效等主要辐照损伤效应。应对策略包括优化材料选择、改进结构设计、应用表面防护技术和加强热管理。
 ---
 ### 背景与概念  
@@ -2251,7 +1932,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -2277,22 +1958,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>嗯，我现在遇到了一个关于ITER诊断系统的问题，需要解释“诊断第一壁”和“端口插件”的作用，同时说明如何在满足诊断视窗要求的同时确保真空密封、结构强度和足够的辐射屏蔽。作为一个刚开始学习核聚变相关知识的人来说，这个问题有点复杂，不过我来试试看能不能理清楚。
-首先，我需要了解什么是ITER。ITER是一个国际热核聚变实验反应堆，目的是为了研究可控核聚变，为未来提供可持续的能源。在ITER的建设中，诊断系统是非常重要的一部分，用来监测等离子体的状态，确保实验的顺利进行。
-问题中的两个关键概念是“诊断第一壁”和“端口插件”。我觉得“诊断第一壁”可能是指 ITER 装置内部用来放置诊断设备的结构，而“端口插件”可能是一些插入到托卡马克壁上的设备，用来进行各种测量和诊断。
-接下来，我需要理解它们在诊断系统中的作用。诊断第一壁可能是一个主要的支撑结构，用来安装各种诊断仪器，比如光谱仪、微波天线等。而端口插件可能是一些插入到特定位置的设备，比如用于高能粒子测量或者中子检测。
-然后，问题还问到了如何在满足诊断视窗要求的同时，确保真空密封、结构强度和足够的辐射屏蔽。这意味着在设计这些诊断系统时，不仅要考虑诊断的需求，还要考虑到ITER的运行环境，比如高真空、强辐射和高温等条件。
-我需要先思考“诊断视窗”是什么。视窗应该是指诊断设备用来观测等离子体的窗口，可能是由特定材料制成，允许特定波长的光线通过，同时又能承受高温和辐射。因此，设计诊断视窗时需要考虑材料的选择、尺寸、形状等因素，以确保信号的传递和设备的保护。
-接下来是真空密封。ITER内部是一个高真空环境，因为等离子体需要在超高温下运行，不能有其他气体干扰。因此，诊断设备必须能够保持高真空，不能有任何泄漏。这可能涉及到密封材料的选择、结构设计的合理性，比如是否有多层密封，是否有冗余设计等等。
-结构强度也是一个关键点。在运行过程中，ITER会经历各种应力，比如高温、震动、电磁力等。诊断设备必须有足够的强度，不会因为这些因素而发生形变或失效。可能需要使用高强度的材料，或者设计结构时考虑应力分布，避免应力集中。
-辐射屏蔽同样重要。聚变反应会产生大量的辐射，包括中子和高能粒子，这些辐射会对诊断设备造成损害，影响其寿命和性能。因此，需要在诊断设备周围设置足够的辐射屏蔽，比如使用铅、混凝土等材料，或者设计设备本身具有一定的抗辐射能力。
-综合以上几点，我需要思考如何在设计诊断系统时，同时满足这些要求。比如，在选择材料时，既要考虑是否适合诊断视窗的光学性能，又要考虑其耐高温、抗辐射的能力，以及是否能够承受结构强度和提供良好的真空密封。结构设计上，可能需要多层结构，每一层有不同的功能，比如外层用于结构支撑，中层用于辐射屏蔽，内层用于安装诊断设备。
-另外，还需要考虑诊断设备之间的布局和兼容性。不同的诊断设备可能需要不同的视窗和插件，如何合理安排这些设备的位置，避免互相干扰，也是需要考虑的问题。
-我可能还忽略了一些关键因素，比如热管理。在高温环境下，诊断设备可能会产生大量的热量，如何有效地散热，也是设计时需要考虑的。这可能涉及到冷却系统的设置，或者使用低热导率的材料，减少热量传递到诊断设备。
-另外，诊断设备的维修和更换也是一个重要的问题。在运行过程中，设备可能会损坏或老化，需要能够方便地进行维护和更换。这可能涉及到设计时预留足够的空间，或者使用模块化设计，方便拆卸和组装。
-总的来说，设计ITER的诊断系统是一个复杂的多学科问题，需要综合考虑物理、材料、机械、热力学、辐射防护等多个方面的知识。只有在各方面的设计都满足要求，才能确保诊断系统的正常运行，为ITER的成功运行提供可靠的数据支持。
-&lt;/think&gt;
-### 解释“诊断第一壁”和“端口插件”在ITER诊断系统中的作用
+          <t>### 解释“诊断第一壁”和“端口插件”在ITER诊断系统中的作用
 #### 诊断第一壁（Diagnostic First Wall）
 诊断第一壁是指ITER装置内部用于安装诊断设备的结构，它是诊断系统的基础。其主要作用包括：
 - **支撑诊断设备**：提供一个稳定的基础，用于安装各种诊断仪器，如光谱仪、微波天线等。
@@ -2325,7 +1991,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -2351,15 +2017,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于现代托卡马克装置中实时等离子体监测与反馈控制的，他们想知道通常使用哪些诊断信号来控制等离子体位形、抑制不稳定性（比如NTM）以及预警破裂。同时，用户还想了解这些诊断系统的时间分辨率和可靠性有什么要求。
-首先，我需要回忆一下托卡马克装置中常见的诊断技术。我记得用于位形控制的可能包括磁诊断，比如磁探针、平衡线圈和广义环形磁探针（GKPI）。这些装置通过测量磁场来确定等离子体的形状和位置。而像位移测量这样的指标，可能使用的是测微计（Extrim）传感器，它们能够检测等离子体垂直位移，这对于维持等离子体的位置非常重要。
-接下来是关于不稳定性控制，尤其是NTM（Neoclassical Tearing Modes）。这通常涉及到测量等离子体的磁岛结构和不稳定性的发展。ECE（Electron Cyclotron Emission）诊断可以用来监测等离子体中的电子温度变化，这对于检测不稳定性很有用。另外，极化诊断可能会用来测量等离子体中的电流分布，帮助判断是否有NTM发生。
-至于破裂预警，热负荷突增是一个关键指标。这可能需要使用滤光片测温系统，比如在第一壁上安装热电堆传感器，来实时监测温度的变化。此外，密度突增也可能是一个预警信号，中性束或微波反射诊断可能被用来监测密度变化。
-接下来考虑时间分辨率和可靠性。实时控制需要快速响应，所以时间分辨率至关重要。比如，位形控制可能需要每毫秒级的采样，这样才能及时调整控制回路。不稳定性控制可能需要更高的时间分辨率，因为NTM的发展速度很快，可能需要亚毫秒级的测量。破裂预警则需要足够快的响应时间，以确保在发生破裂前及时采取措施。
-可靠性方面，这些诊断系统必须在高辐射和高振动的环境中稳定工作，数据的准确性和稳定性直接影响到控制系统的性能。比如，在高功率运行中，诊断设备可能会受到干扰或损坏，所以设计时需要考虑抗干扰能力和冗余机制。
-总结一下，我需要分点列出诊断信号的类型，分别对应位形控制、不稳定性控制和破裂预警，然后详细说明各自的技术，接着讨论时间分辨率和可靠性要求，最后总结其工程意义。这样结构清晰，能够帮助用户全面理解问题。
-&lt;/think&gt;
-### 1. 核心结论  
+          <t>### 1. 核心结论  
 实时等离子体监测与反馈控制通常依赖于多种诊断信号，包括磁诊断、热诊断和图像诊断，以实现等离子体位形控制、不稳定性（如NTM）抑制和破裂预警。这些诊断系统需具备高时间分辨率（毫秒级至亚毫秒级）和高可靠性（抗干扰、冗余设计）以满足聚变装置的运行需求。
 ---
 ### 2. 背景与概念  
@@ -2492,7 +2150,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -2518,14 +2176,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>嗯，用户问的是托卡马克真空室的设计要求和功能，以及需要承受的载荷、材料选择和冷却策略。首先，我得明确真空室在整个聚变装置中的作用。它是一个关键的结构部件，主要是提供超真空环境，保护设备免受外部干扰，同时承受各种载荷。
-接下来，用户提到需要承受哪些载荷。这包括大气压、电磁力、热应力和内部过压。大气压在安装前真空室处于常压环境，所以需要考虑其作用。电磁力来自等离子体中的电流，可能会产生很大的力，比如垂直位移力和环向应力。热应力则是因为设备运行时的温度变化，真空室内部会有热屏蔽，减少直接热流，但仍有残余热。内部过压可能在故障情况下发生，比如失去真空或蒸汽产生，这需要额外的结构强度。
-然后是材料选择。通常用的是不锈钢，比如奥氏体不锈钢，因为它有良好的高温性能和焊接性。低活化钢也是一个选择，特别是在未来聚变堆中，减少放射性产物。关键要考虑材料的强度、抗辐照性能以及经济性。
-冷却策略方面，真空室通常通过水冷来处理残余热量，这涉及到复杂的冷却回路设计。另外，热屏蔽的使用可以将热流降到可管理的水平，进一步减少材料的热应力。
-工程和实验意义方面，设计和选材直接影响装置的性能和寿命。比如，材料的选择不仅影响耐久性，还涉及维护和运行成本。冷却系统的有效性则关系到设备的可靠性和运行时间。
-最后，比较与其他结构部件，真空室虽然不是直接与等离子体接触，但其稳定性对整个装置至关重要。所以在设计时需要综合考虑结构、材料和冷却等多个因素，确保在各种载荷下都能稳定工作。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 托卡马克真空室的主要设计要求包括承受大气压、电磁力、热应力和内部过压等多类载荷，其功能是提供超真空环境以支持等离子体运行。材料选择通常为不锈钢或低活化钢，冷却策略则结合水冷与热屏蔽技术。
 ---
 ### 背景与概念  
@@ -2572,7 +2223,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -2598,16 +2249,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于仿星器的三维复杂线圈和真空室带来的工程挑战，以及QUADCOIL等工具如何帮助平衡物理和工程需求。我需要详细分析这个问题，逐步思考解决方案。
-首先，我得理解仿星器的基本结构。仿星器不同于托卡马克，它的磁场不是轴对称的，而是通过三维线圈来形成更复杂的磁场结构。这种结构有助于抑制等离子体的不稳定性，但同时也带来了工程上的复杂性。
-接下来，工程挑战方面，我想到三维线圈的设计需要精确计算，任何一点的小错误都可能导致整体磁场不均匀，影响等离子体约束。线圈之间的空间安排也很重要，需要避免碰撞，同时确保冷却和维护的可行性。真空室的设计同样复杂，必须与线圈紧密配合，确保密封和耐高温性能。
-然后是材料和制造的挑战。三维线圈可能需要特殊的材料，这些材料不仅要能承受高温，还要有足够的强度和耐腐蚀性。制造过程中，如何精确地成型这些复杂形状也是一个难题。此外，装配过程需要高精度，线圈的位置和对齐必须严格控制，否则会影响整体性能。
-接下来，QUADCOIL等设计工具的作用。这些工具应该能够处理三维结构的复杂性，进行多物理场模拟，比如电磁、热力学、结构力学等。通过模拟，设计师可以优化线圈布局，找到物理性能和工程可行性的最佳平衡点。同时，这些工具还能帮助预测潜在的问题，比如应力集中或磁场不均匀，从而在设计阶段就进行调整。
-再考虑比较与拓展部分，可能会提到其他设计工具，如ANSYS或COMSOL，它们各自的优势和局限。QUADCOIL可能在集成多种物理场模拟方面更具优势，适合仿星器的复杂需求。
-最后，总结部分需要强调这些工具如何帮助解决工程挑战，提升装置的可靠性和性能，同时降低成本和风险。
-整个思考过程中，我需要确保逻辑清晰，覆盖所有关键点，同时用简单明了的语言表达出来，避免过于技术化的术语，让用户能够轻松理解。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 仿星器的三维复杂线圈和真空室设计带来了制造精度、材料应力和装配可行性等多方面的独特挑战，而QUADCOIL等先进设计工具通过多物理场耦合仿真和优化算法，显著提升了设计效率和工程可行性。
 ---
 ### 背景与概念  
@@ -2660,7 +2302,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -2686,18 +2328,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>嗯，我现在需要回答关于ITER遥操作系统的问题，主要包括其组成部分和各部分的功能，以及在强辐射和空间受限环境下面临的关键挑战。让我先理清楚思路，逐步思考这个问题。
-首先，ITER遥操作系统，Remote Handling System（RH），是 ITER 机器设计的关键部分，因为它负责在高辐射和高温的环境中进行维护和更换部件。这可能包括偏滤器、包层、中性束注入器、料盒和端口插件等。所以，我应该逐一分析每个部分的功能。
-偏滤器RH：偏滤器在托卡马克中负责排除高能粒子和杂质，保护第一壁。在运行中，偏滤器会受到高热负荷和强辐射，因此需要定期更换或维护。遥操作在这里的作用应该是远程更换偏滤器组件，比如使用机械臂或机器人，在高辐射环境下完成这些任务。
-包层RH：包层是ITER的一部分，用于吸收中子并产生氚。包层组件也需要定期维护和更换，以确保氚的生产效率和装置的安全性。遥操作在这里应该是用来远程更换和维修这些包层组件，可能涉及到处理放射性物质，所以需要高度防护措施。
-中性束RH：中性束注入器用于加热等离子体，确保其稳定运行。这些设备可能需要定期维护，比如更换部件或调整位置。遥操作在此时用于远程维护这些注入器，可能需要精确的定位和操作，以避免干扰等离子体运行。
-料盒与端口插件RH：料盒用于装载或更换内部组件，端口插件则连接到真空室的端口，用于插入或移除诊断设备和其他部件。遥操作在这些情况下，可能需要打开和关闭这些端口，进行组件的装卸，同时在高辐射环境下确保操作的安全和高效。
-接下来，考虑在ITER的环境下，遥操作系统面临的关键挑战。首先，强辐射会导致设备材料退化，特别是机器人和机械臂的结构部件可能会受到辐射损伤，影响其长期性能。其次，空间受限使得操作路径受限，可能需要更灵活和紧凑的机械设计，以适应狭窄的空间，同时保持操作的精确性。
-还有，高热负荷也是一个问题，因为在处理高温部件时，遥控设备必须能够承受高温，或者有有效的冷却系统。此外，远程操作需要高度的可靠性和精确性，因为在强辐射环境下，任何失误都可能导致设备损坏，甚至影响整个装置的安全运行。
-最后，考虑到ITER的复杂性，遥操作系统的控制和协调可能非常复杂，需要高度自动化和智能化的系统来管理各种操作任务，同时确保与其他系统的协同工作。
-综上所述，我需要将这些思考转化为结构化的回答，按照用户的要求，分为组成部分及其功能，以及关键挑战两部分，每部分都要详细说明。
-&lt;/think&gt;
-### ITER遥操作系统的主要组成部分及其功能
+          <t>### ITER遥操作系统的主要组成部分及其功能
 #### 1. 偏滤器遥操作（Divertor RH）
 - **功能**：负责在ITER运行期间更换和维护偏滤器模块。偏滤器模块暴露在高热负荷和强辐射环境中，定期更换是维持等离子体稳定运行的必要条件。
 - **关键操作**：包括偏滤器模块的拆卸、更换和重新安装。操作过程中需使用远程机械臂和机器人，确保在高辐射环境下的安全性。
@@ -2731,7 +2362,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -2757,14 +2388,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>好，我需要讨论几种先进制造技术在聚变堆关键部件中的应用和优势。首先，有激光焊接和电子束焊接，这两种方法在高真空条件下焊接，能减少污染和杂质，适合需要高洁净度的真空室和偏滤器。接着是增材制造，也就是3D打印，可以制造复杂结构，减少材料浪费，缩短制造周期。然后是热等静压（HIP）技术，能均匀致密化材料，提升性能，适合高应力的包层模块。
-接下来，这些技术如何提高部件质量呢？激光和电子束焊接确保了焊接的高质量和无污染；增材制造能生产复杂精细的结构，避免传统制造的缺陷；HIP则通过均匀的处理提高了材料的均匀性和可靠性，减少内部缺陷。
-关于缩短制造周期，增材制造减少了繁琐的锻造和加工步骤，快速成型；而HIP可以在短时间内完成致密化处理，减少整体时间。
-在降低成本方面，增材制造减少了材料的浪费，传统制造中大量的材料会被切削掉，而3D打印只用所需的材料；HIP处理的材料性能更好，减少后续加工和维护成本。
-综合来看，这些先进制造技术各有优势，激光和电子束适合高洁净度要求，增材制造适合复杂结构，HIP适合高均匀性要求。在设计制造时，需要根据部件的具体需求选择合适的技术组合，以达到最佳效果。
-最后，这些技术的综合应用不仅提高了部件的质量和可靠性，还显著缩短了制造周期，降低了成本，为聚变堆的建造和运行提供了有力的技术支持。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 先进制造技术（激光焊接、电子束焊接、增材制造、热等静压HIP）显著提升了聚变堆关键部件的制造质量、缩短了制造周期并降低了成本，具体体现在焊接质量、材料利用率和结构复杂性处理等方面。
 ### 背景与概念  
 聚变堆的关键部件包括真空室扇段、偏滤器模块和包层模块，这些部件在极端环境中工作，要求材料具备高耐热性、高强度和高完整性。先进制造技术的应用能够满足这些严格要求，具体包括：  
@@ -2807,7 +2431,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -2833,15 +2457,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于聚变装置，特别是像ITER这样的大型项目，如何在建造和装配过程中建立和实施质量保证（QA）和质量控制（QC）体系的。他们还询问了关键的检验和测试环节有哪些。
-首先，我需要理解用户的需求。他们可能是一位参与聚变装置项目的工程师、管理人员，或者是对聚变能有兴趣的学生。他们想了解QA/QC的具体措施和流程，可能希望了解如何确保项目质量和安全。
-然后，我想到QA和QC在大型项目中的重要性。像ITER这样的项目涉及多个国家、众多供应商和复杂的系统，质量保证至关重要，以确保所有部件符合标准，避免故障，确保安全运行。
-接下来，我应该分解问题，看看需要涵盖哪些方面。建立QA/QC体系可能包括文件化、组织架构、培训和风险管理。实施过程中，可能包括采购、制造、安装和调试阶段的质量控制。然后，关键的检验和测试环节可能包括材料检测、部件测试、装配检查和整体测试。
-我还需要考虑具体的测试方法，比如无损检测、压力测试、真空测试等。此外，工程和实验意义部分，应该指出这些措施如何确保装置性能和安全性。
-可能还需要比较不同项目的做法，说明ITER的特殊之处，比如国际合作带来的挑战和解决方案。
-最后，总结时要强调全面的质量管理和国际合作的重要性，确保装置的可靠运行。
-&lt;/think&gt;
-### 质量保证（QA）与质量控制（QC）体系在聚变装置中的建立与实施
+          <t>### 质量保证（QA）与质量控制（QC）体系在聚变装置中的建立与实施
 #### 1. **核心结论**
 聚变装置（如ITER）的QA/QC体系通过严格的文件化管理、多层级组织架构、全面的检验测试流程和国际合作机制确保装置的高质量建设和安全运行。
 ---
@@ -2884,7 +2500,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -2910,19 +2526,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>好，我现在需要回答从现有中小型聚变装置到ITER，再到未来的DEMO电站，装置规模和复杂性的急剧增大会带来哪些主要的工程放大挑战。问题提到了部件制造、现场装配、系统集成和项目管理等方面。用户希望按照特定的答题规范来回答，分为七个部分，每部分都有明确的内容要求。
-首先，核心结论需要简明扼要，概括出主要的挑战。接下来是背景与概念，需要解释聚变装置的放大过程及其面临的挑战。然后，原理与推导部分应该详细分析每种挑战的机理，比如部件制造中的材料特性如何影响性能。定量估算部分需要提供具体的数字，比如ITER的磁铁用量，以说明规模增长。工程意义部分要说明这些挑战对实际项目的影响。比较与拓展可以讨论不同装置设计的不同放大效应，最后要点总结重申关键点。
-在思考过程中，我需要考虑各个阶段的具体情况。比如，ITER相比现有装置在尺寸和复杂性上有很大提升，而DEMO电站则更接近实际发电，需要更高的效率和可靠性。在部件制造方面，材料的需求量大幅增加，同时材料的性能在更大的尺度下可能会变化，需要考虑这些因素。现场装配方面，ITER的磁铁系统重量和规模要求极高的精度，DEMO电站的装配难度更大，可能需要新的技术。
-系统集成部分，ITER需要整合多个复杂系统，协调控制，而DEMO电站则需要更高的稳定性和可用性，系统之间的依赖性更强。项目管理方面，ITER涉及多个国家和机构，协调和资源管理难度大，而DEMO电站的规模更大，需要更高效的管理和沟通机制。
-定量估算部分，可以引用ITER的实际数据，比如磁铁系统的重量和材料用量，以及预计的安装时间，来具体说明问题。比如，ITER的超导磁铁系统重达2000多吨，制造和装配耗时数年，所需铜超过500吨，这些都是具体的例子，能够帮助读者理解放大过程中的困难。
-在背景与概念中，应该提到聚变装置的类型，如托卡马克和仿星器，以及它们在放大过程中面临的共同挑战。同时，定义一些关键参数，如装置的磁约束能力、加热功率和氚增殖效率等，这些参数随着装置规模增大而变化，影响整体设计和工程实现。
-在原理与推导部分，可能需要涉及一些物理公式，比如等离子体约束的性能随装置尺寸的变化，或者磁场强度与线圈材料的关系。例如，聚变反应率可能与装置体积有关，但同时材料的强度和性能可能随尺寸增大而变化，这会影响设计选择。
-在工程或实验意义部分，需要指出这些挑战如何影响项目的可行性，比如成本超支、进度延误，以及如何通过技术创新来缓解这些问题。例如，采用模块化设计和自动化装配技术，可以提高效率和降低成本。
-比较与拓展部分，可以讨论不同的聚变装置设计在放大过程中可能遇到的不同挑战，比如托卡马克和仿星器在制造和装配上的差异，以及各自的优势和劣势。
-最后，要点总结需要简洁明了，强调放大过程中的关键问题，如材料供应、制造精度、系统集成和国际合作，以及解决这些问题的重要性。
-总的来说，我需要系统地分析每个部分，确保内容全面，逻辑清晰，并且符合用户指定的格式和要求。同时，注意使用恰当的例子和数据来支持论点，使回答更具说服力和实用性。
-&lt;/think&gt;
-### 核心结论
+          <t>### 核心结论
 从现有中小型聚变装置到ITER，再到未来的DEMO电站，装置规模和复杂性的急剧增长将带来材料与制造、装配与集成、系统控制、氚供应链、成本管理及国际合作等多方面的放大挑战。
 ---
 ### 背景与概念
@@ -2974,7 +2578,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -3000,16 +2604,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>好，我现在要回答关于聚变堆总体布局和系统集成的关键因素的问题。首先，我得明确问题主要涉及哪些子系统，比如磁体、真空、冷却、加热、诊断等，以及它们之间的接口设计、空间分配和维护通道预留。
-我应该从总体结论开始，说明设计需要综合考虑物理需求、工程可行性和维护便利性。接下来，我需要详细列出每个关键因素，解释每个因素的重要性，并给出具体的设计考虑和示例。
-首先，磁约束系统的布局是核心，因为这决定了聚变反应的核心结构。比如，托卡马克的环形结构会影响其他系统的安排。其次，真空系统和热屏蔽必须高效，以防止等离子体污染和减少辐射热损失。这里可能需要用到高真空泵和适当的屏蔽材料。
-然后，冷却系统的设计对于维持设备温度至关重要，尤其是超导磁体需要极低的温度。如何与外部冷却循环整合，避免氦气泄漏，这些都需要考虑。加热系统需要与等离子体直接耦合，同时又不能干扰其他组件，比如选择合适的射频天线位置。
-诊断系统的设计需要放置各种传感器，确保测量的准确性，同时不影响其他系统的运作。燃料循环系统涉及氚的处理，必须确保安全，避免泄漏。维护通道的设计需要便于机器人进入，同时不影响聚变堆的整体结构和性能。
-我还应该考虑系统之间的接口设计，比如冷却系统的入口和出口，加热天线的位置，这些都需要合理安排，确保系统之间的协调和集成。空间分配方面，要确保所有子系统都有足够的空间，同时整体结构紧凑。
-最后，安全性和维护便利性也是关键因素，包括辐射屏蔽、应急系统以及远程维护通道的设计，这些都是为了保障人员安全和装置的长期稳定运行。
-总的来说，我需要综合考虑聚变堆的物理、工程和安全需求，合理布局各子系统，确保它们之间高效协同，并留有维护和升级的空间。这需要在设计初期就进行全面的规划和协调。
-&lt;/think&gt;
-### 聚变堆总体布局和系统集成的关键因素
+          <t>### 聚变堆总体布局和系统集成的关键因素
 #### 1. 核心结论
 聚变堆的总体布局和系统集成需要综合考虑磁约束系统的物理需求、工程可行性以及维护便利性，确保各子系统协同工作且预留足够的维护通道。
 #### 2. 背景与概念
@@ -3042,7 +2637,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -3068,18 +2663,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，这个问题是关于ITER偏滤器部件的制造和测试过程的。特别是钨/铜等离子体面向部件（PFCs）如何与冷却结构键合，以及高热负荷测试设施在验证部件性能方面的作用。
-首先，我需要了解ITER的偏滤器设计。ITER是一个大型的托卡马克装置，目标是实现可持续的核聚变反应。偏滤器在托卡马克中起到排出等离子体杂质、控制等离子体与壁的相互作用以及处理高热流的作用。因此，偏滤器部件需要承受极高的热负荷和强烈的等离子体冲击。
-钨/铜PFCs是ITER偏滤器的关键材料。钨作为等离子体面向材料，因为它具有高熔点和良好的耐等离子体侵蚀性能。铜则用于传导热量，因为它具有良好的导热性。然而，钨和铜的物理和化学性质差异较大，直接键合可能会产生界面问题，如热膨胀系数差异导致的应力和疲劳。
-接下来，键合工艺是关键。我想到可能的工艺包括扩散键合、钎焊和激光键合等。扩散键合是通过施加压力和温度，使两种材料在原子尺度上相互扩散结合。这种方法的优点是键合界面的强度较高，但需要高温和长的时间，可能会影响材料的性能。
-钎焊则是使用中间钎料，在加热过程中钎料填充材料界面并固化，形成连接。这种方法的优点是温度较低，适用于对温度敏感的材料。但钎料可能会在高温下失效，影响长期性能。
-激光键合利用高能激光束局部加热材料，促进界面结合。这种方法可以精确控制加热区域，减少整体材料的热变形，但设备成本和工艺复杂性可能较高。
-测试和验证阶段是确保PFCs性能的关键。高热负荷测试设施如GLADIS和Divertor Test Facility能够模拟ITER运行中偏滤器承受的极端条件，包括高热流密度和等离子体冲击。
-在测试过程中，会评估PFCs的热性能，如热导率和温度分布，以确保其在高温下的稳定性。机械性能测试则包括疲劳试验，以评估材料在反复热冲击下的耐久性。此外，等离子体兼容性测试需要检查材料在等离子体环境中的侵蚀和溅射行为，确保其不会释放有害物质或被快速侵蚀。
-测试结果将反馈到设计和制造过程，优化材料选择、键合工艺和冷却结构，以提高PFCs的可靠性和寿命。这对于ITER的成功运行至关重要，因为偏滤器部件的失效可能导致装置损坏或运行中断。
-总的来说，钨/铜PFCs的制造需要先进的键合工艺，而高热负荷测试设施则是验证其性能的关键工具。通过这些步骤，可以确保ITER偏滤器部件在极端条件下的稳定性和可靠性。
-&lt;/think&gt;
-### 描述ITER偏滤器部件的制造和测试过程
+          <t>### 描述ITER偏滤器部件的制造和测试过程
 #### 1. **核心结论**
 ITER偏滤器部件的制造和测试涉及复杂的材料处理、精密制造和极端条件下的性能验证。钨/铜等离子体面向部件（PFCs）通过扩散键合、钎焊或激光键合技术与冷却结构结合，而高热负荷测试设施如GLADIS和Divertor Test Facility通过模拟 ITER 的极端运行条件来验证这些部件的性能。
 ---
@@ -3128,7 +2712,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -3154,17 +2738,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>嗯，这个问题是关于聚变堆内部件连接和固定技术的，涉及到结构强度、真空密封、冷却剂流通和遥操作拆装等多个要求之间的权衡。我得先理清楚每个要求的重要性以及它们之间的相互影响。
-首先，结构强度是必须的，因为内部件需要承受高温、高热流和强大的电磁力。所以连接方式必须足够牢固，防止在运行过程中发生损坏或变形。其次，真空密封同样重要，因为聚变反应需要在高度真空的环境中进行，任何泄漏都会影响等离子体的稳定性和反应效率。
-然后是冷却剂流通，内部件通常需要复杂的冷却系统来带走巨大的热量。连接处必须设计合理，确保冷却剂能够顺畅流动，同时不影响整体结构的强度和密封性。最后是遥操作拆装，聚变堆的环境非常恶劣，辐射高，人类无法直接进入，因此所有内部件的安装和维护都必须通过远程操作完成，这对连接和固定技术的可操作性和便捷性提出了很高的要求。
-接下来，我得考虑不同的连接技术，比如机械紧固、焊接、钎焊和粘接等。每种方法都有其优缺点。比如，焊接可能提供很强的结构强度和良好的密封性，但可能会影响冷却系统的布局，且焊接后的部件可能难以拆卸，尤其是在需要远程操作的情况下。机械紧固虽然安装和拆卸较为方便，但可能会在高温和振动环境下出现松动或疲劳，影响结构强度和密封性。
-考虑到真空环境，可能需要使用特殊材料和工艺来确保密封性能。例如，使用金属密封圈或特定的焊接工艺。同时，冷却剂的流通可能需要在连接处设计专门的管道或通道，以保证流速和流量，同时不增加额外的结构负担。
-在权衡这些因素时，或许可以考虑混合使用不同的连接技术。例如，在需要高结构强度和密封性的区域使用焊接，而在需要频繁拆装维护的区域使用机械紧固件。同时，结合密封胶或密封剂来加强密封性能，同时不影响冷却剂的流通。
-另外，材料的选择也非常重要。选择能够承受高温、高辐射和强电磁力的材料，同时具有良好的加工性能，以便于制造和安装。例如，使用特殊合金或复合材料来提高连接处的强度和耐久性。
-最后，设计时还需要考虑到遥操作的具体需求，确保连接和固定技术能够支持机械臂或自动化的拆装工具进行操作。这可能包括设计易于抓取和操作的接口，或者使用可拆卸的模块化设计，方便远程更换和维护。
-综上所述，解决这个问题需要综合考虑多种因素，权衡各方面的技术要求，可能需要采用多种连接技术的组合，并结合先进的材料和设计方法，才能满足聚变堆内部件的连接和固定需求。
-&lt;/think&gt;
-### 聚变堆内部件连接与固定技术的权衡分析
+          <t>### 聚变堆内部件连接与固定技术的权衡分析
 #### 1. 核心结论
 在聚变堆内部件的连接与固定技术中，最优方案需采用组合式固定与密封技术，结合真空钎焊与机械紧固，辅以实时监测系统，以平衡结构强度、真空密封、冷却剂流通和遥操作拆装需求。
 #### 2. 背景与概念
@@ -3198,7 +2772,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -3224,15 +2798,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于聚变堆的热室设施的作用以及设计考虑的因素。我需要先理解热室到底是什么，然后分析它在聚变堆中的具体应用。
-首先，热室，英文叫Hot Cell，通常指的是用于处理高放射性物质的设施，里面环境高度辐射，需要远程操作。所以在聚变堆中，热室应该用于那些因中子辐照而变得高度放射性的部件的处理。
-接下来，思考热室的主要功能。可能包括部件的远程维护和修理，测试这些部件在辐照后的性能，以及处理产生的放射性废物。这些操作都需要在安全的环境中进行，确保工作人员不受到辐射伤害。
-然后，设计要求方面，辐射屏蔽是关键。热室需要使用厚重的材料，比如混凝土或铅，来阻挡辐射。此外，三废处理也很重要，因为聚变反应会产生放射性废物，包括气体、液体和固体，如何安全处理这些废物是一个挑战。遥操作兼容性也是必要的，因为所有操作都需要远程进行，可能需要设计专门的机器人或机械臂。
-还有一些其他考虑，比如通风系统，要保持空气流通并净化放射性气体；还有内部设备和接口的设计，确保所有设备都能在高辐射环境下正常工作。
-可能还需要考虑热室的结构布局，是否与其他设施连通，如何隔离不同区域以防止交叉污染。另外，材料选择也是一个重点，因为材料需要能承受高辐射剂量而不失效。
-总结一下，热室在聚变堆中扮演着不可或缺的角色，提供了一个安全的环境进行高放射性部件的处理。设计时需要综合考虑屏蔽、废物处理、远程操作等多个因素，确保设施的安全性和功能性。
-&lt;/think&gt;
-### 1. **核心结论**  
+          <t>### 1. **核心结论**  
 热室是聚变堆中用于处理高放射性部件和废物的关键设施，其设计需综合考虑辐射屏蔽、废物处理和远程操作等特殊要求。
 ---
 ### 2. **背景与概念**  
@@ -3329,7 +2895,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -3355,19 +2921,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>好，我现在需要比较分析三种主流计算等离子体物理的方法：磁流体力学（MHD）、回旋动理学（Gyrokinetics）和粒子模拟（PIC）。我得先从每个方法的基本概念入手，理解它们各自的物理模型和数值算法特点。
-首先，MHD。我听说过它将等离子体视为流体，用连续介质模型来描述。这样处理的话，计算量应该相对较小，适合研究大尺度的宏观现象，比如磁约束装置中的平衡和稳定问题。不过，MHD忽略了微观的粒子运动，所以对于涉及微尺度动力学的过程，可能不太适用。
-接下来是回旋动理学。这个名字让我联想到回旋运动，可能这种方法处理了部分微观效应，但做了回旋平均，所以计算量比PIC小，但比MHD大。它适用于介于流体和粒子之间的中间尺度，比如湍流、微不稳定性和输运现象。回旋动理学能够捕捉到更多的细节，比如不稳定性增长，这对于理解等离子体的湍流和输运非常重要。
-然后是粒子模拟（PIC）。这种方法直接模拟粒子的轨迹，保留了所有的动理学细节。这意味着它可以研究非常复杂的现象，比如波粒相互作用、高能粒子的行为等。不过，PIC的计算量非常大，通常需要处理大量的粒子和精细的时间步长，所以在计算资源有限的情况下，可能难以处理大规模的问题。
-接下来，我需要比较这三种方法的物理模型。MHD基于流体假设，忽略了粒子的个体运动，适用于宏观问题。Gyrokinetics在流体和粒子之间，考虑了部分微观效应，但通过回旋平均简化了计算，适合中间尺度的研究。PIC则保留了粒子的个体行为，适用于微观和复杂动力学现象。
-在数值算法方面，MHD使用有限差分或有限元方法，求解磁流体力学方程组。Gyrokinetics采用动理学方程，可能使用谱方法或有限差分，同时处理动理学分布函数。PIC则结合拉格朗日和欧拉方法，分别追踪粒子和计算场量。
-计算量需求方面，MHD相对较小，适合大规模计算；Gyrokinetics中等，适合中等规模；PIC最大，通常用于小规模的问题。
-适用领域方面，MHD用于托卡马克平衡、磁重联等宏观问题。Gyrokinetics处理离子回旋波、湍流等中间尺度现象。PIC适用于高能粒子动力学、波粒相互作用等复杂微观过程。
-比较与拓展部分，MHD效率高，但忽略微观效应；Gyrokinetics在中间尺度提供详细，计算量中等；PIC详细全面，但计算量大。因此，选择哪种方法取决于研究的问题规模和所需细节程度。
-最后，总结部分，我需要强调每种方法的优势和适用范围，指导实际应用中的选择。
-现在，我需要把这些思考整理成一个结构清晰的回答，按照用户的要求，分点详细说明每个部分。
-&lt;/think&gt;
-### **比较分析三种计算等离子体物理方法**
+          <t>### **比较分析三种计算等离子体物理方法**
 #### **1. 物理模型**
 - **磁流体力学（MHD）**
   - **模型**：将等离子体视为连续流体，忽略微观粒子运动。基于磁流体力学方程组，描述大规模宏观行为。
@@ -3412,7 +2966,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -3438,19 +2992,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于主流的MHD模拟程序及其在聚变等离子体稳定性研究中的应用。首先，我需要明确用户的需求。他们可能是一名研究人员或学生，想了解这些程序的特点和实际应用情况。
-用户提到了几个程序，比如NIMROD、JOREK、M3D-C1。我应该选择其中一个详细说明。考虑到JOREK在 ITER 等离子体研究中的广泛应用，这可能是一个好的选择，因为它与实际聚变装置的关系密切。
-接下来，我需要分析JORED的特点。它基于二维可扩展的谱有限元方法，能够在复杂几何下处理高精度的非线性MHD问题。这在破裂和ELMs的研究中很重要，因为这些现象涉及复杂的三维运动和非线性效应。
-然后，我需要考虑背景和概念，确保解释清楚MHD和等离子体稳定性的重要性。破裂和ELMs是影响聚变装置性能的关键问题，所以模拟程序的作用非常重要。
-在原理部分，我需要解释JOREK使用的方程和数值方法。比如，它使用欧拉方程，考虑磁场和流体运动的相互作用。谱有限元方法的优势在于高分辨率和并行效率，这对大规模模拟很重要。
-应用实例方面，应该包括破裂和ELMs的研究。破裂会导致极端热负荷和结构损坏，模拟可以帮助预测和缓解。ELMs会导致聚变装置的热负荷脉冲，研究如何控制它们的频率和幅度是关键。
-工程意义部分，需要说明JOREK如何帮助设计更稳定的装置，优化运行参数，减少对材料的损坏。这对ITER这样的大型装置尤其重要，因为它们的设计和运行依赖于准确的模拟结果。
-最后，比较与拓展部分，可以提到其他程序如NIMROD和M3D-C1，说明它们的优缺点。JOREK的优势在于处理复杂几何和多尺度问题的能力，这在研究边缘不稳定性时特别有用。
-总结时，应该强调JOREK在聚变研究中的关键作用，特别是在模拟复杂等离子体现象和优化装置设计方面的贡献。
-现在，我需要确保所有这些点都清晰地表达出来，并且结构符合用户的指示。每个部分都要有明确的小标题，使用LaTeX公式，并且在首次出现时给出单位。同时，要保持客观和严谨，避免猜测。
-总的来说，我需要构建一个结构严谨、内容详实的回答，满足用户对MHD模拟程序及其应用的全面理解。这不仅包括程序的特点，还包括它们在实际研究中的应用和影响，帮助用户更好地理解这些工具的重要性。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 JOREK 是一种主流的 MHD 模拟程序，广泛应用于聚变等离子体稳定性研究，特别是在破裂（Disruption）和边缘局部模态（ELMs）等关键现象的预测与分析中。
 ---
 ### 背景与概念  
@@ -3487,7 +3029,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -3513,15 +3055,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>好的，我现在要解答用户的问题。用户询问的是回旋动理学模拟在研究等离子体微观湍流和反常输运中的核心作用，以及5D模拟的计算量估算及其对高性能计算的依赖性。
-首先，我需要明确回旋动理学模拟的基本概念和GENE程序的作用。回旋动理学模拟是用来研究等离子体中微观尺度的湍流和输运现象，而GENE程序正是这类模拟中的典型工具。核心作用方面，我得突出它在理论建模、实验数据解释和指导工程设计方面的重要性。
-接下来是计算量的估算。问题中提到的5D模拟包括3个空间维度和2个速度空间维度，每个维度有N个网格点，时间步数为Nt。计算量通常与网格点数和时间步数的乘积有关。因此，总计算量应该是N的5次方乘以Nt，即O(N^5 * Nt)。
-然后，我需要解释为什么这种计算量依赖于高性能计算。因为N和Nt的值都很大，计算量呈指数增长，常规计算机无法在合理时间内完成，所以必须依赖超级计算机和并行计算技术。
-在思考过程中，我还需考虑可能的误差或遗漏。例如，实际模拟中可能采用优化算法，减少计算量，或者网格划分是否均匀等因素。但为了估算，假设所有维度的网格点数都相同，时间步数是线性的。
-此外，用户可能还希望了解高性能计算的具体应用，比如如何通过并行计算提高效率，或者分布式存储如何管理大量数据。这些都是解答中需要涵盖的点。
-最后，总结部分要简明扼要，强调回旋动理学模拟的重要性及其对计算资源的需求，为用户提供清晰的结论和应用启示。
-&lt;/think&gt;
-### 1. **核心结论**  
+          <t>### 1. **核心结论**  
 回旋动理学模拟（如GENE程序）通过求解Vlasov-Fokker-Planck方程，揭示等离子体微观湍流和反常输运的物理机制，为聚变装置设计提供关键理论支持。5D回旋动理学模拟的总计算量为$O(N^5 N_t)$，其对高性能计算的依赖性主要源于高维相空间离散化和长时间演化计算需求。
 ---
 ### 2. **背景与概念**  
@@ -3563,7 +3097,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -3589,19 +3123,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>好的，我现在需要回答关于高性能计算（HPC）的进步如何推动聚变等离子体模拟能力的发展，尤其是在更高保真度、更大规模、更长时间尺度的多物理场耦合模拟方面。
-首先，我应该从核心结论入手，明确高性能计算如何影响聚变模拟。高性能计算，尤其是exascale计算，能够显著提升聚变模拟的保真度、规模和时间尺度，从而帮助解决能源危机。
-接下来是背景与概念。我需要解释聚变等离子体模拟的重要性，以及高性能计算在其中的作用。聚变能是清洁的未来能源，托卡马克等装置需要复杂的等离子体控制，而模拟是理解其行为的关键。高性能计算通过更高的计算能力和内存扩展了模拟的范围。
-然后是原理与推导。exascale计算如何提升保真度、规模和时间？更高的计算能力意味着更精细的网格分辨率，减少数值误差。内存扩展允许处理更大的系统，捕捉更多物理过程。同时，长时间尺度模拟需要高效算法，exascale计算能处理更长时间。
-定量估算部分，我可以引用ITER装置的示例。假设ITER有10^21粒子，exascale计算使模拟时间从几天缩短到几小时，时间分辨率从秒级提高到毫秒级，网格点数从10^6增加到10^9。这显示了exascale计算带来的显著提升。
-工程和实验意义方面，高保真模拟能预测等离子体行为，指导实验设计和优化。大规模模拟帮助理解多尺度物理，多物理场耦合模拟则帮助控制不稳定性，提高能源效率。这些进步对设计下一代装置和优化现有装置运行至关重要。
-比较与拓展部分，我需要讨论exascale与前一代超级计算机（如petascale）的差异。exascale在计算能力和内存方面有显著提升，适合更复杂的模拟。此外，exascale还有高能效，减少运行成本。
-最后，要点总结要简明扼要。exascale计算提升了聚变模拟的能力，帮助解决更多复杂问题，对未来聚变能的实现意义重大。
-在整个思考过程中，我需要确保每个部分都有逻辑性，涵盖所有关键点，同时保持结构清晰，便于读者理解。此外，要使用专业术语，但确保定义明确，避免混淆。
-现在，我需要检查是否有遗漏的部分。比如，在原理部分是否详细解释了exascale如何提升每个方面？是否有足够的示例说明其影响？这些都是确保答案全面和准确的关键点。
-最后，确保语言流畅，逻辑连贯，每个部分自然衔接，使整个回答既有深度又易于理解。
-&lt;/think&gt;
-### 核心结论
+          <t>### 核心结论
 高性能计算（HPC）的进步，特别是exascale计算的实现，将显著提升聚变等离子体模拟的保真度、规模和时间尺度，从而推动多物理场耦合模拟的发展，为实现可控核聚变提供关键支持。
 ---
 ### 背景与概念
@@ -3664,7 +3186,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -3690,15 +3212,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>好的，我现在需要回答用户关于聚变研究中计算模型验证和确认（V&amp;V）的问题。首先，我得明确V&amp;V是什么，以及它们在聚变中的重要性。
-用户提到计算模型的验证和确认，所以我得区分这两者。验证通常是指模型是否正确地解决了数学方程，而确认则是模型是否准确地描述了现实世界的现象。这一点很重要，尤其是在复杂的等离子体模拟中。
-接下来，我需要思考V&amp;V在聚变研究中的具体应用。聚变涉及高温等离子体，实验条件极端且复杂，所以模拟在这种情况下尤为重要。但是，模拟是否可靠呢？这就需要严格的V&amp;V来确保结果的可信度。
-用户还问如何利用实验数据对模拟程序进行严格的V&amp;V。这里，我得考虑实验数据的获取方式，比如使用诊断工具测量温度、密度等参数。然后，如何将这些数据与模拟结果进行对比。这可能涉及到统计方法，比如计算误差范围或相关系数，来评估模拟的准确性。
-另外，我得考虑在实际操作中可能遇到的挑战。例如，实验数据可能有噪声，或者模拟的分辨率不够高，导致对比困难。这时候，可能需要进行一些假设，比如选择特定的实验条件，或者调整模拟参数以匹配实验结果。
-我还得想到，V&amp;V不仅仅是技术问题，还涉及到整个研究团队的合作。不同的专家可能需要共同分析结果，讨论可能的误差来源，并制定改进模拟的方案。
-总结一下，我的思考过程包括：区分验证和确认，理解它们在聚变研究中的作用，探讨如何利用实验数据进行V&amp;V，考虑实际挑战，以及团队合作的重要性。这些都需要在回答中体现出来，帮助用户全面理解V&amp;V的过程和应用。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 验证（Verification）和确认（Validation）（V&amp;V）是确保等离子体模拟程序可靠性的关键过程。验证关注模型是否正确地解决了所采用的数学方程，而确认关注模型是否准确地反映了实验或现实系统的行为。两者结合是评估模拟结果可信度的基础。
 ---
 ### 背景与概念  
@@ -3747,7 +3261,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -3773,16 +3287,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>嗯，我现在要回答关于人工智能和机器学习在聚变等离子体模拟和实时控制中的应用的问题。首先，我需要理解用户的需求，他们可能是一名研究人员或学生，对AI在聚变物理中的应用感兴趣，想要了解现状和潜力。
-我得从几个方面入手。首先是核心结论，需要简明扼要，概括AI和ML的主要贡献。然后是背景和概念，解释聚变等离子体的复杂性以及传统模拟方法的局限性，引出AI和ML的优势。
-接下来是原理与推导，这里可能需要分模拟和实时控制两部分来讨论。比如，在模拟中，代理模型如何通过机器学习来加速；在控制中，AI如何用于预测和抑制不稳定性。我需要列举具体的应用案例，比如破裂预测和EDS控制。
-然后是定量估算或示例部分，这里可能需要引用一些实际的数据或结果，比如预测破裂的成功率，或者ML模型在模拟中的计算时间减少情况。这些数据能够增强结论的可信度。
-工程或实验意义部分，需要说明AI和ML如何具体影响聚变装置的设计和运行，比如优化实验参数，提高装置效率，减少材料损伤等。这些都是实际应用中的关键点。
-比较与拓展部分，我得对比传统方法和AI方法的优缺点，比如计算速度、精度、适用范围等。同时指出当前AI方法的局限性，如数据依赖、解释性不足，以及未来的发展方向。
-最后，要点总结要简明扼要，重申AI和ML在加速模拟和实时控制中的重要性，并指出未来的研究重点。
-在整个思考过程中，我需要确保逻辑清晰，涵盖所有关键点，同时用严谨客观的语言表达，避免主观猜测。这样，用户能够得到全面且有深度的回答，帮助他们理解AI在聚变物理中的应用潜力。
-&lt;/think&gt;
-### 1. **核心结论**  
+          <t>### 1. **核心结论**  
 人工智能（AI）和机器学习（ML）在加速聚变等离子体模拟、参数优化及实时控制中展现出巨大潜力，已在代理模型构建、破裂预测和不稳定性控制等方面取得显著进展，成为现代聚变物理研究的重要工具。
 ---
 ### 2. **背景与概念**  
@@ -3829,7 +3334,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -3855,14 +3360,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>嗯，我需要回答关于多尺度、多物理场集成建模的问题，特别是以托卡马克的芯部和边界等离子体耦合为例。首先，我应该理解什么是多尺度和多物理场建模。多尺度意味着在不同空间和时间尺度上建模，比如托卡马克的芯部和边界，这两个区域的物理现象可能在不同的尺度下发生。多物理场则指的是同时考虑多种物理现象，如磁流体动力学（MHD）、电磁波、热传导等。
-接下来，我需要考虑托卡马克芯部等离子体和边界/偏滤器等离子体之间的耦合。芯部等离子体主要涉及高温高密度的等离子体，可能使用MHD模型来描述。而边界等离子体则可能涉及更多的复杂现象，比如湍流、射流、粒子输运等，可能需要不同的模型，比如等离子体流体力学或蒙特卡罗方法。
-然后，我要分析实现这种集成建模面临的挑战。可能的挑战包括不同模型之间的数据传输和同步问题，计算资源的限制，不同尺度和物理过程之间的相互影响，模型参数的不一致等。此外，如何处理不同模型的时间步长和空间分辨率也是一个问题。
-接下来，可能的解决方案可能包括开发耦合接口，使用中间层来协调不同模型的数据交换，采用适应性网格细化技术来处理不同尺度的问题，利用高性能计算资源来提高计算效率，以及开发统一的框架来管理多模型的集成。
-在具体的案例中，托卡马克的芯部和边界等离子体之间可能需要通过某种方式来传递热量、粒子和动量。这可能涉及到边界条件的处理，比如芯部模型的输出作为边界条件输入到边界模型中，反之亦然。同时，还需要处理不同物理过程之间的相互作用，比如湍流对粒子输运的影响。
-最后，我需要总结这些思考，指出多尺度、多物理场集成建模的重要性和面临的挑战，以及可能的解决方案。这可能有助于改善托卡马克装置的性能和设计，促进核聚变能的发展。
-&lt;/think&gt;
-### 多尺度、多物理场集成建模的定义
+          <t>### 多尺度、多物理场集成建模的定义
 **核心结论**：多尺度、多物理场集成建模是一种结合不同空间和时间尺度以及多种物理现象的建模方法，适用于复杂系统如托卡马克等离子体的研究。
 **背景与概念**：
 - **多尺度建模**：涉及不同空间（如微米到千米）和时间尺度（如纳秒到秒）的建模，用于捕捉系统中各种现象的动态。
@@ -3916,7 +3414,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -3942,17 +3440,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，我现在要回答关于模拟等离子体与壁相互作用（PMI）的计算方法的问题，具体包括分子动力学（MD）、二元碰撞近似（BCA）以及流体/动理学耦合模型如何描述溅射、再沉积和表面演化。这个问题有点复杂，但我得一步步理清楚。
-首先，我需要了解每个模型的基本概念和它们是如何工作的。分子动力学听起来像是基于原子级别的模拟，跟踪每个粒子的运动和相互作用。二元碰撞近似可能更简单，假设粒子之间只有两两碰撞，不考虑更复杂的相互作用。流体/动理学耦合模型可能是结合了流体动力学和动理学，用于处理更大尺度的问题。
-然后，我得弄清楚每个模型如何描述溅射、再沉积和表面演化。溅射是粒子撞击壁导致材料飞出，再沉积是这些粒子重新附着在壁上，表面演化就是壁的结构随时间变化。每个模型在处理这些过程时会有不同的方法和适用性。
-我应该考虑这些模型的优缺点。比如，MD虽然精确，但计算资源消耗大，可能适用于小区域或短时间的模拟。BCA在计算效率上可能更好，适合更大规模的模拟，但可能忽略了一些复杂的物理现象。流体/动理学模型可能在处理大尺度的流动和输运时更有效，但可能在细节上不够精确。
-接下来，我需要了解这些模型的应用场景。例如，MD可能在研究特定材料的溅射机制时很有用，而BCA可能在工程设计中用于估算再沉积的量。流体/动理学耦合模型可能在预测整个装置中的壁侵蚀情况时很有帮助。
-我还得考虑这些模型之间的比较，比如它们在处理不同物理现象时的准确性，以及计算资源的需求。可能需要指出在什么情况下选择哪个模型更为合适，比如在需要高精度时选择MD，在需要高效计算时选择BCA，在需要处理大尺度问题时选择流体/动理学模型。
-最后，我需要总结每个模型在描述PMI现象中的作用，以及它们在聚变装置设计和运行中的意义。可能还需要提到这些模型的潜在改进方向，比如如何提高计算效率，或者如何更好地结合不同模型的优点。
-在写作时，我需要确保每个部分都有清晰的标题，使用项目符号和分点来组织内容，方便读者快速浏览。同时，语言要保持专业但不晦涩，确保物理量的单位和符号正确标注。如果有不确定的地方，比如某个模型的具体应用细节，我应该明确指出需要进一步的信息或研究。
-总的来说，我需要系统地介绍每个模型，分析它们如何处理溅射、再沉积和表面演化，比较它们的优缺点，并总结它们的应用价值。这样，读者就能全面理解这些计算方法在模拟PMI中的角色和重要性。
-&lt;/think&gt;
-### 讨论用于模拟等离子体与壁相互作用（PMI）的计算方法
+          <t>### 讨论用于模拟等离子体与壁相互作用（PMI）的计算方法
 #### **1. 核心结论**
 分子动力学（MD）、二元碰撞近似（BCA）及流体/动理学耦合模型各有特点，MD适合微观精确模拟，BCA适用于中等尺度的高效计算，而流体/动理学耦合模型适合宏观尺度的大规模模拟。选择模型需根据研究目标和计算资源权衡。
 #### **2. 背景与概念**
@@ -3993,7 +3481,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -4019,16 +3507,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>嗯，我得帮用户理解如何用计算模拟工具优化聚变装置的设计，比如仿星器的磁体或偏滤器。首先，核心结论应该是参数扫描和优化算法是主要方法。
-接下来，背景和概念部分，我得提到聚变装置设计涉及的多物理场和多目标优化，还有计算模拟工具在这里的重要性。可能要列出一些关键概念，比如参数扫描、优化算法、物理约束、工程约束，还有多物理场模拟。
-然后，关于原理与推导，参数扫描是系统地改变输入参数，观察输出变化，这样可以找到设计变量和性能指标之间的关系。而优化算法，比如遗传算法，粒子群优化，这些是从众多可能性中找到最优解的。需要说明这些算法是如何在设计空间中搜索的，以及它们如何处理约束条件。
-定量估算部分，我可以举一个例子，比如仿星器的优化设计。假设设计变量包括磁体形状、偏滤器几何参数，目标函数是等离子体约束性能，约束条件是成本、空间限制。然后列出每个步骤的具体参数和结果。
-工程或实验意义部分，要强调优化后的设计在提高性能的同时，降低实验成本，减少调试时间，同时可以验证理论模型，为未来装置提供参考。
-比较与拓展的话，可以比较不同优化算法，比如遗传算法适用于复杂问题，粒子群在高维问题中表现好，随机森林适合高计算成本的情况。但每种算法都有优缺点，选择时要考虑问题规模和计算资源。
-最后，要点总结要再次强调参数扫描和优化算法的作用，同时结合专家经验和工程需求，确保设计的可行性和可靠性。
-整个思考过程要保持逻辑清晰，步骤分明，确保用户能够理解每个环节的作用和相互关系。
-&lt;/think&gt;
-### 1. 核心结论  
+          <t>### 1. 核心结论  
 通过参数扫描和优化算法进行聚变装置设计优化的关键在于：在多物理场模拟的基础上，系统性地探索设计参数空间，结合物理约束和工程约束，利用优化算法自动寻找最优设计方案。
 ---
 ### 2. 背景与概念  
@@ -4090,7 +3569,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -4116,14 +3595,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，用户是一位资深的聚变等离子体物理与工程专家，可能正在处理大型托卡马克或仿星器的相关模拟工作。他提出的问题是在大规模聚变等离子体模拟时，数据管理、可视化和后处理面临哪些挑战，以及如何有效提取有用物理信息。
-首先，我需要分析数据管理方面的挑战。大规模模拟会产生海量数据，存储和管理这些数据是一个难题。可能需要考虑数据压缩、分布式存储等方法，但又要避免影响数据的完整性和可用性。另外，数据格式的标准化也很重要，确保不同团队和工具能够兼容使用。
-接下来是可视化部分。聚变等离子体的数据通常在时间和空间上都是高分辨率的，传统的可视化方法可能无法高效处理，导致速度慢或者结果不直观。需要开发更高效的可视化工具，可能结合机器学习或者GPU加速来提升性能。
-然后是数据后处理。如何从庞大的数据中提取有用的物理信息是一个关键问题。传统的方法可能效率低下，需要引入机器学习和AI技术，比如聚类分析、模式识别等，来帮助自动识别关键物理现象，减少人工干预的需求。
-在提出解决方案时，我需要考虑到每一方面的具体措施。例如，数据管理可以采用层次化存储和数据压缩技术，同时建立统一的数据格式和管理系统。可视化方面，可以开发支持大规模数据的渲染工具，并利用机器学习辅助分析。后处理则可以通过AI模型来自动化分析，提取重要的物理特征。
-最后，总结一下，关键是要综合运用数据管理优化、高效可视化工具和AI驱动的分析方法，来应对这些挑战，从而帮助专家们更好地理解和优化聚变装置的性能。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 在大规模聚变等离子体模拟中，数据管理、可视化和后处理面临数据量庞大、维度复杂、实时性要求高以及物理信息提取困难等挑战。通过采用分布式存储、高效压缩算法、机器学习辅助分析和并行可视化技术，可以在海量数据中提取有用的物理信息。
 ---
 ### 背景与概念  
@@ -4237,7 +3709,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -4263,18 +3735,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>嗯，用户让我详细分析p-¹¹B聚变相对于D-T聚变在燃料特性、反应产物、中子产生、材料活化和潜在能量转换方式方面的优势。然后还要解释为什么p-¹¹B被认为是“清洁”的燃料。好的，我得一步一步来。
-首先，用户可能是一位对核聚变技术感兴趣的人，或者是正在研究相关领域的学生或工程师。他们需要了解p-¹¹B聚变的优势，特别是与常用的D-T聚变相比。深层需求可能是寻找更清洁、更安全的核聚变方案，或者是在设计新的聚变装置时考虑使用这种燃料。
-接下来，我得整理p-¹¹B和D-T聚变的基本信息。D-T聚变是现在托卡马克装置中最常用的方法，因为它容易点火，但会产生大量中子和放射性废物。而p-¹¹B理论上更清洁，但需要更高的温度和更复杂的等离子体约束。
-燃料特性方面，p-¹¹B中的硼-11天然丰度高，获取容易，但需要使用离子注入器分离。氘和氚则相对丰度低，尤其是氚需要从锂中生产。然后是反应产物，D-T产生中子，而p-¹¹B产生氦，不会导致材料活化。
-中子产生方面，D-T反应释放大量快中子，这些中子会活化材料，导致放射性废物和材料退化。而p-¹¹B反应不释放中子，所以材料活化问题较少。
-材料活化方面，D-T需要处理放射性活化产物，而p-¹¹B装置的材料活化低，分解后即可安全处理，大幅降低辐射风险和处理成本。
-能量转换方面，D-T的中子能量难以高效利用，而p-¹¹B的聚变产物氦可以直接提取，减少能量损失，提高效率。此外，p-¹¹B反应产生的粒子能量更高，可能更适合某些特定的能量转换方法。
-为什么p-¹¹B被认为是清洁的呢？主要是因为没有中子，所以材料活化少，放射性废物少，装置设计也更安全。但同时也要提到它的挑战，比如高温、材料设计困难和等离子体约束问题，这些限制了它的实际应用。
-现在，我得确保这些分析涵盖用户提到的所有方面，并且结构清晰，每个部分都有足够的细节和比较。可能需要添加一些示例或数字来支持论点，比如温度需求、反应截面等。这样用户能更直观地理解两种聚变方法的优劣。
-最后，总结时要强调p-¹¹B的优势，同时指出其目前的技术挑战，让读者明白虽然它有潜力，但要实现还需要克服一些困难。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 p-¹¹B聚变相较于D-T聚变，具有更清洁的反应特性、更低的材料活化风险和更高效的能源转换潜力，因而被视为一种“清洁”的聚变燃料。
 ---
 ### 背景与概念  
@@ -4341,7 +3802,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -4367,90 +3828,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>嗯，我现在要解决的是关于p-¹¹B聚变反应中轫致辐射功率密度PBrem与聚变功率密度Pfus之比的问题。首先，我需要理解问题的背景和各个参数的含义。
-问题给出：p-¹¹B的理想点火温度Ti约为300keV。等离子体密度ne≈6nB，其中nB是硼离子的密度，质子与硼离子的比例是1:1。此外，等离子体是准中性的，所以电子温度Te=Ti=300keV。
-我需要估算PBrem/Pfus的表达式，并讨论为什么这个比值对p-¹¹B聚变构成严峻挑战。
-首先，我得回忆一下相关的物理公式和概念。
-1. 肋致辐射功率密度PBrem：这是由于等离子体中带电粒子的轫致辐射所释放的能量。一般来说，轫致辐射的功率密度与电子温度、离子温度、电荷数、密度等因素有关。公式应该类似于PBrem ~ (n² * Z² * T_e^3) 的形式。
-2. 聚变功率密度Pfus：聚变功率取决于反应的速率，而反应速率通常由⟨σv⟩（截面乘以相对速度）和反应物的密度决定。对于p-¹¹B反应，Pfus = n_p * n_B * ⟨σv⟩_{pB}。
-问题要求给出PBrem和Pfus的比例，并分析其对聚变的挑战。
-接下来，我需要分别推导这两个功率密度的表达式，然后求出它们的比值。
-首先，处理PBrem：
-在高温等离子体中，轫致辐射主要来自电子和离子之间的相互作用。计算式通常为：
-PBrem = (16 * sqrt(2) * π^2 * n_e * n_i * Z^2 * (k_B T_e)^4) / (3 * (h c)^3))
-其中：
-- n_e是电子密度，
-- n_i是离子密度，
-- Z是离子电荷数，
-- T_e是电子温度，
-- k_B是玻尔兹曼常数，
-- h是普朗克常数，
-- c是光速。
-但问题中提到ne≈6nB，而n_i（离子密度）等于nB，因为硼离子密度是nB，质子密度是nB，总离子密度是2nB？或者可能等离子体是准中性的，所以n_e = n_i = Z * nB？这里可能需要进一步澄清。
-根据问题描述，ne≈6nB，其中nB是硼离子密度，而质子和硼离子的比例是1:1，所以总离子密度n_i = n_p + n_B = nB + nB = 2nB。但是ne=6nB，这说明电子密度是离子密度的三倍，这与准中性情况不符。准中性情况下，n_e = n_i，因为每个离子贡献Z个电荷，所以总电荷守恒：n_p * Z_p + n_B * Z_B = n_e。质子的电荷Z_p=1，硼的电荷Z_B=5，所以n_p + 5n_B = n_e。问题中提到n_p = n_B，所以n_p = n_B，代入得n_p + 5n_p = 6n_p = n_e，所以n_e=6n_p=6n_B，因为n_p=nB。因此，n_i = n_p + n_B = 2n_B，而n_e=6n_B。所以准中性等式成立。
-因此，n_e=6n_B，n_i=2n_B，其中n_i中的每个离子是硼和质子的组合。但是计算PBrem时，可能需要分别考虑每种离子的贡献，或者简化为平均Z值。
-不过，问题可能更简单地将总离子密度视为n_i = n_p + n_B = 2n_B，而Z=5（因为硼的电荷是5，质子是1？或者是否应该考虑质子的贡献？）
-这可能有点复杂，因为质子和硼离子的电荷不同。所以，总离子的平均Z可能为（n_p * Z_p + n_B * Z_B） / (n_p + n_B) = (nB *1 + nB *5)/(2nB) )= 6nB/(2nB)=3。因此，平均Z=3。
-所以，在计算PBrem时，可能可以取Z=3，n_i=2nB，n_e=6nB，或者分别计算质子和硼离子的贡献，然后相加。
-不过，为了简化，可能取平均Z=3，然后用n_i=2nB。或者，分开计算质子和硼对PBrem的贡献。
-因为问题中给出了n_p =n_B，所以n_p= n_B，n_e=6n_B，n_i=2nB。
-所以，对于PBrem，考虑每种离子的贡献，即质子和硼离子。
-质子的Z_p=1，n_p=n_B。
-硼离子的Z_B=5，n_B=n_B。
-因此，总PBrem = PB_p + PB_B，其中PB_p是质子引起的轫致辐射，PB_B是硼离子引起的。
-计算PB_p：
-PB_p = (16 * sqrt(2) * π^2 * n_e * n_p * Z_p^2 * (k_B T_e)^4) / (3 * (h c)^3))
-同样，PB_B = (16 * sqrt(2) * π^2 * n_e * n_B * Z_B^2 * (k_B T_e)^4) / (3 * (h c)^3))
-所以，总PBrem = PB_p + PB_B = (16 * sqrt(2) * π^2 * n_e * T_e^4 / (3 * (h c)^3)) ) * (n_p Z_p^2 + n_B Z_B^2)
-代入n_p =n_B，Z_p=1，Z_B=5：
-n_p Z_p^2 + n_B Z_B^2 = n_B (1^2 +5^2)=n_B (1+25)=26n_B
-所以，PBrem = (16 sqrt(2) π^2 n_e T_e^4 / (3 (h c)^3)) * 26 n_B
-但n_e=6n_B，所以：
-PBrem = (16 sqrt(2) π^2 * 6n_B * T_e^4 * 26 n_B ) / (3 (h c)^3 )
-= (16 sqrt(2) π^2 *6*26 n_B^2 T_e^4) / (3 (h c)^3 )
-= (16*6*26 sqrt(2) π^2 n_B^2 T_e^4) / (3 (h c)^3 )
-= (16*6*26/3) * sqrt(2) π^2 n_B^2 T_e^4 / (h c)^3 )
-计算系数：6/3=2，所以16*2*26=16*52=832
-所以，PBrem = (832 sqrt(2) π^2 n_B^2 T_e^4) / (h c)^3 )
-或者，可以将系数简化为符号形式，例如包括常数项。
-另一方面，Pfus = n_p n_B ⟨σv⟩_{pB}
-因为n_p=n_B，所以Pfus = n_B^2 ⟨σv⟩_{pB}
-因此，PBrem/Pfus = [ (常数项) * n_B^2 T_e^4 ] / [n_B^2 ⟨σv⟩_{pB} ] = (常数项 * T_e^4) / ⟨σv⟩_{pB}
-现在，我需要分析这个比值是否大，即是否PBrem &gt; Pfus，这将导致聚变能量无法有效积累，从而无法维持聚变燃烧。
-通常，聚变反应中，聚变功率需要大于辐射损失，否则等离子体无法维持高温，点火失败。
-因此，PBrem/Pfus 应该远小于1，否则聚变无法持续。
-接下来，我需要推导这个比值的表达式，并讨论其对p-¹¹B聚变的挑战。
-首先，表达式：
-PBrem/Pfus ≈ [C * n_B^2 T_e^4] / [n_B^2 ⟨σv⟩ ] = C T_e^4 / ⟨σv⟩
-其中，C包含所有常数项和Z相关的因素。
-接下来，分析当Ti=300keV时，这个比值是否很大。
-计算常数项：
-常数项C = (832 sqrt(2) π^2 ) / (h c)^3 )
-需要计算这个值的大致量级，以估计C的值。
-但是，问题可能只需要符号形式，因此可以用符号表达，而不具体计算数值。
-所以，表达式可以表示为：
-PBrem/Pfus = (C Z^2 n_e T_e^4 ) / ⟨σv⟩_{pB} }
-这里可能需要调整符号，以更准确地反映各参数的影响。
-或者，更精确地说，PBrem/Pfus = [ (16 sqrt(2) π^2 n_e (n_p Z_p^2 + n_B Z_B^2) (k_B T_e)^4 ) / (3 (h c)^3) ) ] / (n_p n_B ⟨σv⟩_{pB} )
-代入n_p =n_B，n_e=6n_B，Z_p=1，Z_B=5：
-PBrem/Pfus = [16 sqrt(2) π^2 * 6n_B * (n_B (1 +25)) * (k_B T_e)^4 ) / (3 (h c)^3) ) ] / (n_B^2 ⟨σv⟩_{pB} )
-= [16 sqrt(2) π^2 *6n_B * 26n_B * k_B^4 T_e^4 ) / (3 (h c)^3) ) ] / (n_B^2 ⟨σv⟩ )
-= [16*6*26 sqrt(2) π^2 n_B^2 k_B^4 T_e^4 / (3 (h c)^3) ) ] / (n_B^2 ⟨σv⟩ )
-= [ (16*6*26/3) sqrt(2) π^2 k_B^4 T_e^4 ) / (h c)^3 ) ] / ⟨σv⟩
-= [ (832 sqrt(2) π^2 k_B^4 T_e^4 ) / (h c)^3 ) ] / ⟨σv⟩
-所以，PBrem/Pfus ≈ (C * T_e^4 ) / ⟨σv⟩，其中C是一个包含所有常数项的系数。
-现在，问题转化为为什么这个比值在p-¹¹B聚变中很高，导致挑战。
-原因可能在于：
-1. T_e=300keV，这使得T_e^4非常大，从而PBrem增加很快。
-2. p-¹¹B反应的⟨σv⟩相对较小，因为这是一个较难的聚变反应，需要高能量（如D-T反应的点火温度较低，而p-¹¹B需要更高的温度，因此在相同温度下，⟨σv⟩可能较低？或者相反？这需要确认。）
-或者，可能在高温下，⟨σv⟩随温度变化的情况，例如，⟨σv⟩ ∝ T^0.5或更高，具体取决于截面的温度依赖性。
-另外，截面 ⟨σv⟩ 随温度的变化情况也会影响PBrem/Pfus的比值。
-通常，聚变反应率 ⟨σv⟩ 在高温下会增加，但可能不如T_e^4增加得快，因此PBrem/Pfus可能会变得很大。
-此外，p-¹¹B反应的截面可能在高温下有特定的行为，这可能使得⟨σv⟩不够大，无法克服高温下的辐射损失。
-总结来说，PBrem与Pfus的比值随着T_e^4增长，而⟨σv⟩可能增长较慢，导致这个比值很大，使得聚变无法持续，因为辐射损失太大，无法积累足够的能量来维持点火。
-现在，我需要将这些分析整理成结构化的回答，按照用户的要求，分为各部分。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 对于p-¹¹B聚变，其理想点火温度约为300keV，此时轫致辐射功率密度与聚变功率密度之比PBrem/Pfus较大，对维持聚变燃烧构成严峻挑战。
 ---
 ### 背景与概念  
@@ -4509,7 +3887,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -4535,17 +3913,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>好的，我现在要仔细思考用户的问题。用户的问题是关于p-¹¹B等离子体中离子温度Ti和电子温度Te的关系对聚变功率和辐射损失的影响，以及为什么通常需要维持Ti&gt;Te，以及实现和维持这种非平衡态面临的挑战。
-首先，我需要理解问题的基本背景。p-¹¹B聚变反应是聚变能源研究的一个重要方向，因为它是一种无碳、清洁的聚变燃料。在托卡马克等聚变装置中，等离子体需要达到极高的温度和压力才能发生聚变反应。在这个过程中，离子温度和电子温度的关系是非常关键的参数。
-接下来，我要考虑Ti&gt;Te的原因。这可能与聚变反应的热力学条件有关。聚变反应率通常与离子温度有关，因为反应发生在离子之间。如果Ti高于Te，可能会有助于提高反应率，从而增加聚变功率。另一方面，电子温度过高可能会导致更多的辐射损失，因为高温电子更容易通过轫致辐射等方式损失能量。因此，维持Ti&gt;Te可能有助于减少辐射损失，提高能量的利用率。
-然后，我需要分析这种非平衡态对聚变功率和辐射损失的具体影响。聚变功率主要取决于离子的温度和密度，而辐射损失则与电子的温度和密度有关。如果Ti高于Te，可能会降低辐射损失，因为电子温度较低，辐射强度较低。同时，较高的Ti可以提高聚变反应率，从而增加聚变功率。这可能是一个优化的过程，需要平衡两者的关系以达到最佳的聚变效率。
-接下来，我要探讨实现和维持这种非平衡态所面临的加热和约束挑战。加热方面，通常使用射频波加热、中性束注入等方式来加热离子。然而，这些方法可能需要更高的能量输入，以维持较高的Ti。同时，如何避免电子温度过高也是一个挑战，可能需要精确控制加热的方式和功率分配。
-约束方面，等离子体的约束性能直接影响温度的分布和保持。在托卡马克装置中，磁约束的质量直接影响到温度梯度和热传导。如果约束性能不佳，温度梯度可能无法维持，导致Ti和Te趋于平衡。因此，需要优化磁约束，减少热传导损失，以维持Ti&gt;Te的状态。
-我还需要考虑其他可能的因素，比如等离子体的稳定性。高温离子可能会导致不稳定性，如 Alfven波不稳定性，这可能对装置的运行产生负面影响。因此，在维持Ti&gt;Te的同时，还需要确保等离子体的稳定性，避免出现严重的不稳定性问题。
-另外，诊断和控制也是一个挑战。实时监测Ti和Te的温度，并进行精确的控制，以维持所需的温度梯度，这对于聚变装置的运行至关重要。这需要先进的诊断技术和控制系统，能够快速响应并调整加热和约束参数。
-最后，我需要总结这些思考，形成一个有条理的回答。回答需要包括核心结论、背景与概念、原理与推导、定量估算、工程或实验意义、比较与拓展以及要点总结。在回答中，要确保使用规范的单位，清晰的概念定义，并结合实际聚变装置的情况，提供具体的分析和建议。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 在p-¹¹B等离子体中，维持离子温度（$T_i$）高于电子温度（$T_e$）可以有效提升聚变功率并减少辐射损失。然而，实现并维持这种非平衡态需要克服加热效率、能量约束和稳定性等方面的挑战。
 ---
 ### 背景与概念  
@@ -4592,7 +3960,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -4618,18 +3986,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>嗯，用户让我解释“α粒子通道效应”（alpha channeling）的物理机制，以及它如何改善p-¹¹B聚变的能量经济性。好，我得先弄清楚什么是α粒子通道效应。我记得这和托卡马克中的等离子体加热有关，α粒子指的是氦核，也就是聚变反应产生的高能粒子。
-首先，背景和概念。托卡马克中的聚变反应生成α粒子，这些粒子的高能量可能会导致问题，比如热损失或维持等离子体所需的能量。传统上，这些α粒子的热量会部分损失，这不利于能量经济性。所以，通道效应的目的是利用这些高能粒子，而不是让它们白白流失。
-物理机制方面，我记得这涉及到波-粒子相互作用。利用外部射频波或者等离子体本身的波动，与α粒子发生共振，使得它们的能量被有效地提取出来。这样，α粒子的能量可以被转换为其他形式，比如用于加热燃料离子，或者直接转化为电能，从而提高聚变装置的能量输出。
-接下来，能量经济性方面。在p-¹¹B聚变中，主要产物是α粒子和中子。常规情况下，α粒子的动能可能无法被完全利用，导致效率低下。而通过通道效应，可以将这些α粒子的能量更多地用于有用功，比如加热或者发电，这样就能减少所需的外部加热功率，提高能量的利用率。
-在实际应用中，这可能涉及到设计特定的波系统，调整等离子体参数以优化通道效应。同时，也需要考虑工程上的可行性，比如如何有效发射射频波，如何诊断和控制这种效应。
-用户可能希望了解这个机制的具体工作原理，以及它对聚变装置的实际意义。他们可能还想知道这种技术是否已经在实验中得到验证，或者还有哪些挑战需要克服。此外，用户可能想比较其他提高能量经济性的方法，比如其他类型的加热或能量转换技术，通道效应的优势和局限性是什么。
-总结一下，我需要详细解释α粒子通道效应的机制，涉及到波与粒子的相互作用，以及如何通过这种方式将α粒子的能量转化为有用的输出。同时，还要说明这如何直接影响p-¹¹B聚变的能量经济性，可能包括减少能源浪费，提高效率，或者减少对其他能源输入的依赖。
-在写作时，我需要确保结构清晰，每个部分都有明确的小标题，使用LaTeX方程来解释关键公式，比如波数、频率等参数的关系。还要给出具体的应用场景，比如在托卡马克中的潜在实现方式，以及可能遇到的工程挑战。
-最后，要点总结部分要简洁明了，重申该效应的重要性，以及对聚变装置设计和运行的潜在影响。这可能包括建议在设计中考虑通道效应，以优化能量输出，同时指出需要进一步研究的地方，比如不同参数下的效果，或者与其他技术的比较。
-总的来说，我需要系统地解释这个概念，从基本原理到实际应用，确保内容准确且易于理解，同时满足用户的需求，可能涉及到的技术细节和实际意义。
-&lt;/think&gt;
-### **核心结论**  
+          <t>### **核心结论**  
 α粒子通道效应（alpha channeling）是一种通过波-粒子相互作用机制，将聚变产生的高能α粒子的能量高效利用的技术，可用于改善p-¹¹B聚变装置的能量经济性。
 ---
 ### **背景与概念**  
@@ -4675,7 +4032,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -4701,17 +4058,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>好，我现在要回答用户关于TAE Technologies使用场反位形（FRC）约束p-¹¹B等离子体的问题。首先，用户问FRC在约束这种高β、高温等离子体方面有何潜在优势，以及TAE在NBI驱动FRC方面的关键进展。
-先来看第一个问题，FRC的优势。我需要回想FRC和托卡马克的基本结构和原理。FRC的特点是磁场主要是由电流产生的，而托卡马克主要是环向磁场。高β等离子体意味着等离子体压强大，这对于托卡马克来说可能是个挑战，因为托卡马克需要较强的磁场来维持等离子体稳定，而FRC在高β情况下可能更稳定。此外，FRC的结构可能更紧凑，这对工程实现有好处。
-接下来，考虑高温等离子体。高温等离子体的热传导和约束是关键。FRC可能在磁通量管中更好地约束等离子体，减少热量损失，从而在高温下表现更好。另外，FRC的几何形状可能更容易实现长时间的等离子体约束，这对聚变反应来说很重要。
-然后是高比压，也就是高β值。FRC通常能支持更高的β值，这意味着在相同的磁场下，等离子体的压力更高，这对聚变反应效率有帮助。托卡马克则需要更强大的磁场来维持高β，这会增加工程难度和成本。
-在诊断方面，FRC的紧凑结构可能使诊断更容易，因为磁通量管的结构相对简单，而托卡马克的复杂结构可能使得诊断更困难。
-接下来是TAE在NBI驱动FRC方面的进展。NBI是中性束注入，用于加热和驱动等离子体。TAE可能在NBI的效率、注入束的控制和与FRC的兼容性方面有进展。高效的NBI可以提升等离子体的温度和密度，这对聚变反应至关重要。此外，优化NBI在FRC中的应用可能涉及束的注入角度、能量和密度控制，以最大化等离子体的响应。
-在控制方面，FRC的稳态运行可能得益于NBI提供的持续加热和驱动，避免了托卡马克常见的脉冲运行限制，从而延长等离子体的运行时间，提高聚变装置的性能。
-最后，TAE可能在等离子体稳定性方面取得了进展，通过NBI驱动实现更好的等离子体平衡和稳定性，减少湍流损失，从而提高能量约束时间。这对聚变装置的整体效率和可行性有重要影响。
-综上所述，FRC在高β、高温等离子体方面有独特优势，而TAE在NBI驱动技术上的进展为FRC的实际应用提供了重要支持，推动了紧凑型聚变装置的发展。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 场反位形（FRC）在约束高β、高温等离子体方面具有高β承载能力、优越的热传导特性及紧凑结构的优势；TAE在NBI驱动FRC方面取得了高能量注入效率、稳定等离子体运行及先进诊断技术的关键进展。
 ---
 ### 背景与概念  
@@ -4762,7 +4109,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -4788,13 +4135,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>好的，我现在需要回答关于激光驱动p-¹¹B聚变方案，特别是质子快点火的基本原理，以及它与磁约束聚变的异同和挑战。首先，我要确保自己理解了p-¹¹B聚变是什么，它是利用质子（p）与硼-11（¹¹B）核聚变，产生两个氦-4（³He）核，释放能量。
-接下来，我需要了解质子快点火的原理。这是激光驱动的内点火机制，激光产生的质子束在燃料内部加热，这与传统惯性约束中的外点火不同。质子通过与燃料原子核的弹性散射传递能量，导致燃料内部温度骤升，触发聚变链式反应。
-然后，我需要将激光驱动与磁约束聚变进行比较。激光驱动的特点是高能量、高功率激光器，而磁约束依赖于强大的磁场，如托卡马克或仿星器。两者在燃料压缩、点火机制和等离子体约束方面都有所不同。激光驱动的燃料可能以固态形式开始，而磁约束则通常使用气态或等离子态燃料。
-关于异同点，激光驱动的优点在于可能更高效地达到聚变条件，因为质子束直接加热燃料内部。而磁约束的优势在于可维持长时间的聚变反应，适合发电。挑战方面，激光驱动需要极高的激光能量和精确控制，可能面临激光与燃料相互作用的不确定性。磁约束则面临等离子体稳定性控制的难题。
-最后，我需要思考这些信息如何整合成一个结构清晰、符合要求的正式回答，确保涵盖核心结论、背景与概念、原理分析、比较与拓展等部分。
-&lt;/think&gt;
-### 核心结论
+          <t>### 核心结论
 激光驱动的p-¹¹B聚变方案（如质子快点火）通过激光产生的质子束直接加热燃料内部，实现高效点火，与磁约束聚变相比，具有更高的能量转换效率和更低的中子辐射，但面临极端激光参数需求和精确控制的挑战。
 ### 背景与概念
 p-¹¹B聚变是一种核聚变反应，质子（p）与硼-11（¹¹B）聚变生成两个氦-4（³He）核，并释放能量。质子快点火是一种内点火机制，利用高功率激光产生的质子束直接加热燃料靶丸的内部，触发聚变反应。磁约束聚变则通过磁场约束高温等离子体，使其持续发生聚变。
@@ -4820,7 +4161,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -4846,18 +4187,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于D-³He聚变燃料循环的特点、优势和挑战，还有自旋极化燃料的影响。首先，我得确定D-³He燃料循环的基本情况，比如反应式和主要产物。D-³He的反应式是D + ³He → α + p，这个反应主要产生α粒子（氦核）和质子，所以带电粒子产物为主，中子很少，这应该是它的主要优势之一。
-接下来，考虑带电粒子产物的好处。因为不需要中子辐照材料，材料的寿命会更长，装置的结构也可能更简单，辐射防护的问题也减轻了。此外，带电粒子的能量可以直接转化为电能，效率可能更高。
-然后，优势方面可能还有中子产额低，这对装置的材料选择和防护有好处。低中子产额意味着核废料较少，装置可能更安全，更易于维护。
-不过，挑战方面，³He的来源是个大问题。自然界的³He非常稀少，主要存在于天然气和月球土壤中，但目前地球上的储备有限，如果要大规模使用，可能需要从月球进口，这显然成本和技术上都有很大挑战。
-还有燃料循环的问题。D-³He的反应产生的氦-4可能需要从等离子体中分离出来，否则会影响反应效率。此外，混合燃料的供应和管理也可能比较复杂，因为需要同时供应D和³He。
-关于自旋极化燃料的影响，我需要回顾一下相关知识。自旋极化是指粒子的自旋方向高度一致，这可能会影响反应率。在某些情况下，自旋极化可以提高反应的截面，从而提高反应率，这可能对聚变性能有帮助。
-另外，自旋极化可能会导致聚变产物的角分布发生变化。比如，如果燃料的高度自旋极化，聚变产物可能在特定方向上更集中，这对装置的中子和粒子束流控制可能有影响，可能需要调整设计来适应这种分布。
-总结一下，D-³He燃料循环的优势在于带电粒子产物为主、中子产额低，但挑战在于燃料来源有限，燃料循环复杂。自旋极化可能提高反应率并影响产物分布，但还需要更多的研究来验证这些影响。
-最后，回答问题时，我需要按照规范的结构来组织内容，确保每个部分都有详细的信息，同时语言要严谨，使用正确的物理符号和单位。比如，在讨论反应式时，使用LaTeX来书写方程，解释每个符号的含义，这有助于读者理解。
-总的来说，我需要从背景、优势、挑战、自旋极化的影响等方面全面分析D-³He燃料循环，并提供工程或实验上的意义，指出未来研究的方向。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 D-³He聚变燃料循环具有低中子产额和以带电粒子产物为主的优势，但面临³He燃料来源有限和燃料循环管理的挑战。自旋极化燃料可能显著提高反应率并改变聚变产物的角分布。
 ---
 ### 背景与概念  
@@ -4908,7 +4238,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -4934,14 +4264,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>好的，我需要详细解释缪子催化聚变（μCF）的基本原理、为何可以在较低温度下发生，以及当前面临的主要瓶颈和可能的解决方案。让我分步骤来思考这个问题。
-首先，缪子催化聚变的基本原理是什么？缪子是一种基本粒子，类似于电子，但质量更大。在聚变反应中，缪子可以替代电子，使得原子核之间的库仑势垒降低，从而更容易发生聚变反应。
-接下来，为什么μCF可以在较低温度下发生？因为缪子的中子化效应使得原子核之间的距离更近，从而降低了反应所需的温度。这与传统聚变需要极高温的情况不同。
-现在，关于主要瓶颈，首先是α粒子粘滞问题。在聚变反应中，产生的α粒子可能会被氢原子捕获，形成He-4，这可能会阻碍进一步的聚变反应。其次，缪子的产生需要大量能量，因为缪子是不稳定的，需要通过高能粒子加速器来产生，这增加了成本和复杂性。
-可能的解决方案包括优化反应堆设计以减少α粒子的捕获，或者寻找更高效的缪子产生方法，比如利用更高能的粒子束或改进加速器技术。此外，还可以探索使用其他类型的催化剂或改进聚变燃料的循环利用，以提高效率并降低成本。
-综上所述，缪子催化聚变虽然在理论上可行，但实际应用中仍面临诸多技术挑战。需要在材料科学、粒子物理和工程设计等领域进行进一步的研究和开发，以克服这些瓶颈并实现可持续的聚变能生产。
-&lt;/think&gt;
-缪子催化聚变（Muon-Catalyzed Fusion, μCF）的基本原理涉及利用缪子作为催化剂来促进聚变反应，从而在较低温度下实现核聚变。以下是详细分析：
+          <t>缪子催化聚变（Muon-Catalyzed Fusion, μCF）的基本原理涉及利用缪子作为催化剂来促进聚变反应，从而在较低温度下实现核聚变。以下是详细分析：
 ### 1. 核心结论
 缪子催化聚变（μCF）通过缪子替代氢原子中的电子，降低原子核之间的库仑势垒，从而在较低温度下实现核聚变。目前面临的主要瓶颈包括α粒子粘滞和缪子产生成本，但已有解决方案正在探索中。
 ### 2. 背景与概念
@@ -4961,7 +4284,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -4987,15 +4310,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>好，我现在要回答用户关于直接能量转换（DEC）技术在p-¹¹B和D-³He燃料中的重要性，以及相关的DEC方案、技术挑战和效率问题。首先，我需要明确DEC的基本概念和其在聚变能源中的作用。
-DEC的主要目的是将聚变反应产生的高能带电粒子直接转化为电能，这样可以避免传统的热力学循环效率损失。这对于p-¹¹B和D-³He燃料尤其重要，因为它们的聚变产物是带电粒子，而不像DT燃料那样产生中子。
-接下来，我需要列举几种可能的DEC方案。收集器-加速器系统是一个常见方案，利用静电场来加速和收集带电粒子。磁镜收集器也是一种方案，通过磁场来捕获粒子。另外，离子束直接转换和基于等离子体的转换方法也是值得考虑的。
-然后，我需要分析每种方案的技术挑战。例如，收集器-加速器系统需要精确的电势分布，否则可能导致粒子损失和效率低下。磁镜收集器则面临磁场精确控制的问题，以防止粒子逸出。离子束方法需要处理空间电荷效应，这可能限制电流密度，进而影响整体效率。
-接下来，关于效率，这些DEC系统理论上可以达到50%以上的效率，但实际中可能会因为各种损失而降低。例如，系统中的电阻损耗、粒子散射和未被收集的粒子都会影响实际效率。
-最后，我需要总结这些信息，强调DEC的重要性以及未来研究的方向。例如，实验验证、材料研究和系统集成都是未来需要重点关注的领域，以推动DEC技术的发展和应用。
-总结一下，回答的结构应该是先讲核心结论，然后逐步展开背景、原理、挑战、效率和未来方向。这样用户能够清晰地理解DEC在先进聚变燃料中的重要性及其相关技术的现状和挑战。
-&lt;/think&gt;
-### **核心结论**  
+          <t>### **核心结论**  
 直接能量转换（DEC）技术对p-¹¹B和D-³He等先进聚变燃料至关重要，因为它能够高效回收聚变反应中带电粒子的能量，避免传统热力学循环的效率损失，从而显著提高聚变装置的经济性和可行性。
 ---
 ### **背景与概念**  
@@ -5073,7 +4388,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -5099,17 +4414,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，我需要综合评估发展p-¹¹B等先进燃料聚变反应堆的长期前景，特别是从系统工程和经济性的角度出发。除了物理和技术挑战，还有哪些非技术性障碍呢？让我一步步梳理一下。
-首先，燃料供应方面。p-¹¹B，也就是硼-11，需要从自然界提取。自然界中硼主要以硼-10和硼-11的形式存在，大概比例是20%和80%。所以，要分离出高纯度的硼-11，需要高效的技术，而且成本可能会比较高。另外，硼资源的分布情况如何呢？主要集中在哪些国家？这会影响到供应链的安全和稳定性。如果依赖少数几个国家，可能会有供应风险，增加经济负担。
-接下来，技术成熟度和研发成本。托卡马克装置目前主要使用氘氚燃料，技术相对成熟，而转向p-¹¹B需要完全不同的技术路径。系统工程的复杂性很高，因为要确保燃料在高温等离子体中的稳定供应和高效反应。研发需要长期的投入，包括理论研究、实验验证和工程实施。这些都需要大量的资金支持，而且研发周期可能很长，存在技术和经济上的双重风险。
-政策和国际协作也是关键因素。聚变能的发展需要各国政府的支持和协作，特别是在研发投入和监管框架方面。国际热核聚变实验堆（ITER）就是一个国际合作的例子，但p-¹¹B技术可能需要更紧密的合作，尤其是在资源分配和知识共享方面。政策支持不足可能会影响项目的推进速度和成功可能性。
-公众接受度和社会因素同样不容忽视。聚变能虽然被认为是清洁和安全的能源，但公众对聚变技术的了解可能有限。历史上，核电项目常常面临公众反对，主要是因为对安全性的担忧和对放射性废物处理的不信任。如果公众不接受，可能会影响项目的实施，甚至导致政策上的阻力。
-经济性和成本效益分析是决定项目可行性的重要因素。虽然p-¹¹B燃料的经济性可能在长期具有优势，比如资源丰富、无碳排放，但在初期阶段，建设和运营成本可能会非常高昂。此外，还需要评估其与其他清洁能源技术（如风能、太阳能）相比的竞争力。如果成本过高，可能会限制其市场竞争力，影响长期的商业化前景。
-国际合作与竞争也是一个重要方面。聚变能的发展需要全球范围内的合作，特别是在资源和技术方面。然而，不同国家在研发投入和优先级上可能存在差异，这可能影响项目的整体进度。此外，技术的商业化过程中，可能会面临国际市场的竞争，如何在全球市场中占据优势位置，是需要考虑的问题。
-最后，环境和安全评估。聚变反应堆的设计必须确保安全性，防止事故的发生，并且处理好废物问题。公众对聚变能的信任建立在长期的安全运营记录上。此外，环境保护的要求也在不断提高，聚变能的环境友好性需要得到充分验证，以满足未来的法规要求。
-综上所述，发展p-¹¹B等先进燃料聚变反应堆不仅需要克服技术上的挑战，还需要在燃料供应链、政策支持、公众接受度、经济性和国际合作等多个非技术领域进行深入的评估和规划。这些因素相互交织，将共同决定项目的长期前景。
-&lt;/think&gt;
-从系统工程和经济性的角度综合评估，发展p-¹¹B等先进燃料聚变反应堆的长期前景面临着多方面的挑战和机遇。以下是对这些挑战和机遇的详细分析：
+          <t>从系统工程和经济性的角度综合评估，发展p-¹¹B等先进燃料聚变反应堆的长期前景面临着多方面的挑战和机遇。以下是对这些挑战和机遇的详细分析：
 1. **燃料供应链与经济性**
    - **背景**：p-¹¹B燃料需要从自然界中的硼资源中提取，其丰度较低（约占80%），需要进行复杂的分离和提纯过程。这将直接影响燃料的成本和供应链的稳定性。
    - **挑战**：分离高纯度的p-¹¹B需要高效的分离技术，可能带来较高的初始投资和持续的运营成本。此外，硼资源的地理分布可能导致供应链的集中化，增加供应风险。
@@ -5200,7 +4505,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -5226,17 +4531,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>好吧，我现在需要详细解释理想磁流体力学（MHD）的基本方程组，以及如何利用能量原理分析等离子体的MHD不稳定性。这对我来说有点挑战，但我会尽力一步步理清楚。
-首先，理想MHD方程组包括哪几个方程呢？我记得应该有三个主要方程：质量守恒、动量守恒和能量守恒，此外还有描述磁场的方程，比如Faraday定律和磁高斯定理。那我应该先逐一列举这些方程，并写出它们的数学表达式，同时解释每个方程的物理意义。
-接下来，理想MHD的核心物理假设有哪些呢？我记得包括磁冻结定理，这意味着等离子体中的磁场与流体运动紧密耦合，不会出现滑移。此外，还有忽略粘性、电阻、热传导等效应，因为理想情况下这些效应可以忽略不计，这样方程组会更简化。
-然后，如何利用能量原理分析MHD不稳定性？这可能涉及到分析系统的自由能，当系统处于某种状态时，如果有扰动会导致自由能降低，那么这种状态就是不稳定的。我记得这涉及到考虑扰动下的能量变化，可能需要用一些数学工具，比如变分法或波动方程的求解。
-在具体操作中，可能需要写出扰动后的MHD方程，线性化之后进行分析，然后通过求解本征值问题来判断系统的稳定性。稳定性和能量之间的关系，比如如果系统的总能量（比如磁场能）随着扰动而降低，那么系统就会趋向于这种扰动，导致不稳定性。
-可能需要举一些例子，比如 tearing 模或者 sausage 模，这些是常见的MHD不稳定性，用能量原理分析它们的触发条件和成长机制。同时，还要讨论这些分析对实际聚变装置设计的意义，比如如何通过改变磁场配置、等离子体参数来抑制这些不稳定性。
-在思考过程中，我可能会有些不确定的地方，比如磁高斯定理的具体表达，或者能量原理的具体应用步骤。这时候，我需要回忆课本或者参考文献中的相关内容，确保自己对这些概念的理解是正确的。如果有遗漏，可能需要补充更多的细节，比如在动量方程中包括磁场力项，或者在能量方程中考虑磁场的做功。
-此外，如何连接理论与实际应用也是一个关键点。比如，理解MHD不稳定性对托卡马克等装置的影响，如何通过控制等离子体参数来优化装置的稳定性，这些都是需要思考的方面。
-总的来说，我需要系统地梳理理想MHD方程组，理解其基本假设，然后深入分析能量原理在稳定性分析中的应用，结合实际例子和工程意义，确保自己的理解全面而准确。
-&lt;/think&gt;
-### 理想磁流体力学（MHD）的基本方程组及核心假设
+          <t>### 理想磁流体力学（MHD）的基本方程组及核心假设
 #### 方程组
 1. **连续性方程**（质量守恒）：
    描述等离子体密度随时间和空间的变化，确保质量守恒。
@@ -5304,7 +4599,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -5330,18 +4625,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>嗯，我现在需要解释Grad-Shafranov方程，它是托卡马克等离子体平衡的核心方程。首先，我得回忆一下这个方程的背景和推导过程。Grad-Shafranov方程是在托卡马克这种磁约束装置中，描述等离子体在稳态下的平衡状态的。它考虑了等离子体的电流分布、压强分布以及外部磁场的影响。
-我应该从等离子体的基本动力学开始，考虑磁场对等离子体的约束。托卡马克使用强磁场来约束高温等离子体，使得离子和电子沿着磁场线运动。等离子体内部的电流会产生自己的磁场，与外部线圈产生的磁场相互作用，从而达到平衡。
-接下来，我需要推导这个方程。首先，考虑到等离子体处于平衡状态，所有力必须平衡，包括电磁力和压强梯度力。等离子体的动量守恒方程应该满足，其中洛伦兹力平衡压强梯度。这可能涉及到磁流函数的引入，因为磁场的结构可以用流函数来描述。
-磁流函数ψ是一个标量函数，其梯度给出了磁场的环向分量，而磁场的轴向分量则由ψ在某个截面上的值决定。引入ψ后，方程可以简化为关于ψ的方程，这样问题就转化为求解一个椭圆型的偏微分方程。
-在推导过程中，我需要假设一些条件，比如稳态、无粘性、忽略重力等。这些假设可以帮助简化方程，使其更容易求解。同时，还需要考虑到等离子体的电流分布，这通常用电流密度j来表示，而j与ψ有关，因为电流是由等离子体的运动产生的。
-此外，方程的右边涉及到等离子体的压强分布，具体来说是等离子体的总压强，包括电子和离子的压强。压强梯度驱动电流，而电流又进一步影响磁场结构。因此，方程的右边必须包含压强梯度的信息。
-然后，外部磁场线圈的配置也会影响方程的解。外部线圈产生的磁场可以增强或改变等离子体的约束性能。这些外部磁场的影响需要通过边界条件来考虑，即在等离子体与外部磁场的交界处，磁场必须连续，或者满足特定的边界条件。
-求解Grad-Shafranov方程通常需要数值方法，比如有限元或有限差分法，因为方程的非线性和复杂的边界条件很难用解析方法解决。在工程应用中，还需要考虑等离子体参数的变化，如密度、温度、电流密度等，这些参数会随着等离子体状态的变化而变化，从而影响磁场结构。
-最后，我需要讨论该方程的求解对托卡马克设计和运行的影响。通过求解Grad-Shafranov方程，可以优化等离子体的形状，调整外部磁场线圈的配置，以获得最佳的约束性能和稳定的运行状态。这对方程的设计和实验诊断都有重要的指导意义。
-总结一下，Grad-Shafranov方程描述了托卡马克等离子体的平衡状态，其求解依赖于等离子体内部的电流和压强分布，以及外部磁场的配置。理解这个方程对于设计和优化托卡马克装置至关重要。
-&lt;/think&gt;
-### 核心结论
+          <t>### 核心结论
 Grad-Shafranov方程是托卡马克等离子体平衡的核心方程，描述了等离子体在强磁场约束下的平衡状态，其求解依赖于等离子体的电流分布、压强分布以及外部磁场线圈的配置。
 ---
 ### 背景与概念
@@ -5408,7 +4692,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -5434,16 +4718,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>嗯，我现在需要比较托卡马克和仿星器在等离子体平衡实现方式上的主要异同，并且解释为什么仿星器的三维复杂磁场构型能够消除对大等离子体电流的需求，这对稳定性有什么潜在优势。
-首先，我得回顾一下托卡马克和仿星器的基本结构和工作原理。托卡马克是一个环形的磁约束装置，主要依靠强磁场来约束高温等离子体。而仿星器则是一个更复杂的结构，通常也是环形，但其磁场是由多个线圈产生的，形成一个三维的磁笼。
-等离子体的平衡在托卡马克中，主要是通过环向磁场和纵向磁场的相互作用，特别是在等离子体中心产生一个强大的纵向磁场。这种配置会导致等离子体中产生一个环形电流，这个电流对维持等离子体的平衡至关重要。而仿星器则不同，它利用外部线圈产生的三维磁场来约束等离子体，这样就不需要内部的环形电流，从而减少了对大电流的需求。
-接下来，我需要比较这两者在实现等离子体平衡上的相同点和不同点。相同之处可能包括两者都使用外部磁线圈来产生约束磁场，都试图保持等离子体的稳定，防止其接触器壁。不同点则在于托卡马克依赖于内部的等离子体电流，而仿星器则通过复杂的外部磁场结构来实现。
-关于仿星器如何消除对大等离子体电流的需求，我想这主要是因为仿星器的三维磁场结构能够更有效地约束等离子体，不需要依靠内部的电流来维持平衡。这可能意味着仿星器在某些方面更稳定，因为内部的大电流常常会导致等离子体的不稳定性，比如磁流体动力学（MHD）不稳定性。
-稳定性方面，仿星器可能具有更好的控制能力，因为它们可以设计出各种三维磁场形状，以优化等离子体的约束条件。这可能使得仿星器在面对扰动时更具恢复能力，从而提高整体运行的稳定性。
-不过，我也要考虑到仿星器设计和运行的复杂性，三维磁场的控制和维护可能比托卡马克更加困难，这也可能导致其他类型的不稳定性。但总体来说，仿星器在消除对大电流的需求方面确实有其优势，这可能带来更好的稳定性和更长的运行时间。
-总结一下，托卡马克和仿星器在平衡实现上的主要异同在于磁场结构和电流依赖性，而仿星器的三维磁场构型通过减少对大电流的需求，可能带来了更好的稳定性。
-&lt;/think&gt;
-托卡马克和仿星器在等离子体平衡实现方式上的主要异同点如下：
+          <t>托卡马克和仿星器在等离子体平衡实现方式上的主要异同点如下：
 ### 相同点
 1. **磁约束原理**：两者均利用强磁场来约束高温等离子体。
 2. **外部磁场源**：都依赖外部线圈产生的磁场来维持等离子体的平衡。
@@ -5465,7 +4740,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -5491,15 +4766,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于理想MHD中的主要不稳定性模式，扭曲模和气球模，它们的驱动机制以及对聚变等离子体的约束影响。首先，我得回忆一下MHD的基本概念，理想MHD是研究等离子体在电磁力作用下的行为，忽略电阻和磁场重连接。
-扭曲模，我记得它发生在纵向磁场中，与磁绳结构有关。当等离子体环状分布时，由于压力梯度和磁力的平衡被打破，可能会发生扭曲不稳定性。这种不稳定性会导致等离子体形状改变，可能破坏约束，影响聚变反应的稳定进行。
-气球模呢，这个名字让我联想到气球膨胀。它涉及到等离子体的局部区域因压力梯度或电流梯度而膨胀，形成类似气球的结构。驱动这种不稳定性的因素可能包括纵场梯度或垂直于磁场的电流分布。气球模会导致磁面的相互交叉，从而降低约束效果，增加逃逸损失。
-接下来，驱动机制方面，扭曲模主要由纵磁场和压力梯度的不平衡引起。当压力梯度过大，超过磁力的支撑时，系统就会变得不稳定。而气球模则涉及到纵向和横向的电流梯度，特别是当电流密度变化较大时，容易引发不稳定性。
-对约束的影响方面，这两种不稳定性都会导致等离子体形状的改变，破坏原来的约束条件。比如，扭曲模可能导致等离子体的纵截面扭曲，影响整体的热传导和粒子运输。而气球模则会使得磁面结构变得复杂，磁岛形成，进而增加粒子和能量的损失，降低聚变装置的效率。
-在工程设计中，为了抑制这些不稳定性，通常会采用优化磁 confinement 场结构，比如使用磁场 shaping，调整纵场和环流的分布，来平衡压力和电流梯度。此外，湍流耗散和电阻效应也可以通过增加加热功率或调整等离子体参数来改善，但这些都是权衡取舍的过程，需要综合考虑。
-总的来说，理解这些不稳定性模式的机制和影响，对于设计高效稳定的聚变装置至关重要。通过合理的磁 confinement 设计和参数控制，可以有效抑制这些不稳定性，提高聚变反应的效率和可持续性。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 理想磁流体力学（MHD）中的主要不稳定性模式包括扭曲模（Kink modes）和气球模（Ballooning modes）。扭曲模主要由压力梯度与纵向磁场的不平衡驱动，而气球模则由纵向磁场梯度和电流梯度共同驱动。这些不稳定性会破坏等离子体的磁约束，导致粒子和能量的逃逸，从而影响聚变装置的性能。
 ---
 ### 背景与概念  
@@ -5560,7 +4827,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -5586,36 +4853,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>好，我现在要解决这个问题，定义等离子体的beta值β和环向beta值βt，然后估算Troyon极限对应的βN值，最后计算最大允许的平均压强。
-首先，我需要明确beta值的定义。β是等离子体压力与磁压力的比值，公式是β= (8πP)/B_t²。其中P是等离子体的平均压强，B_t是环向磁场的磁感应强度。环向beta值βt，同样是指环向磁场方向的压力比，βt=(8πP_t)/B_t²，其中P_t是环向压力。
-接下来，题目给出了托卡马克的参数：大环径R0=3米，小半径a=1米，环向磁场Bt=5特斯拉，等离子体电流Ip=5百万安培。我要用这些参数来估算Troyon极限对应的βN值，其中Troyon系数g≈2.8。
-首先，计算等离子体的电流Ip与环向磁场Bt的关系。托卡马克中的环向磁场由等离子体电流和外加电流共同产生，这里假设等离子体电流占主导，或者已知Bt与Ip的关系。一般来说，Bt可以表示为Bt = μ0 * (Ip * R0²)/(2a²)，其中μ0是真空磁导率，约为4π×10^-7 H/m。代入数值：R0=3m，a=1m，Ip=5MA=5×10^6 A。计算Bt：
-Bt = μ0 * (5×10^6 A * (3)^2) / (2*(1)^2) = 4π×10^-7 * (5×10^6 *9)/(2) = 4π×10^-7 * (4.5×10^7) ≈ 4π×(4.5×10^0) ≈ 56.55特斯拉。但题目给出Bt=5T，这明显不符，说明我可能误解了问题。或许Bt已经给出，不需要计算。因此，我应该直接使用题目提供的Bt=5T进行计算，而Ip=5MA用于其他计算。
-接下来，计算βN值。Troyon极限给出βN的上限，βN = g * (R0/a) * (Bt/(8πP))。或者，可能βN = g * (R0/a) * (Bt/Bt0)，这里可能需要重新审视公式。实际上，βN的定义通常与等离子体的电流密度和磁场分布有关，可能涉及到安全因数q和压力梯度。但为了简化，这里可能直接使用公式βN = g * (R0/a) * (Bt/Bt0)，其中Bt0是中心的环向磁场。
-不过，更准确的方法可能是使用βN = (Bt * R0)/(μ0 * Ip)。但不确定是否正确。或者，考虑βN = (Bt * R0)/(μ0 * Ip * a)，这需要重新推导。可能我需要更准确地回顾Troyon极限的公式。
-Troyon极限指出，等离子体的压力梯度受到磁流体力学不稳定的限制，当βN超过某个临界值时，等离子体将发生失稳。βN的定义通常为：βN = (Bt * R0)/(μ0 * Ip * a) * g，其中g是系数，约为2.8。代入数据：
-βN = (5 T * 3 m) / (4π×10^-7 H/m * 5×10^6 A * 1 m) * 2.8 = (15) / (4π×10^-7 *5×10^6) *2.8。
-计算分母：4π×10^-7 ≈ 1.2566×10^-6；乘以5×10^6得到≈6.283。所以分母≈6.283。因此，βN ≈ 15 / 6.283 *2.8 ≈ 2.39*2.8≈6.70。
-这似乎过高，可能哪里计算错误。或者，正确的公式可能为βN = (g * R0 * Bt) / (2μ0 * Ip * a)。重新计算：
-βN = (2.8 *3m *5T) / (2*4π×10^-7 H/m *5×10^6 A *1m) = (42) / (2*4π×10^-7 *5×10^6) =42/(8π×10^-7 *5×10^6)=42/(4π×10^-6 *5)=42/(20π×10^-6)=42/(6.283×10^-5)=约6.69×10^5？这显然不对，可能我弄错了公式。
-或许正确的公式是βN = g * (R0/a) * (Bt)/(μ0 * Ip). 代入：
-R0/a=3/1=3；Bt=5T；μ0=4π×10^-7；Ip=5×10^6 A。
-βN=2.8 *3*(5)/(4π×10^-7 *5×10^6)=2.8*3*5/(4π×5×10^-1)=2.8*3/(4π×0.1)=2.8*3/(0.4π)=8.4/(1.2566)≈6.685。
-所以，βN≈6.685，约等于6.69。
-然后，根据Troyon极限，βN_max≈2.8*(R0/a)=2.8*3=8.4？或者，我可能混淆了公式，因为之前的计算得到约6.69。可能正确的公式是βN = g*(R0/a)*(Bt/(Bt0))，其中Bt0是中心磁场，或者直接用βN= g*(R0/a)*(Bt/(μ0*Ip))。
-另一个可能的方法是使用βN = (Bt * R0)/(μ0 * Ip * a) * g。代入：
-Bt=5T；R0=3m；μ0=4π×10^-7；Ip=5×10^6 A；a=1m；g=2.8。
-βN=5*3/(4π×10^-7 *5×10^6 *1) *2.8=15/(20π×10^-1) *2.8=15/(6.283) *2.8≈2.39*2.8≈6.70。
-这似乎合理，所以βN≈6.7。
-然后，计算最大允许的平均压强P。根据β= (8πP)/Bt²，而βN=β*(R0/a)*q，其中q是安全因数。但可能更直接的是，β=βN/(g*(R0/a))。所以：
-β=βN/(g*(R0/a))=6.7/(2.8*3)=6.7/8.4≈0.797。
-然后，平均压强P=β*Bt²/(8π)=0.797*(5)^2/(8π)=0.797*25/(25.1327)=约0.797*25/25.1327≈0.797*(0.995)=≈0.793 MPa，即约793 kPa。
-这可能偏低，因为实际托卡马克的压强通常更高，可能在数兆帕范围内。可能我在β与βN的关系上有误，或者公式需要重新审视。
-另一种方法是，利用βN=β*(R0/a)*q，其中q是安全因数，通常接近或超过2，以确保稳定。如果忽略q，或者设q=1，则β=βN/(R0/a)=6.7/3≈2.23。然后，P=β*Bt²/(8π)=2.23*25/(25.1327)=≈2.23*25/25.1327≈≈2.23*(0.995)=≈2.22 MPa，即约2.22 MPa。
-这更合理，因为压强在数兆帕范围内。因此，最大允许的平均压强约为2.2 MPa。
-总结，计算步骤可能存在一些混淆，但最终得出βN≈6.7，平均压强≈2.2 MPa。
-&lt;/think&gt;
-**答案：**
+          <t>**答案：**
 1. **核心结论**  
    托卡马克等离子体的Troyon极限对应的βN值约为6.7，最大允许的平均压强约为2.22 MPa。
 2. **背景与概念**  
@@ -5638,7 +4876,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -5664,16 +4902,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>嗯，我现在需要回答关于电阻MHD中的撕裂模（Tearing Modes）的问题。问题包括物理机制、磁岛形成过程、对等离子体约束的破坏，以及Δ'参数的意义。
-首先，我要理解撕裂模的基本概念。撕裂模是一种磁流体力学不稳定性，常见于托卡马克装置中。它涉及到等离子体中磁力线的断裂和重新连接，导致磁岛的形成。
-接下来，物理机制方面。撕裂模的发生与电流分布和磁场梯度有关。当等离子体中的电流分布不均匀时，局部区域的磁力线会被撕裂，形成新的磁通量结构。这个过程需要考虑电阻率和磁场的相互作用。
-然后，磁岛的形成过程。撕裂模的初期是一个微小扰动，导致磁力线开始断裂。随着不稳定性的发展，磁力线重新连接形成闭合的磁岛。这些磁岛会合并和生长，最终导致磁通量的交换和等离子体的输运增加。
-对等离子体约束的破坏作用，主要是因为磁岛使得等离子体沿着磁力线方向扩散，导致能量损失和约束性能下降。这会影响托卡马克装置的高效运行。
-关于Δ'参数，它是一个无量纲参数，用于判断撕裂模的稳定性。Δ'主要考虑了磁压力、电流梯度和磁场的配置。当Δ'小于某个临界值时，撕裂模趋于不稳定，反之则稳定。Δ'帮助设计者优化等离子体参数，避免撕裂模的发生。
-在总结过程中，我需要确保各部分内容清晰，逻辑连贯。可能还需要查阅一些文献来确认具体参数的定义和影响因素。此外，考虑到用户希望结构清晰，可能会使用列表或分点来组织内容。
-最后，检查是否有遗漏的关键点，比如撕裂模与其他MHD不稳定的区别，以及Δ'在实验中的实际应用情况。确保回答全面且准确，符合用户的要求。
-&lt;/think&gt;
-### **核心结论**  
+          <t>### **核心结论**  
 撕裂模（Tearing Modes）是电阻磁流体力学（MHD）中的一种不稳定性，其物理机制涉及等离子体中电流和磁场的重新分布，导致磁岛的形成，从而破坏等离子体的约束性能。Δ'参数是判断撕裂模稳定性的关键指标，其值小于临界值时撕裂模不稳。
 ---
 ### **背景与概念**  
@@ -5747,7 +4976,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -5773,15 +5002,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>好吧，我现在需要详细讨论仿星器在MHD稳定性分析中的特殊挑战，特别是三维效应和缺乏连续对称性。然后还要简述VMEC和CAS3D等计算程序在这方面的应用。
-首先，MHD稳定性在聚变装置中非常重要，因为它直接关系到等离子体的约束和装置的运行效率。对于托卡马克来说，由于其环形对称结构，分析相对简单一些，但仿星器因为其复杂的三维磁场结构，带来了更多的挑战。
-三维效应方面，仿星器的磁场不是简单对称的，导致等离子体的运动也变得复杂。这可能引入更多不稳定的模式，比如三维的磁流涡旋或者漂移波不稳定性。同时，缺乏连续对称性，比如仿星器通常不具有像托卡马克那样的高对称性（如环向对称性），这意味着传统的对称假设可能不再适用，传统的分析方法可能不够准确。
-接下来，计算程序方面，VMEC和CAS3D都是重要的工具。VMEC主要用于求解等离子体的平衡状态，也就是确定在给定的磁场下，等离子体如何分布。它通过计算等离子体的压强和电流分布，得到稳定状态下的磁场结构。这对于仿星器的设计和优化非常重要，因为它可以预测不同的磁场配置对等离子体行为的影响。
-而CAS3D则用于稳定性分析，即确定在给定的平衡状态下，等离子体是否会变得不稳定。它通过求解线性化的MHD方程，寻找可能的不稳定性模式及其增长速率。这有助于研究人员在设计阶段就预测和规避潜在的不稳定因素，从而提高装置的稳定性和运行效率。
-不过，使用这些程序也面临一些挑战。首先是计算资源的需求，三维问题通常需要大量的计算资源，这在实际应用中可能是一个瓶颈。其次是模型的复杂性，如何在保持计算可行的同时，又能准确捕捉到所有重要的物理效应，这是一个需要权衡的问题。此外，还需要可靠的诊断数据和实验结果来验证计算模型的准确性，这在实验资源有限的情况下也是一个挑战。
-总的来说，仿星器的MHD稳定性分析需要结合理论、数值模拟和实验，而VMEC和CAS3D等程序提供了强大的工具来支持这一过程。但要充分理解和利用这些工具，还需要进一步的研究和开发，特别是在提高计算效率、完善模型和验证方法方面。
-&lt;/think&gt;
-### 仿星器MHD稳定性分析的特殊挑战
+          <t>### 仿星器MHD稳定性分析的特殊挑战
 #### 1. 核心结论
 仿星器的MHD稳定性分析面临三维效应和缺乏连续对称性的特殊挑战，这些因素使得传统的托卡马克分析方法失效，需要专门的数值方法和工具。
 #### 2. 背景与概念
@@ -5826,7 +5047,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -5852,19 +5073,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，这个问题看起来有点复杂，但我会慢慢理清楚思路。首先，问题是在托卡马克的先进运行模式中，如何通过优化电流密度剖面和压强剖面来提高MHD稳定性极限，特别是避免或抑制新经典撕裂模（NTMs）和电阻壁模（RWMs）。作为一个刚开始学习聚变物理的学生，我得先理解什么是MHD稳定性、NTMs和RWMs，以及电流密度剖面和压强剖面是如何影响它们的。
-首先，MHD稳定性是聚变等离子体中的一个重要问题。当等离子体在强磁场中运行时，任何微小的扰动都可能导致不稳定性，破坏等离子体的约束。这可能降低聚变反应的效率，甚至导致等离子体崩溃。因此，确保等离子体的稳定性对于托卡马克的高效运行至关重要。
-接下来，NTMs（新经典撕裂模）和RWMs（电阻壁模）是两种常见的MHD不稳定性。NTMs通常出现在高密度、高压力梯度的等离子体中，它们会撕裂磁面，导致等离子体的突然损失。RWMs则与托卡马克的外部结构，特别是真空室壁有关，当等离子体与壁之间的电阻发生变化时，可能会引发RWMs，导致等离子体的剧烈扰动。
-现在，问题是如何通过优化电流密度剖面和压强剖面来抑制这两种不稳定性。我需要先了解电流密度剖面和压强剖面在托卡马克中的作用。
-电流密度剖面指的是等离子体中电流密度的空间分布。托卡马克中的电流通常是通过外部线圈产生的，但也可以通过等离子体内部的电流来维持。电流密度的分布会影响磁场的结构和等离子体的稳定性。一般来说，较大的电流密度梯度会增加等离子体的不稳定性风险，因为它们会导致更强的磁场变化，从而更容易引发MHD不稳定性。
-压强剖面指的是等离子体中压强的空间分布。较高的压强梯度会增加等离子体的不稳定性，因为它们会导致等离子体的运动和扰动。优化压强剖面，使其分布更均匀，可能会减少这种风险。
-为了抑制NTMs，我需要考虑如何调整电流密度和压强剖面。研究表明，避免电流密度的最大值出现在磁面的外边界可以减少NTMs的发生。此外，增加磁场的旋转可以抑制撕裂模的发展，因为旋转会使得撕裂模的扰动波在传播过程中受到抑制。
-对于RWMs，优化压强梯度是关键。较大的压强梯度会增加RWMs的不稳定性，因此需要平缓压强梯度，避免过大的压力变化。此外，确保等离子体的形状对称，减少外部结构的影响，也可以降低RWMs的风险。
-在优化过程中，还需要考虑其他因素，比如等离子体的加热方式、外部磁场的配置以及诊断手段。例如，使用射频加热来优化电流密度剖面，或者通过调整线圈的位置来控制磁场的分布。
-总的来说，优化电流密度和压强剖面是一个多方面的过程，需要综合考虑各种因素，以达到提高MHD稳定性极限的目的。虽然这听起来有点复杂，但通过逐步分析和实验验证，应该能够找到有效的解决方案。
-接下来，我需要进一步查阅相关文献和资料，以确保我的理解是正确的，并且找到具体的优化策略和方法。此外，了解现有的实验结果和模拟数据，可以帮助我更好地理解这些优化措施的实际效果。
-&lt;/think&gt;
-在托卡马克先进运行模式中，优化电流密度剖面和压强剖面以提高MHD稳定性极限，特别是抑制新经典撕裂模（NTMs）和电阻壁模（RWMs），可以通过以下步骤实现：
+          <t>在托卡马克先进运行模式中，优化电流密度剖面和压强剖面以提高MHD稳定性极限，特别是抑制新经典撕裂模（NTMs）和电阻壁模（RWMs），可以通过以下步骤实现：
 ### 1. 理解电流密度剖面与MHD稳定性
 - **电流密度剖面**：描述了等离子体中电流密度的空间分布。较高的电流密度梯度可能引发MHD不稳定性，如NTMs和RWMs。
 - **影响**：避免电流密度的最大值出现在磁面的外边界，可以减少NTMs的发生。同时，增加磁场的旋转有助于抑制撕裂模的发展。
@@ -5888,7 +5097,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -5914,17 +5123,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>嗯，我现在得解释一下Mercier判据和气球模判据在仿星器的局部稳定性评估中的应用，以及为什么即使这些判据满足了，还是需要做全局的稳定性分析。这个问题对我来说有点挑战，但我先从基础开始思考。
-首先，我需要回顾一下仿星器是什么，它和托卡马克有什么不同。仿星器是一种利用扭曲磁线来限制等离子体的聚变装置，与托卡马克相比，它不需要强大的外部磁场，也不需要环向电流，因此在运行方面可能更灵活，但控制等离子体的稳定性可能更复杂。
-接下来，Mercier判据。我记得这在托卡马克中被用来判断压致 instability，也就是当等离子体压力梯度太大时，可能导致不稳定。在托卡马克中，圆柱形或环形的几何结构下，这种判据适用。那在仿星器中，Mercier判据是不是也被用来评估局部稳定性呢？仿星器的磁场结构比较复杂，可能有不同的分支，所以每个局部区域的稳定性都需要评估。
-然后是气球模判据。气球模指的是等离子体中的一种模，当某些条件满足时，等离子体开始膨胀，像气球一样，导致不稳定性。气球模判据通常和磁场强度与等离子体压力的梯度有关，尤其在环向和垂直方向上的压力梯度。在仿星器中，这种判据是不是用来确保在每一个局部区域，压力梯度不会太大，从而避免气球模不稳定性？
-现在，为什么在仿星器中，即使这些局部判据满足了，仍需进行全局的稳定性分析？也许因为仿星器的磁场结构是非轴对称的，可能有更复杂的不稳定性模式，而局部判据只能评估一部分情况。例如，可能有全局性的模，如kink模或者其他类型的不稳定性，这些不会被局部判据捕捉到。此外，仿星器中的不稳定性可能跨越多个局部区域，形成整体性的问题，因此必须考虑整个装置的稳定性。
-我还需要思考一下每个判据的理论基础和适用范围。Mercier判据通常是在等离子体参数空间的某种极限下推导出来的，可能适用于特定的几何形状或参数范围。气球模判据则可能依赖于不同方向的梯度平衡。而仿星器的复杂结构可能意味着这些判据的假设在某些情况下并不完全成立，或者有新的不稳定性模式出现。
-另外，仿星器的运行参数可能与托卡马克有很大不同，比如更低的磁通量或更高的温度梯度，这些都会影响判据的应用。即使局部稳定性得到了满足，全局的相互作用和不同区域的相互影响可能导致新的不稳定性，这需要更全面的分析。
-还有，工程上仿星器的设计可能涉及多个模块或区域，每个区域的稳定性都可能影响整体性能。因此，除了局部评估，还需要进行整体的稳定性分析，确保整个装置在各种运行条件下都保持稳定。
-最后，我需要组织一下思路，将这些点整合成一个清晰的解释，说明每个判据的应用和局限性，以及为什么全局分析是必要的。
-&lt;/think&gt;
-### Mercier判据和气球模判据在仿星器局部稳定性评估中的应用
+          <t>### Mercier判据和气球模判据在仿星器局部稳定性评估中的应用
 #### 1. 核心结论
 在仿星器的等离子体约束系统中，Mercier判据主要用于评估压致不稳定性，而气球模判据则用于判断与压力梯度相关的气球模不稳定性。然而，即使这些局部判据满足，仍需进行全局稳定性分析以确保整个系统稳定。
 #### 2. 背景与概念
@@ -5953,7 +5152,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -5979,16 +5178,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，这个问题是关于自由边界和固定边界MHD不稳定性的区别，以及真空区和理想导电壁对外部扭曲模稳定性的影响，还有壁稳定效应。我得先理清楚这些概念。
-首先，MHD不稳定性主要分为两种：自由边界和固定边界。自由边界意味着等离子体与外部是直接接触的，没有固体壁约束。而固定边界则有固体壁，限制等离子体的运动。
-那它们的区别是什么呢？自由边界因为没有壁，等离子体可以自由膨胀，这可能导致不稳定性更容易发生，比如外部扭曲模。而固定边界因为有壁的存在，可能会对不稳定性产生抑制，这就是所谓的壁稳定效应。
-接下来，真空区和理想导电壁如何影响外部扭曲模的稳定性？外部扭曲模通常发生在等离子体外部区域，影响边界附近的磁场结构。在自由边界情况下，等离子体边界可以移动，这可能会加剧不稳定性的发生。而在固定边界，理想导电壁的存在会使等离子体的运动受到限制，这可能抑制外部扭曲模的发展。
-壁稳定效应具体是怎么回事？理想导电壁能够反射某些波动，使得磁场在边界附近被约束，这可能改变等离子体的运动模式，从而提高稳定性。特别是在低模式数的情况下，壁的影响更为显著，可能稳定一些不稳定的模式。
-我可能需要回顾一下外部扭曲模的条件，比如玛雅不稳定性，看看壁的存在如何改变其发生的条件。比如，是否存在壁会改变磁压力的平衡，从而影响不稳定性的发展。
-另外，模式数也是一个关键因素，高模式数可能对壁的存在不太敏感，而低模式数则容易受壁的影响。这一点在分析中应该提到。
-总结一下，我需要明确区分自由边界和固定边界MHD不稳定性，解释真空区和壁对稳定性的影响，详细分析壁稳定效应的机理，并结合典型参数进行讨论。这样用户的问题才能得到全面而清晰的解答。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 自由边界和固定边界MHD不稳定性在不稳定性机理和稳定性条件上有显著区别。真空区和理想导电壁的存在会通过改变磁场拓扑和等离子体-壁耦合机制，显著影响外部扭曲模的稳定性，壁稳定效应能够抑制某些不稳定性的发展。
 ---
 ### 背景与概念  
@@ -6104,7 +5294,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -6130,18 +5320,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>好，我现在要详细阐述离子温度梯度（ITG）模的物理机制，并根据给定的密度梯度尺度长度Ln和离子温度梯度尺度长度LTi，推导ITG模的简化线性阈值条件，比如ηi=Ln/LTi&gt;ηicrit。同时，还要讨论这个阈值如何受到其他参数，如安全因子q和磁剪切s的影响。
-首先，ITG模是一种重要的磁流体力学不稳定性，主要发生在托卡马克等离子体中，特别是在高密度和中等温度的区域，例如阴极区。它会导致等离子体的输运，影响能量的约束效率。因此，了解ITG模的物理机制以及如何控制其发生，对于聚变装置的设计和运行至关重要。
-接下来，我需要回顾一下ITG模的线性稳定性分析。在磁流体力学中，不稳定性通常由波动的增长率决定。对于ITG模，增长率γ与各种参数相关，如梯度参数ηi=Ln/LTi，安全因子q，磁剪切s等。为了推导线性阈值条件，通常需要将γ=0的情况作为临界点，从而得到ηi的临界值ηicrit。
-根据Galeev和Furth的早期工作，ITG模的线性稳定性条件可以简化为ηi=Ln/LTi&gt;ηicrit。而ηicrit与q和s有关。具体来说，随着q的增加，ηicrit会增加，即需要更大的梯度才能触发不稳定性，这可能是因为更高的q导致了更稳定的磁场结构。而磁剪切s的影响可能更复杂，可能需要进一步的分析或文献回顾来确定。
-在推导过程中，我需要确保每一步的假设和近似都是合理的。例如，是否考虑了平行于磁场方向的运动，还是仅限于磁面内的情况。此外，还需要确定是否使用了特定的简化模型，如常规的ITG模型，还是考虑了漂移-波动的相互作用等。
-同时，考虑到安全因子q和磁剪切s对ITG模的稳定性的影响，这些参数的变化会如何调整ηicrit的值，从而影响ITG模的发生条件。例如，增加q可能会提高临界梯度，使得ITG模更难被触发，这对等离子体的稳定运行是有利的。
-在讨论参数影响时，可能还需要参考相关的实验结果或数值模拟，以验证理论推导的正确性。例如，实验中观察到的ITG模的发生条件是否与推导出的临界条件一致，或者是否存在偏差，这可能提示需要更精确的模型或考虑更多的物理效应。
-总的来说，推导ITG模的线性阈值条件涉及到对多种参数的依赖性分析，了解这些参数如何影响临界梯度，可以帮助优化聚变装置的设计，例如通过调整q和s来控制等离子体的稳定性，从而提高能量约束效率。
-此外，考虑到ITG模在不同边界条件和几何结构下的表现可能会有所不同，这可能需要进一步的研究来全面理解其物理机制。不过，从基本的线性稳定性分析出发，已经能够得到关于ITG模发生的初步条件，这对于指导实验和工程设计是非常有用的。
-最后，总结一下，ITG模的阈值条件ηi=Ln/LTi&gt;ηicrit，其中ηicrit依赖于q和s。理解这些参数的影响有助于优化聚变装置的参数设置，以减少ITG模引起的输运，从而提高能量的约束效率。
-&lt;/think&gt;
-### 离子温度梯度（ITG）模的物理机制与阈值条件分析
+          <t>### 离子温度梯度（ITG）模的物理机制与阈值条件分析
 #### 1. 核心结论
 离子温度梯度（ITG）模的线性阈值条件为 $\eta_i = \frac{L_{n}}{L_{T_i}} &gt; \eta_{i,crit}$，其中 $\eta_{i,crit}$ 受安全因子 $q$ 和磁剪切 $s$ 影响，增加 $q$ 会使 $\eta_{i,crit}$ 增大，从而抑制 ITG 不稳定性。
 #### 2. 背景与概念
@@ -6186,7 +5365,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -6212,47 +5391,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>好吧，我现在遇到了一个关于新经典撕裂模（NTM）的问题，我得仔细想想怎么解决它。首先，我需要理解什么是NTM，以及它在托卡马克等离子体中的作用。
-NTM，全称是新经典撕裂模，是一种不稳定性，会导致磁约束等离子体中的磁通量被撕裂，从而破坏等离子体的约束性能。这种撕裂模通常发生在中高剪切的区域，而不仅仅是低剪切区域，这与经典撕裂模不同。因此，NTM的触发条件和机制涉及到更多复杂的因素。
-接下来，问题提到了自举电流扰动和极化电流效应对NTM激发和增长的作用。我得回忆一下自举电流和极化电流的基本概念。
-自举电流（Bootstrap Current）是由于等离子体中的梯度，特别是离子温度梯度和密度梯度，驱动的电流。在托卡马克中，自举电流通常出现在高剪切区域，并且在高密度、高温度的情况下更为显著。这种电流扰动可能会影响磁通的分布，从而影响撕裂模的稳定性。
-极化电流（Polarization Current）则是指等离子体中的粒子在磁场梯度中运动时产生的电流。这种电流通常与位形变化有关，比如在撕裂模发生时，局部磁场结构的变化会引发极化电流，进而影响撕裂模的生长。
-现在，问题还提到广义卢瑟福方程在NTM分析中的应用。广义卢瑟福方程是一个用来分析磁流约束装置中磁通表面稳定性的基本方程。它描述了扰动增长的速率，考虑了电流密度和磁通量的分布。在分析NTM时，广义卢瑟福方程被用来计算扰动的生长率，从而判断撕裂模是否会发生。
-为了深入理解这些机制，我需要分步骤分析：
-1. **背景与概念**：
-   - 介绍NTM的基本概念，包括它在托卡马克等离子体中的触发条件和位置。
-   - 解释自举电流扰动和极化电流效应的定义及其在等离子体中的作用。
-   - 简述广义卢瑟福方程及其在磁通量表面稳定性分析中的应用。
-2. **激发和增长机制**：
-   - 阐述NTM的激发条件，如中高剪切区域中的温度和密度梯度。
-   - 分析自举电流扰动如何在高剪切区域驱动电流梯度，从而增加局部电流密度，导致撕裂模的不稳定性。
-   - 讨论极化电流效应如何在磁通量表面位移时响应，影响撕裂模的增长。
-3. **广义卢瑟福方程的应用**：
-   - 写出广义卢瑟福方程的数学表达式，定义各变量和符号。
-   - 详细推导方程的各个部分，包括电流密度、位移、剪切梯度等的影响。
-   - 说明方程中各项的物理意义，如自举电流项如何影响扰动的生长率。
-4. **自举电流扰动和极化电流效应对广义卢瑟福方程的影响**：
-   - 将自举电流扰动和极化电流效应引入广义卢瑟福方程，分析它们对扰动生长率的贡献。
-   - 讨论这些效应如何改变撕裂模的稳定性，例如增加或减少增长率。
-5. **定量分析与示例**：
-   - 选取典型参数，如剪切梯度、自举电流密度、极化电流密度等。
-   - 代入广义卢瑟福方程进行计算，得出扰动的生长率。
-   - 讨论计算结果，说明自举电流和极化电流效应对增长率的具体影响。
-6. **工程与实验意义**：
-   - 说明理解NTM激发和增长机制对托卡马克设计和运行控制的重要性。
-   - 讨论如何通过优化等离子体参数（如剪切梯度、密度和温度分布）来抑制NTM的发生。
-   - 提出可能的实验验证方法，以确认理论分析的准确性。
-7. **比较与拓展**：
-   - 比较NTM与其他撕裂模类型（如经典撕裂模）的不同之处，特别是在激发条件和机制上的差异。
-   - 讨论广义卢瑟福方程在不同模型或方案中的应用，分析其优缺点和适用范围。
-8. **要点总结**：
-   - 重申NTM的基本概念及其在托卡马克中的重要性。
-   - 强调自举电流扰动和极化电流效应对NTM增长的关键作用。
-   - 提出未来研究的方向，如更精确的参数化模型或实验验证计划。
-在整个思考过程中，我需要确保对每个概念都有清晰的理解，并且在分析时考虑到各物理量之间的相互作用。同时，我得确保引用的方程和计算步骤是正确的，避免因为疏忽导致错误的结论。此外，还需要结合实际的工程背景，讨论这些理论结果对实际聚变装置设计和运行的意义。
-最后，在组织答案时，我要按照给定的答题规范，分段落和步骤来解释，确保内容逻辑清晰，便于读者快速理解。特别是在数学推导部分，要详细列出每一步骤，并解释所做的假设和近似，以提高答案的严谨性和可信度。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 新经典撕裂模（NTM）的激发和增长由中高剪切区域的自举电流扰动和极化电流效应对磁通量表面的稳定性和电流密度分布的破坏驱动，广义卢瑟福方程是分析NTM的关键工具。
 ---
 ### 背景与概念  
@@ -6305,7 +5444,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -6331,18 +5470,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>好，我现在要回答关于边缘局域模（ELMs）的问题。首先，用户问的是ELMs是什么，主要类型有哪些，以及它们对等离子体约束和第一壁的影响。然后，还要讨论大型装置如ITER中用于控制或缓解ELMs的主要策略，比如RMP和颗粒注入。
-首先，我需要明确什么是ELMs。边缘局域模是托卡马克等离子体中的一种不稳定性现象，通常发生在高约束模式（H模）下。它们会导致边缘等离子体突然释放能量，影响到等离子体的约束性能，甚至对装置的第一壁造成损害。
-接下来，主要类型。Type-I是最常见的ELMs，能量释放剧烈，通常与等离子体边缘的不稳定性有关。Type-II则释放的能量较低，持续时间更长，通常与较低的剪切速率相关。还有Type-III，可能涉及更复杂的机制，但目前了解较少。
-然后，影响方面。ELMs会导致等离子体约束变差，能量突然释放到边缘，可能损坏第一壁材料。此外，反复的能量释放会增加装置部件的疲劳和侵蚀风险。
-关于控制策略，ITER可能会采用多种方法。例如，利用外部磁扰动（RMP）来抑制ELM的增长，或者通过注入颗粒（如氖、氩）来改变等离子体边缘的参数，从而缓解ELMs。此外，改变运行参数（如电流或压力）也可能有助于控制ELMs。
-在讨论这些策略时，我需要考虑每种方法的优缺点。比如，RMP可能会引入额外的磁干扰，影响等离子体的全局性能；颗粒注入则可能增加等离子体的污染风险。
-最后，总结部分要强调ELMs对聚变装置的重要性，控制策略的多样性和复杂性，以及未来研究的方向，如开发更有效的ELM控制方法，减少对装置的影响。
-整个回答需要按照用户的规范，分步骤进行，每部分都要有明确的小标题，使用清晰的结构，可能包括一些公式或示例数据，帮助读者理解。
-现在，我应该开始组织这些信息，确保每个部分都涵盖到用户的问题，并且符合写作要求。可能还需要引用一些典型参数，比如ELMs的能量释放范围，或者RMP的磁扰动强度，来支持我的观点。
-总之，我需要系统地梳理ELMs的基本概念、类型、影响，以及控制策略，并以清晰、有条理的方式呈现出来，确保用户能够全面理解相关内容。
-&lt;/think&gt;
-### 边缘局域模（ELMs）及其对等离子体约束和第一壁的影响
+          <t>### 边缘局域模（ELMs）及其对等离子体约束和第一壁的影响
 #### 1. 核心结论
 边缘局域模（ELMs）是托卡马克等离子体在高约束模式（H模）下的一种不稳定性现象，其能量释放会削弱等离子体约束并损害第一壁材料。主要类型包括Type-I和Type-II ELMs，其中Type-I是最强烈的。控制策略如外部磁扰动（RMP）和颗粒注入是缓解ELMs的主要方法。
 ---
@@ -6398,7 +5526,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -6424,18 +5552,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>嗯，我现在需要讨论锯齿不稳定性，也就是Sawteeth现象，包括它的物理过程、周期性崩溃和重联机制。然后，还要分析锯齿对等离子体芯部约束的影响，以及它与其他MHD不稳定性，比如NTM之间的关系。作为一个刚开始接触聚变等离子体物理的学生，我需要先了解Sawteeth的基本概念。
-首先，我记得在托卡马克装置中，等离子体会经历各种不稳定性，Sawteeth就是其中之一。Sawteeth通常表现为等离子体核心的温度和密度周期性下降，看起来像锯齿状的信号，所以得名。这种现象可能与磁重联有关，磁重联是磁场线断裂并重新连接的过程，会释放大量能量。
-接下来，我需要弄清楚Sawteeth的物理过程。根据之前的阅读，Sawteeth可能分为两种类型：类型I和类型II。类型I锯齿是由于边缘的磁扰动引起的，而类型II可能涉及到更复杂的机制。类型I锯齿通常会导致等离子体的突然崩溃，而类型II可能较为缓慢。
-然后，关于周期性崩溃，Sawteeth通常会有固定的周期，比如几秒到几十秒，这取决于托卡马克的具体参数，如电流、温度、密度等。崩溃时，核心的温度和密度会急剧下降，但随后又会逐渐恢复，直到下一次崩溃，形成周期性的锯齿状信号。
-在崩溃过程中，会发生磁重联。重联通常发生在等离子体的边缘，导致能量的快速释放和等离子体的重新配置。这种重联可能涉及到雪崩式的不稳定性，即多次重联事件迅速发生，导致整个核心区域的参数变化。
-那么，Sawteeth对等离子体芯部约束有什么影响呢？我知道约束的好坏直接影响到聚变反应的效率。Sawteeth会导致温度和密度的下降，这可能会降低聚变反应的速率。此外，频繁的崩溃可能增加等离子体的湍流，从而恶化约束。
-至于与其他MHD不稳定性如NTM的关系，我记得NTM是NeoclassicalTearingMode的缩写，是一种经典撕裂模的不稳定性，同样会导致等离子体的不稳定。Sawteeth和NTM都可能导致磁表面的破坏，从而影响约束性能。但它们的机制不同，Sawteeth更注重周期性的崩溃和重联，而NTM则可能与电流密度的不均匀分布有关。
-我还需要思考Sawteeth的分类和各自的机制。类型I可能主要是由于边缘不稳定的触发，导致核心参数的下降。而类型II可能涉及更复杂的过程，比如内部的磁重联或等离子体的重新组织。这种分类对于理解Sawteeth的影响和如何控制它们非常重要。
-此外，我需要考虑如何定量描述Sawteeth的周期和重联速率。可能需要一些参数，如崩溃时间、恢复时间、重联区域的面积等。这些参数可以用于模型中，预测Sawteeth的行为，并指导实验设计。
-总结一下，Sawteeth是一个复杂的MHD现象，涉及周期性的崩溃和磁重联，对等离子体的约束有显著影响，并且与其他不稳定性如NTM有关。理解这些机制对于优化托卡马克的运行和提高聚变反应效率至关重要。
-&lt;/think&gt;
-### 锯齿不稳定性（Sawteeth）的物理过程及其影响
+          <t>### 锯齿不稳定性（Sawteeth）的物理过程及其影响
 #### 核心结论
 锯齿不稳定性（Sawteeth）是一种与磁重联相关的托卡马克等离子体MHD不稳定性，会导致等离子体核心温度和密度周期性下降，影响芯部约束。锯齿不稳定性与其他MHD不稳定性如NTM（Neoclassical Tearing Modes）不同，主要表现为周期性崩溃和重联机制，对等离子体约束性能有显著影响。
 ---
@@ -6488,7 +5605,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -6514,18 +5631,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>嗯，用户让我阐述电阻壁模（RWMs）的物理特性，以及它对托卡马克先进运行模式的威胁。还要讨论等离子体旋转和主动反馈控制系统在RWMs稳定化中的作用。好的，我得先回忆一下相关的知识。
-首先，RWMs是一种磁流体不稳定性，通常发生在托卡马克的高约束模式下，比如H模。这些不稳定性会导致边缘等离子体的径向位移，可能引起等离子体与壁的接触，导致放电中断或者损坏壁材料。所以，这对托卡马克的稳定运行是一个很大的威胁。
-接下来，等离子体旋转对RWMs有什么影响呢？我记得旋转可以提供一个科里奥利力，抑制不稳定性的发展。当等离子体有适当的旋转速度和方向时，可以增加系统的稳定性。不过，如果旋转不够或者方向不对，可能反而会加剧不稳定。
-然后是主动反馈控制系统，这是通过实时监测RWMs的信号，利用线圈产生校正磁场来抵消不稳定性。这样的系统需要高带宽和快速响应，才能及时抑制不稳定性的发展。这种方法在许多托卡马克装置中已经被证明有效，尤其是在稳态运行中。
-我还需要考虑RWMs的物理机制，比如它的驱动力是什么，为什么在高约束模式下更严重。可能是因为边缘等离子体的高梯度和高带电粒子浓度，导致磁场和等离子体的相互作用更容易激发不稳定性。
-另外，等离子体旋转不仅仅是边缘，整个等离子体的旋转剖面都可能影响RWMs的发展。因此，控制等离子体的旋转，比如通过射频加热或外部驱动，可能会成为稳定化RWMs的一种手段。
-在讨论主动反馈系统时，我应该提到它的工作原理，比如如何检测RWMs的信号，如何快速调整线圈电流来产生校正磁场。这可能涉及到复杂的控制算法和传感器布局。
-还有，可能需要对比旋转和主动反馈系统在稳定化RWMs中的效果，或者讨论两者的结合使用是否能提供更 robust 的稳定性。
-最后，总结一下，RWMs对托卡马克的威胁主要在于它会导致等离子体的不规则运动，影响高约束模式的维持。而等离子体旋转和主动反馈控制系统是两种有效的稳定化手段，各有优缺点，可能需要根据具体装置的情况选择合适的策略。
-好的，现在我需要把这些思路整理成一个结构化的回答，按照用户给的规范来组织内容，确保每个部分都有足够的细节和清晰的解释。
-&lt;/think&gt;
-### 电阻壁模（RWMs）的物理特性及其对托卡马克先进运行模式的威胁
+          <t>### 电阻壁模（RWMs）的物理特性及其对托卡马克先进运行模式的威胁
 #### 1. **核心结论**
 电阻壁模（RWMs）是一种磁流体不稳定性，可能导致托卡马克等离子体与器壁接触，破坏高约束运行模式（H-mode）。等离子体旋转和主动反馈控制系统是稳定RWMs的关键手段。
 ---
@@ -6588,7 +5694,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -6614,15 +5720,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>好，我现在要回答关于速度空间不稳定性的问题。首先，我得理解什么是速度空间不稳定性。从名称上看，它可能与等离子体中粒子的速度分布有关，特别是当速度分布不均匀时可能引发的不稳定性。
-问题中提到了双流不稳定性、碰撞－尾部不稳定性等例子。我需要先分别解释这两种不稳定性，以及它们各自的驱动机制。然后，还要说明这类不稳定性在聚变等离子体中的重要性，特别是在中性束注入或波加热场景下的应用。
-首先，双流不稳定性。我想，这可能是在等离子体中存在两股相反方向运动的离子流，导致整体不稳定性。当这两股离子流的速度差超过某个临界值时，就会引发这种不稳定性，进而产生电磁波。这可能会影响聚变反应的稳定性，比如在中性束注入时，中性束的离子可能与原有等离子体中的离子形成双流结构。
-然后是碰撞－尾部不稳定性。这可能与高能粒子的“尾部”分布有关。当高能粒子由于与背景等离子体的碰撞而形成速度分布的尾部时，这些粒子可能驱动不稳定性。这可能发生在波加热过程中，当使用高频波加热等离子体时，高能粒子的分布可能变得不稳定，从而引发不稳定性。
-接下来，我要解释这些不稳定性在聚变等离子体中的重要性。双流不稳定性可能会影响中性束注入的效率和等离子体的加热效果，甚至可能导致等离子体不稳定性，影响装置的运行稳定性。碰撞－尾部不稳定性则可能出现在波加热过程中，导致能量的非预期损失，影响加热效率和等离子体的性能。
-在分析这些不稳定性时，可能需要考虑粒子的速度分布、碰撞率、频率等因素。此外，这些不稳定性可能通过驱动电磁波影响等离子体的整体动力学行为，进而影响聚变装置的性能和运行。
-综上所述，速度空间不稳定性是聚变等离子体中常见的现象，对装置的稳定性和性能有着重要影响。理解和控制这些不稳定性对于优化聚变反应堆的设计和运行至关重要。
-&lt;/think&gt;
-### 速度空间不稳定性
+          <t>### 速度空间不稳定性
 #### 核心结论
 速度空间不稳定性是指在等离子体中，由于粒子速度分布的不均匀性而引发的不稳定性现象，常见于中性束注入和波加热场景，影响等离子体的稳定性和能量 confinement。
 #### 背景与概念
@@ -6655,7 +5753,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -6681,16 +5779,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>嗯，我现在要比较宏观MHD不稳定性比如Kink模和微观漂移波不稳定性比如ITG/ETG模的不同。首先，我得回顾一下MHD和漂移波不稳定性各自的基本概念和特点。
-宏观MHD不稳定性主要涉及大尺度的等离子体行为，驱动机制通常是磁流体动力学中的磁压力和惯性效应。比如，Kink模不稳定性通常出现在环形等离子体中，当等离子体的磁压力超过磁张力时，就会发生这种不稳定性。它会导致等离子体形状的变化，比如扭曲，进而影响约束性能。
-微观漂移波不稳定性，如ITG和ETG模，起因于等离子体中离子和电子的微漂移运动。这些不稳定性在小尺度上发生，通常在托卡马克等装置的边界区域活跃。它们主要由梯度驱动，也就是等离子体的密度和温度梯度提供能量。这些不稳定性会导致粒子和热量的输运，影响整体的等离子体性能。
-在空间尺度方面，宏观MHD模式的空间尺度通常较大，与整个等离子体装置的尺寸相当，比如托卡马克的半径。而微观漂移波模式则在更小的尺度上，可能只涉及数毫米的范围。时间尺度上，宏观MHD模式通常发展较慢，时间尺度可能在秒级别，而微观模式则可能在毫秒或更短的时间内发展，导致高频振荡。
-对等离子体的影响方面，宏观MHD不稳定性可能导致等离子体形状的剧烈变化，甚至触发其他不稳定性或导致等离子体崩溃。微观漂移波不稳定性主要影响输运特性，特别是粒子和热量的输运，进而影响等离子体的约束性能和热负荷分布。
-我还需要考虑这些不稳定性在实验中的观测特征。宏观MHD不稳定性可能通过磁测量和等离子体形状的变化被检测到，而微观漂移波可能需要专门的诊断手段，如高分辨率的射线或微波诊断，来捕捉其快速变化。
-另外，控制和缓解这些不稳定性的方式也不同。对于宏观MHD，可能通过改变磁场配置、使用反馈控制或者调整等离子体参数来稳定。对于微观漂移波，可能需要优化等离子体的梯度分布，使用射频波或者其他手段来抑制它们的发展。
-总的来说，宏观和微观不稳定性在驱动机制、空间时间尺度以及影响等方面都有显著的不同，理解这些差异对于设计和优化聚变装置非常重要。
-&lt;/think&gt;
-### 宏观MHD不稳定性（如Kink模）与微观漂移波不稳定性（如ITG/ETG模）的比较分析
+          <t>### 宏观MHD不稳定性（如Kink模）与微观漂移波不稳定性（如ITG/ETG模）的比较分析
 #### 1. **核心结论**
 宏观MHD不稳定性（如Kink模）和微观漂移波不稳定性（如ITG/ETG模）在驱动机制、空间尺度、时间尺度以及对等离子体影响方面存在显著差异，具体如下：
 - **驱动机制**：Kink模由磁压力和惯性效应驱动，而ITG/ETG模由梯度驱动的离子和电子微漂移运动引起。
@@ -6746,7 +5835,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -6772,15 +5861,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，用户问的是如何利用先进的等离子体诊断技术来研究和识别不同类型的MHD不稳定性。首先，我得明确MHD不稳定性具体包括哪些类型，比如磁岛结构、模结构、增长率等等。然后，用户提到了几种诊断技术：ECE成像、微波反射计、软X射线阵列。我需要分别分析这些技术各自的特点和应用场景。
-ECE成像主要是用来测量电子温度的，它通过等离子体中的电子回旋谐波辐射来实现。当发生MHD不稳定性时，等离子体的温度分布会改变，ECE成像能够捕捉到这些变化，显示出温度的扰动区域，比如磁岛的结构。这一步我需要详细解释ECE的原理以及如何通过温度分布的变化来识别MHD现象。
-接下来是微波反射计，它测量的是等离子体的电子密度。微波反射计通过发送微波信号并接收反射信号来获取密度信息。在MHD不稳定性中，密度的波动也会伴随发生，比如在磁岛结构中，密度会出现周期性的变化。通过分析这些密度的时间序列和空间分布，可以判断不稳定性的发展情况，比如增长率的快慢。
-然后是软X射线阵列，这种诊断技术用于测量高能电子和离子的分布。软X射线通常来自等离子体中的热电子，当发生MHD不稳定性时，特别是在磁重联等过程中，高能电子的分布会发生变化。软X射线阵列能够提供关于能量分布的信息，帮助识别如模结构等特定类型的MHD不稳定性。
-在分析过程中，我还需要考虑这些诊断技术的综合应用。例如，ECE成像提供温度信息，微波反射计提供密度信息，软X射线阵列提供能量信息，三者结合可以更全面地识别MHD不稳定性类型，并评估其增长率和结构。
-此外，我还需要讨论每种技术的优缺点。例如，ECE成像的空间分辨率高，但对等离子体参数的依赖较强；微波反射计的时间分辨率高，但可能会受到噪声的影响；软X射线阵列能够提供能量信息，但对诊断系统的灵敏度要求较高。
-最后，总结这些诊断技术在实验中的实际应用和意义，指出它们对聚变装置设计和运行控制的帮助。比如，通过识别和分析MHD不稳定性，可以优化等离子体控制策略，提高装置的稳定性和效率。
-&lt;/think&gt;
-### 如何利用等离子体诊断技术研究MHD不稳定性？
+          <t>### 如何利用等离子体诊断技术研究MHD不稳定性？
 #### 1. 核心结论
 先进的等离子体诊断技术（如ECE成像、微波反射计、软X射线阵列）可以通过测量电子温度、密度和高能粒子分布等参数，实时捕捉MHD不稳定性（如磁岛结构、模结构、增长率）的时空演化特征，从而实现对不同MHD不稳定性类型的实验识别。
 ---
@@ -6836,7 +5917,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -6862,22 +5943,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>好，现在我要讨论“种子岛”在新经典撕裂模（NTM）发展过程中的关键作用，以及哪些物理过程或事件可能提供这些种子岛。作为一个刚开始学习聚变物理的学生，我对这些概念还不是很熟悉，所以需要慢慢理清楚。
-首先，我需要明确什么是“种子岛”以及新经典撕裂模（NTM）是什么。根据问题中的信息，种子岛是指在等离子体中形成的局部的、稳定的磁场结构，为NTM的形成提供初始的条件。NTM是一种非线性撕裂模，涉及等离子体中的磁场重联过程，可能导致等离子体的不稳定性。
-接下来，我需要了解哪些物理过程或事件可能提供种子岛。问题提到了锯齿、ELMs（边缘局域模）、误差场等可能性。我需要逐一分析这些过程是如何产生种子岛的。
-首先，锯齿现象。锯齿是托卡马克等离子体中常见的一种现象，通常涉及离子回旋频率附近的振荡。锯齿的形成可能与密度梯度的不稳定性有关。在锯齿过程中，可能会出现局部的密度梯度增加，从而导致磁场的重新连接，形成种子岛。不过，我还不太确定锯齿是否直接导致种子岛的形成，还是间接影响。
-接下来是ELMs，边缘局域模。ELMs是发生在托卡马克等离子体边缘的局域的、重复性的爆发现象，通常与高密度、高温度的区域有关。ELMs的发生可能涉及到边缘区域的磁场波动和不稳定性，这些波动可能导致局部磁场结构的改变，进而形成种子岛。不过，ELMs主要发生在边缘，而NTM的种子岛可能更靠近核心，因此需要考虑两者之间的关系。
-然后是误差场，即实验装置中的不完美磁场结构。误差场可能导致等离子体中的磁场出现局部的扰动，从而引发不稳定性。误差场的长期存在可能导致磁场的重新连接，形成种子岛。这种情况下，种子岛的形成是由于外部磁场的不完美，而非等离子体内部的动态过程。
-此外，我还需要考虑其他可能的因素，比如外部加热、电流驱动的不均匀性、等离子体与壁的相互作用等。这些因素可能会导致局部的磁场结构变化，从而形成种子岛。
-现在，我需要将这些思考整理成一个结构化的回答，按照问题给出的答题规范来组织内容。首先，给出核心结论，说明种子岛的关键作用以及可能的来源。然后，分背景与概念、原理与机理、工程意义、比较与拓展、要点总结几个部分详细阐述。
-在背景部分，需要明确种子岛和NTM的基本概念，以及它们在聚变等离子体中的重要性。接下来，在机理分析中，详细说明锯齿、ELMs、误差场是如何分别提供种子岛的。对于每个过程，需要解释其物理机制，并说明可能导致种子岛形成的条件。
-在工程或实验意义部分，需要讨论如何通过控制这些过程来抑制种子岛的形成，进而控制NTM的发展，以提高等离子体的稳定性和聚变反应的效率。
-比较与拓展部分，可以比较不同过程在形成种子岛方面的优缺点，指出哪种情况下更可能成为种子岛的主要来源，以及如何根据装置的具体情况采取相应的控制策略。
-最后，在要点总结中，重申种子岛的重要性，并提出具体的建议，如优化加热和电流驱动，控制误差场的水平，以减少种子岛的形成。
-在整个过程中，我需要注意逻辑的连贯性和条理的清晰性，确保每一部分都紧密联系，并且内容准确可靠。如果遇到不确定的地方，需要查证相关文献或资料，以确保结论的正确性。
-现在，我将按照这个思路来组织答案，确保每个部分都涵盖必要的内容，并且表达准确。
-&lt;/think&gt;
-## 逐步解析与答案
+          <t>## 逐步解析与答案
 ### 核心结论
 种子岛是新经典撕裂模（NTM）发展的关键，它通过提供初始的磁场重联结构启动NTM。锯齿、ELMs（边缘局域模）和误差场是可能的种子岛来源，各自通过不同的物理机制为NTM提供必要的初始条件。
 ### 背景与概念
@@ -6912,7 +5978,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -6938,22 +6004,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>好吧，我现在要解决这个问题，设计一个综合性的不稳定性控制策略，针对像ITER这样的未来聚变装置。首先，我得理解问题的各个关键因素和不同控制手段之间的权衡。
-首先，问题的核心在于控制托卡马克装置中的不稳定性，比如磁流体不稳定性（MHD）和边缘局部模（ELMs）。这些不稳定性会影响等离子体的稳定性和性能，因此控制它们对于聚变反应的成功至关重要。
-然后，我需要考虑的关键因素包括：
-1. 等离子体的宏观参数，如密度、温度、压力剖面，以及它们如何影响MHD稳定性。
-2. 边缘区域的稳定性，特别是ELMs，它们会导致能量和粒子的突然释放，影响壁材。
-3. 装置的硬件限制，如电流、电压、功率等对控制手段的约束。
-4. 不同控制手段之间的相互影响和潜在的权衡，比如主动反馈可能会影响其他参数，进而影响其他类型的不稳定性。
-接下来，思考各种控制手段的有效性和工程可行性：
-- 剖面控制通过调整压力、密度和温度来优化稳定性。这可能需要复杂的反馈系统，但可以有效预防不稳定性。
-- 主动反馈使用MHD传感器和控制线圈实时调整等离子体，快速响应，但硬件复杂且需要精确校准。
-- ELM缓解技术，如三维场误差或触发小ELMs，可以减少能量释放，但可能影响全局稳定性和等离子体约束。
-权衡这些手段时，需要考虑装置的具体运行模式，比如高约束模式（H-mode）可能更容易引发ELMs，因此可能需要更多的缓解策略。同时，要考虑成本、复杂性和维护可行性，确保策略能够在实际运行中实施。
-最后，综合策略可能需要分层控制，先使用剖面控制预防不稳定性，然后结合主动反馈快速响应，同时在边缘区域应用ELM缓解技术。这需要跨学科的合作和详细的模拟与实验验证，以确保策略的有效性和可行性。
-总的来说，设计这样的策略需要全面考虑多种因素，并在不同控制手段之间找到平衡，确保装置的稳定高效运行。
-&lt;/think&gt;
-针对ITER等未来聚变装置的不稳定性控制策略设计，需要综合考虑多种关键因素，并权衡不同控制手段的有效性和工程可行性。以下是详细的分步解释和答案：
+          <t>针对ITER等未来聚变装置的不稳定性控制策略设计，需要综合考虑多种关键因素，并权衡不同控制手段的有效性和工程可行性。以下是详细的分步解释和答案：
 ---
 ### **1. 核心结论**
 设计综合不稳定性控制策略的核心在于平衡磁流体稳定性（MHD）、边缘局部模（ELMs）和控制手段的工程可行性。策略应结合剖面控制、主动反馈和ELM缓解技术，确保等离子体在高约束条件下的稳定性。
@@ -7077,7 +6128,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -7103,17 +6154,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>嗯，我现在要比较托卡马克的L模、H模和I模运行的主要特征，包括边缘输运垒、ELM行为、粒子与能量约束以及杂质输运特性。然后还要解释为什么I模被认为是有吸引力的未来反应堆运行模式。
-首先，我得回顾一下托卡马克的不同运行模式。L模（低约束模式）是基本的，H模（高约束模式）则有更强的约束，I模（中间约束模式）可能是介于两者之间或者有其独特之处。
-关于边缘输运垒，L模可能没有明显的垒，因为约束较差。H模通常有明显的边缘输运垒，这是由于等离子体的梯度变化导致。I模可能有部分或者更弱的垒，或者结构不同。
-ELM行为方面，H模通常会周期性地发生ELM，释放大量能量，这可能对壁材料有侵蚀。I模可能有更稳定的ELM，或者更小的爆发，从而减少对壁的损坏。L模可能没有显著的ELM，因为约束不够。
-粒子和能量约束方面，H模显然比L模好，I模可能在这方面介于两者之间，或者有特别的优势，比如更高效的粒子排除或能量保持。
-杂质输运特性，L模可能杂质较多，因为输运垒弱，杂质容易进入核心。H模由于有垒，杂质可能被限制在边缘，减少污染。I模可能有更有效的杂质排除机制，或者更稳定的控制，防止杂质积累。
-为什么I模更有吸引力呢？可能因为它结合了H模的部分优点，比如较高的约束，同时降低了ELM的负面影响，比如爆发能量过大。此外，I模可能更容易控制，适合持续运行，减少维护需求，适合商业化反应堆。
-我还得考虑这些模式的触发和维持条件，比如射频加热、磁场配置等，这些可能影响各模式的特性。此外，不同装置的设计可能会影响这些模式的表现，比如仿星器和托卡马克的差异，但这里主要讨论托卡马克的情况。
-总结一下，I模可能在约束性能、ELM控制和杂质管理方面找到平衡，使其成为未来聚变反应堆的理想选择。它可能减少了对结构材料的热负荷，提高了运行的稳定性和经济性，这些都是未来反应堆设计的关键因素。
-&lt;/think&gt;
-### 比较托卡马克的L模、H模和I模运行的主要特征
+          <t>### 比较托卡马克的L模、H模和I模运行的主要特征
 #### 1. **核心结论**
 H模具有最佳的能量和粒子约束，L模则相反，I模则在约束性能、边缘稳定性和杂质控制方面表现出色，被认为是未来反应堆有吸引力的运行模式。
 #### 2. **背景与概念**
@@ -7142,7 +6183,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -7168,25 +6209,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>好吧，我现在遇到了一个关于托卡马克等离子体启动阶段的问题，需要估算击穿所需的最小环向电场，也就是Paschen最小场。同时，还有一个关于中心螺线管磁通变化量的推导问题。作为刚开始学习聚变物理的学生，我得一步一步地理清楚思路，看看能不能解决这个问题。
-首先，关于Paschen最小场的问题。我记得Paschen定律是关于气体击穿电压的，通常用于气体放电现象。公式大概是V=(B + A/p) * pd，其中p是压力，d是电极间距，A和B是与气体类型相关的常数。那在托卡马克中，这个电场是环向的，可能和极向电场有关？或者说，这里的问题其实是关于产生足够的环向电场来启动等离子体放电。
-托卡马克中的环向电场通常由纵磁场（poloidal field）的时变来产生，根据法拉第定律，变化的纵磁场会产生环向电动势。在启动阶段，可能需要克服电阻，所以必须有足够的电场来推动电流流动。那Paschen最小场是否在这里指的是启动所需的最低环向电场呢？
-假设我们需要一个环向电场E_φ，那么根据欧姆定律，E_φ = (V_φ)/R，其中V_φ是环向电压降，R是大环径。同时，启动阶段可能涉及到等离子体的电导率，这会影响所需的电场强度。如果电导率σ较低，那么需要更高的电场来产生足够的电流。
-然后是第二个问题，推导中心螺线管所需的磁通变化量ΔΨCS。中心螺线管用于产生纵磁场，进而驱动等离子体电流。已知等离子体电流从0增加到Ip，时间Δt，等离子体电感Lp和电阻Rp。根据电磁感应定律，螺线管的磁通变化会产生感应电动势，进而驱动电流。
-首先，等离子体电流的变化率是dI/dt = Ip / Δt。根据法拉第定律，感应电动势E = Lp * dI/dt。同时，E也等于螺线管磁通的变化率ΔΨCS / Δt。所以，我们可以得到ΔΨCS = Lp * Ip。这可能是一个初步的推导，但需要考虑电阻等因素吗？
-或者，是否需要考虑电阻对电压的贡献？因为欧姆定律中，电压还可能有V = E * R，其中E是电场，R是电阻。所以，总的电动势应该是V = E_感应 + E_欧姆，也就是V = Lp * dI/dt + Rp * I。但在这个问题中，等离子体电流从0开始，所以I在Δt时间内线性增长，平均电流是Ip/2，可能影响结果。
-不过，题目中说通过中心螺线管在Δt时间内将电流从0驱动到Ip，那么可能主要关注的是螺线管产生的磁通变化来驱动电流，而电感和电阻的影响可能分别考虑。具体来说，磁通变化引起的感应电动势应该等于等离子体中的电压降，包括电感和电阻部分。
-那正确的公式是否应该是ΔΨCS = Lp * dI/dt * Δt + Rp * I * Δt？或者更准确地说，积分感应电动势和电阻压降。但可能我在这里有点混淆了，因为感应电动势是dΦ/dt，而电阻压降是I*R。
-再回到问题，它要求推导ΔΨCS的表达式。根据法拉第电磁感应定律，螺线管磁通的变化会产生一个电动势，等于感应电动势。等离子体中的电流变化需要克服电阻，同时电感储存磁场能量。因此，总的电动势应该满足E = Lp * (dI/dt) + Rp * I。
-由于电流从0开始，线性增加到Ip，在Δt时间内，电流I(t) = (Ip/Δt) * t。所以，dI/dt = Ip/Δt。积分感应电动势和电阻压降：
-ΔΨCS = ∫ E dt = ∫ (Lp * dI/dt + Rp * I) dt 从0到Δt。
-积分第一项：∫ Lp * (Ip/Δt) dt = Lp * Ip。
-积分第二项：∫ Rp * (Ip/Δt) * t dt = Rp * Ip/Δt * (Δt^2)/2 = Rp * Ip * Δt / 2。
-所以，ΔΨCS = Lp * Ip + Rp * Ip * Δt / 2。
-但不确定是否正确，或者是否有更简单的方式。因为有时候，可能假设电阻压降相对于电感来说可以忽略不计，尤其是在快速变化的情况下，可能主要考虑电感部分。但题目中给出的参数包括Rp，所以可能需要考虑进去。
-总结一下，核心结论是：托卡马克启动时的最小环向电场约为E_min = (2eV)/(n^(1/3) R)，中心螺线管磁通变化量ΔΨCS = Lp * Ip + (Rp * Ip * Δt)/2。
-&lt;/think&gt;
-### 问题答案
+          <t>### 问题答案
 #### 1. 击穿所需的最小环向电场（Paschen最小场）
 **核心结论**  
 托卡马克等离子体启动阶段的最小环向电场约为 $E_{\text{min}} = \frac{B}{n^{1/3}R}$，其中 $B \approx 2 \, \text{V·cm}^{-1}$ 是常数，$n$ 是电子密度，$R$ 是大环半径。
@@ -7227,7 +6250,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -7253,18 +6276,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>嗯，我现在要回答关于托卡马克中等离子体位形控制以及垂直不稳定性和快速反馈控制系统的问题。我得先理清这些概念，然后一步步分析。
-首先，核心结论应该是精确控制位形对托卡马克运行至关重要，而垂直不稳定性是其中一大挑战，需要用快速反馈系统来应对。
-背景方面，托卡马克的等离子体位形由大半径、小半径、垂直位置、拉长和三角变形等参数描述。这些参数的变化影响等离子体的稳定性、约束性能以及壁相互作用。特别是垂直位置的不稳定，可能导致等离子体接触器壁，造成损坏或中断运行。
-接下来，机理分析部分需要详细说明垂直不稳定的原理。这种不稳定性通常是由于等离子体的电磁力导致的垂直方向上的运动。当等离子体的自举电流变化时，可能会引发垂直漂移，进而导致不稳定性。
-然后，实现方法部分要讨论如何通过控制线圈和反馈系统来精确调节位形。这可能涉及实时监测等离子体参数，利用传感器数据快速计算所需的控制信号，然后调整线圈电流来抵消不稳定性。
-定量估算部分，可能需要引入一些公式，比如描述垂直位置动态的方程，以及反馈系统响应时间的计算。这里可能需要假设一些参数，如等离子体的质量、阻尼系数、反馈增益等，来估算系统的稳定性和响应速度。
-工程意义方面，精确的位形控制可以提高等离子体的稳定性和约束性能，延长运行时间，减少对壁的损伤。而快速反馈系统则能及时抑制不稳定，防止等离子体失控。
-比较与拓展部分，可以比较不同类型的反馈控制策略，如比例-积分-微分（PID）控制、模型预测控制（MPC）等，讨论它们的优缺点和适用条件。
-最后，要点总结要简明扼要地重申精确控制的重要性以及快速反馈系统的关键作用。
-整个思考过程中，我需要确保每个部分都有清晰的逻辑，理论推导部分要准确，避免遗漏关键点。同时，要注意使用规范的术语和单位，确保回答的专业性和严谨性。
-&lt;/think&gt;
-### 托卡马克中等离子体位形控制的重要性及实现方法
+          <t>### 托卡马克中等离子体位形控制的重要性及实现方法
 #### 1. **核心结论**
 托卡马克中等离子体位形的精确控制对实现稳定的聚变反应至关重要，而垂直不稳定性是主要挑战，需通过快速反馈控制系统来实现稳定。
 ---
@@ -7336,7 +6348,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -7362,17 +6374,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>嗯，今天老师布置了一个关于托卡马克破裂的问题，我得好好想想怎么回答。首先，什么是托卡马克破裂呢？我记得托卡马克是一种用于核聚变的装置，它利用强磁场来约束等离子体。破裂应该是指等离子体约束突然失效，导致能量迅速释放的情况。这可能对装置造成严重损害。
-接下来，问题要求列举几种主要的破裂前兆和触发机制。破裂前兆应该是破裂发生前的一些征兆，比如等离子体参数的变化。触发机制则是导致破裂发生的直接原因。比如，如果等离子体的约束不稳定，就可能引发破裂。我还记得有些机制是关于等离子体内部突然放电的，比如电流突然变化。
-然后，讨论破裂对装置的潜在危害，特别是第一壁和真空室。这可能包括热负荷、电磁力和逃逸电子。热负荷应该是指破裂时大量能量突然释放到装置壁上，导致温度骤升，可能损坏材料。电磁力可能是因为等离子体中的电流变化迅速，产生强大的力，导致结构变形。逃逸电子则是指从等离子体中逃出的高能电子，可能打到装置壁上，造成进一步的损害。
-现在，我需要详细思考每一个部分。首先是托卡马克破裂的定义。托卡马克利用环形磁场来约束等离子体，维持高温高压环境。如果磁场突然失去控制，等离子体可能会迅速失去约束，这就是破裂。这种现象对装置来说非常危险，因为大量的能量会在短时间内释放，可能损坏设备甚至引发事故。
-然后是破裂前兆。可能的前兆包括等离子体参数的快速变化，比如温度、密度、电流等的异常波动。例如，内部扰动可能表现为局部温度突然升高，或者等离子体形状的急剧变化。此外，磁场传感器可能会检测到异常的磁信号，预示着即将发生的破裂。
-触发机制方面，可能包括等离子体不稳定性，如磁流体动力学不稳定性（MHD）。当等离子体中的某些模式变得不稳定时，可能会触发破裂。另一个可能的机制是电流突然增加或减少，导致磁场结构破坏。还有，边界条件的突然变化，比如等离子体与壁接触，也可能触发破裂。
-关于潜在危害，热负荷是一个大问题。破裂时，等离子体中的能量可能迅速传递到装置壁，导致第一壁温度急剧上升，可能超过材料的熔点，造成损坏。电磁力方面，由于等离子体中的电流变化迅速，会产生强大的电磁力，可能导致托卡马克的结构变形或受损。此外，逃逸电子携带高能量，可能与装置壁发生碰撞，产生X射线或其他辐射，进一步威胁装置的安全。
-我还需要考虑这些危害的具体影响。例如，热负荷可能导致材料剥落，影响后续的聚变反应。电磁力可能损坏支撑结构，导致装置无法正常运行。逃逸电子可能引起局部的高剂量辐射，威胁设备和人员的安全。
-总结一下，托卡马克破裂是一个严重的物理现象，涉及等离子体约束的突然失效。它由多种前兆和触发机制引起，对装置的结构和材料造成多方面的危害。了解这些机制和危害对于设计更安全、更可靠的聚变装置至关重要。
-&lt;/think&gt;
-**什么是托卡马克破裂？列举几种主要的破裂前兆和触发机制。讨论破裂对装置（特别是第一壁和真空室）的潜在危害，如热负荷、电磁力和逃逸电子。**
+          <t>**什么是托卡马克破裂？列举几种主要的破裂前兆和触发机制。讨论破裂对装置（特别是第一壁和真空室）的潜在危害，如热负荷、电磁力和逃逸电子。**
 ### 核心结论
 托卡马克破裂是等离子体约束失效导致的能量快速释放事件，主要由不稳定性、外部触发和边界问题引起，对装置造成热负荷、电磁力和逃逸电子等危害。
 ### 背景与概念
@@ -7404,7 +6406,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -7430,16 +6432,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>好，我现在需要帮用户综述托卡马克破裂的预测和规避技术，以及讨论AI/机器学习在实时预测中的优缺点和挑战。
-首先，托卡马克破裂是什么？它是指等离子体约束失效，导致能量突然释放，可能损坏装置。所以，预测和规避非常重要。
-对于预测技术，我记得有基于物理模型的方法，比如二维流体模型，用来分析等离子体的稳定性。不过这些模型计算量大，可能不适合实时预测。还有一种是基于诊断数据的统计方法，比如使用机器学习模型分析多种参数，寻找破裂的前兆信号。这种方法可以处理大量数据，但需要足够的训练数据，而且结果可能不够直观。
-再来看规避技术，常见的有破裂前的触发控制，比如迅速向等离子体注射吹灰气体，或者破坏环流结构，迫使等离子体破裂在早期发生，减少对设备的损害。还有主动控制，比如调整磁场或射频波，维持等离子体的稳定性。但是这些方法需要精确的控制和快速的响应，实现起来有难度。
-现在，关于AI/机器学习在实时预测中的优势。首先，AI可以处理多源数据，同时分析很多参数，发现潜在的破裂模式。其次，AI模型在训练后预测速度快，适合实时应用。此外，AI能从大量历史数据中学习，发现人类难以察觉的模式，提高预测的准确性。
-不过，挑战也不少。AI模型需要大量高质量的数据来训练，这可能是一个问题。另外，AI的预测结果有时候是黑箱，难以解释，这对于需要明确物理机制的聚变实验来说是个挑战。还有，AI模型的泛化能力有限，如果测试环境与训练环境差异大，预测效果会下降。此外，实时预测需要低延迟，而复杂的AI模型可能计算时间过长，影响实时性。
-用户可能的背景是什么？可能是一位聚变物理的研究生或工程师，想了解最新的技术进展，尤其是AI在其中的应用。他们可能想知道这些方法的可行性和限制，以便在实际工作中应用或进一步研究。
-综上所述，我需要将这些思考整理成结构化的回答，确保涵盖核心结论、背景、技术综述、AI的优势和挑战，以及工程意义，同时保持逻辑清晰，语言准确。
-&lt;/think&gt;
-### 1. **核心结论**  
+          <t>### 1. **核心结论**  
 托卡马克破裂可以通过多种物理模型和实时诊断技术进行预测和规避。人工智能/机器学习方法在实时破裂预测中具有处理多源数据和快速预测的优势，但也面临数据质量、模型可解释性和实时性等挑战。
 ---
 ### 2. **背景与概念**  
@@ -7483,7 +6476,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -7509,18 +6502,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>好的，我现在需要回答用户关于托卡马克破裂缓解策略的问题，特别是大规模气体注入（MGI）和碎裂弹丸注入（SPI）的比较。用户希望我按照之前的规范来详细回答，所以我需要一步步理清楚思路。
-首先，我得明确问题的核心是什么。用户想知道这两种方法的优缺点、物理机制以及它们在SPARC和ITER装置上的应用前景。所以，我的回答需要覆盖这些方面，并且按照用户给出的结构来组织内容。
-接下来，我应该先回忆一下托卡马克中的破裂现象。破裂通常指的是等离子体突然失去稳定性，导致性能急剧下降，可能对装置造成损害。因此，破裂缓解策略非常重要，以保护设备并提高运行效率。
-关于MGI，我知道它是通过向等离子体中注入大量气体来稀释温度和压力，从而减缓破裂的影响。而SPI则是利用弹丸靶材料，碎裂后快速注入等离子体内部，增加等离子体的密度，同样达到缓解的效果。
-在物理机制上，MGI主要是通过增加等离子体的体积和压力来降低内爆力，同时稀释温度，减少能量释放。而SPI则是在破裂发生时，通过快速注入材料，使等离子体内部的压力和温度迅速变化，从而减少对壁的影响。
-然后，比较两者的优缺点。MGI的优点在于可以预见地进行气体注入，控制较为容易，适用性强。缺点是需要大量气体，可能会影响等离子体的性能，例如增加杂质浓度，影响后续运行。而SPI的优点是响应速度快，能够精准地注入到破裂区域，减少对整体等离子体的干扰。缺点是技术复杂，需要精确控制弹丸的碎裂和注入，而且在破裂发生时可能难以及时应对。
-在应用前景方面，SPARC和ITER作为下一代聚变装置，它们的规模和运行参数更高，因此破裂缓解的需求更迫切。MGI已经在一些装置中得到了验证，可能更容易在SPARC和ITER中实施。而SPI由于其高效性和针对性，也可能在未来的装置中得到应用，特别是在快速响应方面。
-此外，我还需要考虑工程和实验意义。MGI在工程上较为成熟，但需要处理气体供应和杂质控制的问题。SPI则需要解决弹丸设计和控制系统的技术挑战。
-最后，总结要点时，应强调每种方法的适用场景和可能的发展方向，以及它们在不同装置中的应用前景。
-现在，我需要将这些思路组织成符合用户要求的结构，包括核心结论、背景与概念、原理与推导、优缺点比较、应用前景、比较与拓展，以及要点总结。确保每个部分都清晰明了，语言规范，符合学术严谨性。
-&lt;/think&gt;
-### 核心结论
+          <t>### 核心结论
 托卡马克破裂缓解主要通过大规模气体注入（MGI）和碎裂弹丸注入（SPI）实现，两者均通过向等离子体注入物质来缓解破裂，但MGI适用于预测性破裂缓解，而SPI适合突发性破裂缓解，且SPI在极端条件下效果更佳。
 ---
 ### 背景与概念
@@ -7565,7 +6547,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -7591,15 +6573,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>嗯，我现在要分析托卡马克和仿星器实现稳态或长脉冲运行的关键挑战。首先，这两种装置都是核聚变研究中的重要设备，但它们的结构和运行机制有所不同，所以面临的挑战可能也有差异。
-连续的加热和电流驱动可能是主要问题。托卡马克通常使用射频波加热，比如电子回旋加热和离子回旋加热，而仿星器可能更多地依赖中性束注入或者射频波。电流驱动方面，托卡马克可能需要外部的电流驱动技术，如低杂波电流驱动，而仿星器则可能依靠其结构的自举电流。但如何维持稳定的电流分布和足够的电流密度，特别是在长时间运行中，是个难点。
-热量和粒子排除也是一个关键问题。长时间运行意味着更多的能量需要被排出，否则会导致等离子体参数偏离最佳值。托卡马克可能需要高效的排热系统，比如利用边缘的散热，而仿星器可能因为其复杂磁拓扑结构，排热路径更长，处理起来更困难。此外，粒子排除需要处理燃料补充和杂质控制，这可能影响等离子体的纯净度。
-等离子体与壁的相互作用在长时间运行中尤为重要。托卡马克的等离子体边界可能会因为频繁的接触而产生侵蚀，释放出杂质影响聚变反应。仿星器的结构可能导致等离子体与壁的接触更为复杂，需要更有效的壁保护技术，比如使用偏滤器或者其他保护层。
-部件的可靠性直接关系到整个装置的运行寿命。托卡马克的超导磁体和仿星器的复杂线圈都需要长时间承受高应力，材料的耐久性和冷却系统的可靠性都是挑战。此外，诊断设备和控制系统需要长时间稳定工作，这要求很高的工程制造水平和维护能力。
-比较两者，托卡马克可能在加热和排热方面有更成熟的技术，但需要解决复杂的等离子体边界问题；而仿星器在实现稳态运行方面有潜力，但工程实现和材料可靠性是主要障碍。未来的发展可能需要结合两者的优点，开发更高效的加热和排热系统，同时优化材料和结构设计。
-总结一下，关键挑战包括加热与电流驱动、热量和粒子排除、等离子体壁相互作用以及部件可靠性。每种装置都有其特定的难点，需要针对性的技术突破和工程创新。
-&lt;/think&gt;
-### 分析实现托卡马克和仿星器稳态或长脉冲运行的关键挑战
+          <t>### 分析实现托卡马克和仿星器稳态或长脉冲运行的关键挑战
 #### **核心结论**
 托卡马克和仿星器实现稳态或长脉冲运行面临的核心挑战包括连续的加热与电流驱动、高效的热量与粒子排除、等离子体与壁的长期相互作用，以及关键部件的可靠性与寿命。
 ---
@@ -7657,7 +6631,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -7683,16 +6657,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>好，我现在要回答关于误差场在托卡马克中的来源及其对稳定性的影响，以及如何通过制造和安装线圈来控制这些问题。我得先理清楚误差场的基本概念。
-误差场主要来自工程上的不精确，比如线圈位置偏移、形状偏差，还有铁磁材料的影响。这些不完美的地方会导致原本设计中的完美环形磁场出现扰动，形成误差场。误差场会影响等离子体的稳定性，特别是锁定现象，这会破坏等离子体的约束性能。
-接下来，我要详细分析误差场对托卡马克等离子体稳定性的影响。锁定是指误差场导致等离子体和磁场之间产生同步，使得等离子体的环向运动被锁定，从而引发较大的不规则运动，导致等离子体不稳定性。这里需要解释误差场如何导致锁模现象，以及锁模对等离子体的影响。
-然后，如何通过精密制造和安装线圈来控制误差场？首先，线圈制造需要极高的精度，误差控制在微米级别。其次，安装过程中必须确保每个线圈的位置准确无误，可能需要使用高精度的定位设备和检测工具。此外，还可以在设计上加入冗余，以便后续调整。
-主动误差场补偿也是重要的一环。通过在托卡马克周围布置额外的线圈，实时检测误差场，并施加相反的磁场来抵消误差场的影响。这部分需要涉及如何选择线圈的位置和数量，以及控制系统的反馈机制。
-在讨论这些措施时，我还要考虑到工程上的可行性。比如，高精度制造的成本和复杂性，以及主动补偿系统的实时性和可靠性。这些都是实际应用中需要权衡的因素。
-最后，要点总结部分要简明扼要，重申误差场的来源、影响及控制方法。这有助于读者迅速抓住关键信息。
-在整个思考过程中，我需要确保每一步都逻辑清晰，用词准确，并且紧密结合实际应用，避免过于理论化。同时，要确保各部分内容之间有良好的衔接，使整个回答结构严谨，易于理解。
-&lt;/think&gt;
-### 误差场的来源及其对托卡马克等离子体稳定性的影响
+          <t>### 误差场的来源及其对托卡马克等离子体稳定性的影响
 #### 1. 核心结论
 误差场主要来源于制造、安装过程中的不精确性和铁磁材料的影响，会导致托卡马克等离子体中的锁模现象，降低等离子体稳定性。通过高精度制造、安装线圈和使用主动误差场补偿系统，可以有效控制误差场的影响。
 #### 2. 背景与概念
@@ -7711,7 +6676,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -7737,17 +6702,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>好吧，我需要讨论在长脉冲或稳态运行条件下，等离子体控制系统（PCS）需要具备哪些先进功能，尤其是如何同时控制动理学剖面（温度、密度、旋转）和磁面位形。首先，我要理解PCS的基本功能，以及长脉冲或稳态运行对PCS的不同要求。
-长脉冲或稳态运行意味着等离子体需要长时间保持稳定，这对PCS的控制功能提出了更高的要求。传统PCS可能在控制等离子体基本参数上已经比较成熟，但在面对长时间运行时，可能需要更先进的功能来维持稳定。
-首先，动理学剖面的控制包括温度、密度和旋转。温度梯度和旋转化学动力学剖面会影响等离子体的稳定性。比如，温度梯度大可能导致不稳定性，而旋转有助于增强稳定性。磁面位形控制涉及维持等离子体的形状和位置，以防止与壁接触或避免内部扰动。同时控制这两个方面需要PCS能够协调多种控制手段，可能涉及射频（RF）、中性束注入（NBI）以及磁反馈控制等。
-然后，我想到PCS需要具备多目标优化能力，因为同时控制动理学和磁面位形涉及多个变量和目标。优化算法需要处理复杂的相互作用，可能需要机器学习或模型预测控制等先进技术。
-实时性和鲁棒性也是关键，因为长时间运行中参数可能会有漂移或外部干扰。PCS需要快速响应并维持控制性能，可能需要闭环控制和自适应调整。
-此外，耦合动力学行为需要考虑，比如电流驱动、动理学效应和磁扰动之间的相互影响。PCS应该能够处理这些复杂的相互作用，可能需要综合模型和多物理场仿真。
-量化评估功能也很重要，系统需要在运行中持续评估控制效果，及时调整策略。这可能包括在线诊断数据的反馈和实时优化。
-最后，冗余和容错能力确保系统在部分故障时仍能继续运行，这对长时间运行尤其重要。
-总的来说，PCS在长脉冲或稳态运行条件下需要具备多目标优化、实时鲁棒控制、处理复杂耦合、量化评估以及冗余容错等功能，以确保等离子体的长期稳定和高效运行。
-&lt;/think&gt;
-在长脉冲或稳态运行条件下，等离子体控制系统（PCS）需要具备以下先进功能，以实现对动理学剖面（温度、密度、旋转）和磁面位形的同时控制：
+          <t>在长脉冲或稳态运行条件下，等离子体控制系统（PCS）需要具备以下先进功能，以实现对动理学剖面（温度、密度、旋转）和磁面位形的同时控制：
 ### 1. 核心结论
 等离子体控制系统（PCS）需要具备多目标优化能力，同时控制动理学剖面和磁面位形，以确保长时间的稳定运行。
 ### 2. 背景与概念
@@ -7773,7 +6728,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -7799,17 +6754,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，今天遇到了一个问题，是关于仿星器和托卡马克在等离子体运行和控制方面的区别，特别是破裂现象和运行边界的决定因素。作为刚刚接触聚变等离子体物理的新手，我得先理清楚这些概念。
-首先，我得回忆一下托卡马克和仿星器的基本结构。托卡马克是利用环形磁铁的装置，等离子体在环形路径中运行，而仿星器则具有三维的磁结构，这可能使得它们的磁场分布和等离子体行为有所不同。
-关于破裂现象，我知道在托卡马克中，破裂是等离子体突然失去约束，导致能量迅速释放的现象。这通常与等离子体的不稳定性有关，比如压磁不稳定性。那么，仿星器是否存在类似的破裂现象呢？可能仿星器的三维磁场能够更好地抑制某些不稳定性，所以破裂的可能性较低。
-接下来是运行边界的问题。托卡马克的运行边界主要由磁安全因子q、等离子体压力和电流等因素决定。那么仿星器的边界又由哪些因素决定呢？可能包括磁场的三维结构参数，如扭曲角、螺旋度等，以及电流分布、等离子体压力等。
-我得进一步思考，三维磁场的复杂性是否带来了更多的控制参数，这些参数如何影响等离子体的稳定性和约束性能。比如，磁场的螺旋度可能影响等离子体的输送过程，而扭曲角可能影响等离子体的稳定性。
-另外，仿星器的几何形状和尺寸是否也影响运行边界？比如，设备的大小是否会影响等离子体的行为，或者磁场的强度和分布如何影响等离子体的约束。
-在查阅相关资料时，我发现仿星器确实利用三维磁场来实现等离子体的约束，这使得它们在某些方面比托卡马克更有优势，比如更好的粒子输送和能量约束。然而，仿星器的设计和控制也更为复杂，需要考虑更多的参数。
-至于破裂现象，虽然仿星器的三维磁场可以减少不稳定性，但并不意味着完全没有破裂的风险。例如，极端的等离子体参数或外部扰动仍可能导致等离子体失去约束，引发破裂。因此，仿星器可能也有破裂现象，但其触发条件和机制可能与托卡马克不同。
-总结一下，仿星器与托卡马克在等离子体运行控制方面的本质区别主要体现在磁场的结构和维度上，仿星器的三维磁场提供了更好的约束和稳定性，但也引入了更多的控制参数和复杂的物理过程。运行边界由磁场参数、电流分布、等离子体压力等因素共同决定，而破裂现象虽然可能存在，但其触发机制可能与托卡马克不同。
-&lt;/think&gt;
-仿星器和托卡马克在等离子体运行控制方面存在显著差异，主要体现在磁场结构和等离子体行为上。以下是详细分析：
+          <t>仿星器和托卡马克在等离子体运行控制方面存在显著差异，主要体现在磁场结构和等离子体行为上。以下是详细分析：
 ### 1. 核心结论
 仿星器与托卡马克在等离子体运行控制方面存在本质区别，主要体现在磁场的三维结构和等离子体行为的复杂性。仿星器的三维磁场设计能够减少某些不稳定性，但仍可能存在破裂现象，其运行边界由多种参数共同决定。
 ### 2. 背景与概念
@@ -7887,7 +6832,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -7913,16 +6858,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>好的，我现在需要比较中性束注入（NBI）、电子回旋共振加热（ECRH）和离子回旋共振加热（ICRH）这三种主要的辅助加热方法。首先，我应该理解每种方法的基本原理和作用机制。
-中性束注入听起来是通过注入中性粒子，这些粒子通过与等离子体中的离子碰撞来传递能量，加热等离子体。而电子回旋共振加热和离子回旋共振加热则是利用微波与特定粒子的回旋共振来加热，但分别针对电子和离子。
-接下来，我需要分析每种方法的能量耦合机制。NBI是通过直接碰撞，所以能量传递效率可能依赖于中性束的注入能量和等离子体的密度。而ECRH和ICRH则是非接触式的，通过电磁波与粒子的相互作用，因此效率可能与波的频率、等离子体的参数（如密度、温度）有关。
-然后是加热效率，这可能涉及到能量传递的有效性和是否产生不必要的副作用，比如对等离子体其他参数的影响。比如，NBI会增加等离子体的密度，可能还引入杂质，而ECRH和ICRH可能会影响电流分布或者产生过热的电子。
-对等离子体参数的影响也很重要。比如，NBI注入的中性粒子会增加等离子体的密度，而ECRH主要加热电子，可能导致电子温度过高，影响整体温度平衡。ICRH则主要加热离子，可能有助于维持离子温度，从而促进聚变反应。
-技术挑战方面，NBI可能需要高效的中性束产生装置，以及防止束与等离子体相互作用时的损失。ECRH和ICRH可能面临波的传播和共振条件的复杂性，以及如何有效耦合到等离子体中。
-最后，我应该总结每种方法的优缺点，指出它们在实际应用中的适用性。比如，NBI在高密度等离子体中效果较好，但可能需要处理杂质问题；ECRH适合需要快速电子加热的情况，但可能对等离子体稳定性有影响；ICRH则在加热离子方面有效，适合维持较高的离子温度。
-在整个过程中，我需要确保自己对每种方法的理解是准确的，必要时查阅相关资料来确认关键点，比如具体的加热机制、能量传递效率的计算方式，以及它们对等离子体参数的具体影响。
-&lt;/think&gt;
-### 比较中性束注入（NBI）、电子回旋共振加热（ECRH）和离子回旋共振加热（ICRH）
+          <t>### 比较中性束注入（NBI）、电子回旋共振加热（ECRH）和离子回旋共振加热（ICRH）
 #### 1. **物理原理**
 - **中性束注入（NBI）**：通过将中性粒子束注入聚变装置中，这些中性粒子与等离子体中的离子发生碰撞，将动能传递给等离子体，从而加热等离子体。
 - **电子回旋共振加热（ECRH）**：利用微波与等离子体中电子的回旋共振，将电磁波的能量转化为电子的热能。
@@ -7952,7 +6888,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -7978,18 +6914,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>好的，我现在要回答用户的问题，关于ITER计划中1 MeV中性束注入系统的关键技术特点和挑战，以及如何通过实验监测NBI的性能。这个问题涉及聚变等离子体物理和工程，所以我需要详细分析。
-首先，我需要明确问题中的关键技术点。用户提到了负离子源的产生与中性化、束线的长距离传输和功率沉积控制，这些都是中性束注入系统的重要部分。我需要逐一分析每个部分的技术特点和挑战。
-对于负离子源的产生与中性化，我知道负离子的产生通常涉及复杂的物理过程，比如电弧放电或者射频放电。从中性氢到H-的过程需要克服库仑势垒，这通常需要高密度等离子体环境和精确控制的几何结构。中性化部分，比如使用气体靶或固体靶，各有优缺点，需要考虑中性化效率和束流质量。
-接下来是束线的长距离传输。ITER的束线很长，约30米，所以需要考虑电场的精确控制，避免束流散焦。磁场的使用也很关键，可能需要高精度的磁铁和磁场分析。束流的稳定性在传输过程中也是一个挑战，因为任何微小的波动都可能导致束流损失。
-功率沉积控制则是另一个关键点。中性束注入的高能量会导致等离子体加热，产生高能粒子，这些粒子可能引起多种不稳定性。ITER需要精确控制功率沉积的位置和分布，以避免对设备的损害和对等离子体稳定性的影响。这可能需要复杂的反馈控制系统。
-然后是实验监测NBI性能的部分。用户提到了沉积剖面，我需要考虑如何监测。常用的诊断方法包括光谱学，比如测量中性束与等离子体相互作用产生的光谱，可以推断出沉积的位置和能量分布。另外，中子诊断可以用来测量注入的中性束与等离子体的相互作用情况。还有探针测量，可以监测束流的强度和分布。
-接下来，我需要将这些思路整合成一个有结构的回答，按照用户提供的格式规范。核心结论要简明，背景与概念要清晰，原理与推导要详细，定量估算如果有数据的话，工程或实验意义也要明确，比较与拓展如果有相关内容的话，最后要点总结。
-在写作过程中，我需要确保使用正确的物理术语和单位，方程部分用Latex表示，结构清晰，每个部分都有小标题。同时，要注意问题是否需要进一步假设或信息，如果有的话，也要明确指出。
-最后，我要检查整个回答是否符合用户的写作要求，确保严谨、客观，不输出未经验证的猜测，避免遗漏任何关键点。可能还需要在回答中加入一些实际案例或数据，以增强说服力。
-通过这样的思考过程，我应该能够提供一个全面、结构清晰且符合规范的回答。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 ITER计划的1 MeV中性束注入系统采用负离子源、高效的中性化和长束线传输技术，面临负离子产生效率低、束流中性化不完全及束线传输损耗等挑战，通过光谱学、中子诊断和探针测量等手段监测沉积剖面。
 ---
 ### 背景与概念  
@@ -8066,7 +6991,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -8092,24 +7017,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>好的，我现在要详细思考用户关于电子回旋电流驱动（ECCD）在新经典撕裂模（NTM）控制中的应用问题。首先，我需要理解用户的需求和背景。用户是一名资深聚变等离子体物理与工程专家，所以问题可能比较深入，需要详细的理论分析和计算。
-问题分为两部分：第一部分是讨论ECCD在控制NTM中的应用原理，第二部分是估算所需ECCD驱动电流ICD的大小，并解释如何通过调整发射镜角度控制ECCD的功率沉积位置。
-首先，关于ECCD的应用原理，我应该回忆ECCD的基本概念。ECCD是通过注入高能量的微波，使电子发生回旋运动，从而在等离子体中产生电流。这个电流可以用来稳定或者抑制撕裂模。NTM是一种不稳定性，会形成磁岛，影响聚变反应的稳定性。ECCD可以通过在磁岛附近产生电流，提供一个外部电流扰动，从而稳定磁岛。
-接下来，我需要解释ECCD如何影响NTM。这可能涉及到电流扰动与磁岛结构的相互作用。关键参数包括电流密度、磁场强度和ECCD注入的位置。可能需要使用安培环定理或相关的磁流体力学方程来分析。
-然后是估算ICD的大小。问题中给出了磁岛宽度W，位置r，安全因子q。这些参数需要结合起来，通过某种模型或公式进行估算。可能需要引入电流密度与磁岛宽度的关系，或者利用ECCD的效率和注入功率来计算。
-关于发射镜角度调整，这是工程上的问题。发射镜的角度决定了微波束的注入方向，从而控制ECCD产生的电流的位置。调整角度可以改变ECCD的沉积位置，使其更接近磁岛，提高控制效果。这部分需要解释角度与功率沉积的关系，可能涉及到光束的折射、反射以及在等离子体中的传播特性。
-在思考过程中，我可能会考虑以下几点：
-1. ECCD的基本物理机制：电子回旋共振、电流生成。
-2. NTM的形成和不稳定性：磁岛的产生、安全因子q的作用。
-3. 电流扰动对NTM的影响：如何通过外部电流改变磁流结构。
-4. 计算ICD的公式：可能需要查找相关文献或标准模型，确保计算的准确性。
-5. 发射镜角度调整的技术细节：角度变化如何影响注入位置，可能涉及的控制方法和诊断工具。
-可能需要做一些假设，例如磁岛的几何形状、ECCD的效率系数等，这些假设会影响最终的结果，所以在回答时需要明确指出这些假设。
-另外，工程或实验意义部分需要强调ECCD在聚变装置中的实际应用价值，比如如何通过精确控制电流来维持等离子体的稳定性，提升聚变反应的效率和安全性。
-最后，总结部分需要简明扼要地重申关键结论，确保用户能够快速抓住重点。
-在实际回答时，需要按照用户提供的规范，分步骤详细解答，确保每一步都有清晰的逻辑和理论支持，同时提供定量的估算和具体的工程意义分析。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 电子回旋电流驱动（ECCD）通过在新经典撕裂模（NTM）产生的磁岛附近产生定向电流，能够有效抑制或稳定NTM。估算所需ECCD驱动电流 `ICD` 的大小时，考虑磁岛宽度 `W`、位置 `r` 和安全因子 `q` 等参数，调整发射镜角度可以实现ECCD功率在等离子体内的精确沉积。
 ---
 ### 背景与概念  
@@ -8144,7 +7052,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -8170,19 +7078,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>嗯，我现在要解释离子回旋共振加热（ICRH）中的少数离子加热机制和模式转换加热机制，以及ICRH天线的设计和与等离子体耦合的主要问题。首先，我需要回忆一下ICRH的基本原理。
-ICRH是一种通过射频波将能量传递给等离子体离子的加热方法。射频波的频率接近离子的回旋频率，从而引发共振，使离子吸收能量。然而，在托卡马克等离子体中，通常存在多种离子，如氘、氚和可能的杂质离子。因此，ICRH可能有两种不同的加热机制：少数离子加热和模式转换加热。
-少数离子加热机制：当射频波的频率与某种离子的回旋频率匹配时，这种离子作为少数离子被加热。例如，在以氘为主要燃料的等离子体中，少量的氚离子可能会被加热。这通常发生在重离子的情况下，因为它们的回旋频率较低，更容易被射频波捕获。
-模式转换加热机制：当射频波在等离子体边界区域遇到某种条件时，波的模式会发生转换，从而将能量传递给不同种类的离子。例如，快波（X波）可能在边界转换为慢波（O波），从而加热更多的离子种群，包括主要离子。
-接下来，关于ICRH天线的设计和与等离子体的耦合问题，主要物理和工程挑战包括：
-1. 阻抗匹配：天线需要在宽频率范围内与等离子体阻抗匹配，以确保高效能量传输。
-2. 温度和等离子体参数变化：等离子体温度和密度的变化会影响天线的性能，需要动态调整。
-3. 杂质产生：天线材料在高能粒子冲击下可能释放杂质，影响等离子体的纯净度。
-4. 鞘层效应：天线表面的电子积累可能导致射频波的反射，降低耦合效率。
-5. 结构稳定性：天线需要在高温、高辐射环境中保持结构完整性。
-总结一下，ICRH利用射频波加热离子，通过少数离子和模式转换机制实现能量传递。天线设计和耦合面临匹配、动态调整、杂质、鞘层效应和结构稳定等挑战。
-&lt;/think&gt;
-### 1. 离子回旋共振加热（ICRH）中的少数离子加热机制和模式转换加热机制解释
+          <t>### 1. 离子回旋共振加热（ICRH）中的少数离子加热机制和模式转换加热机制解释
 #### 1.1 少数离子加热机制
 **机制描述**  
 ICRH中的少数离子加热机制是指射频波与等离子体中某种较少的离子物种（例如氘或氚）发生回旋共振。当射频波的频率接近少数离子的回旋频率时，这些离子通过捕获波的能量而被加热。
@@ -8236,7 +7132,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -8262,14 +7158,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>嗯，我现在要回答关于低杂波电流驱动（LHCD）的问题。首先，我需要理解LHCD的物理原理。LHCD是一种利用低杂波来驱动等离子体电流的技术，这在托卡马克装置中非常重要。
-我记得低杂波指的是频率较低的波，可能在几十兆赫兹左右。这些波是如何与等离子体相互作用的呢？应该是通过某种波-粒子相互作用机制，比如共振吸收。等离子体中的离子或电子可能以特定的频率与波发生共振，导致动量传递，从而产生电流。
-接下来，为什么在等离子体边缘区域或低温下LHCD的效率更高呢？可能是因为在这些区域，等离子体参数更容易满足波的共振条件。边缘区域的密度较低，温度也较低，这可能使得波能够更有效地与离子相互作用，而核心区的高温和高密度可能让波的行为不同，影响驱动效率。
-然后，讨论LHCD在托卡马克稳态运行和电流剖面控制中的作用。稳态运行需要持续的电流驱动，而LHCD可以提供这种驱动，帮助维持等离子体的形状和稳定性。在电流剖面控制方面，LHCD可能用于调整q剖面，比如在边缘区域增加电流，从而控制锯齿振荡或其他不稳定性。
-局限性方面，LHCD可能在高密度或高温条件下效率降低，因为这些条件可能改变了波的传播和吸收特性。此外，驱动电流可能受到波的传输和功率沉积的限制，难以均匀分布在整个等离子体中。这些限制可能影响LHCD在不同运行条件下的适用性。
-总结一下，LHCD通过波-粒子相互作用驱动电流，在边缘和低温下效率高，因为这些区域更容易满足共振条件。在托卡马克中，它用于稳态运行和电流剖面控制，但在高密度或高温下效率降低，这是其局限性。
-&lt;/think&gt;
-### 低杂波电流驱动（LHCD）的物理原理及应用
+          <t>### 低杂波电流驱动（LHCD）的物理原理及应用
 #### 核心结论
 低杂波电流驱动（LHCD）通过波-粒子相互作用驱动等离子体电流，在等离子体边缘区域或低温下效率较高，因其在这些条件下更易实现波与离子的共振。LHCD在托卡马克稳态运行和电流剖面控制中具有重要作用，但其效率受限于等离子体参数。
 ---
@@ -8315,7 +7204,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -8341,15 +7230,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>好，我现在需要回答关于阿尔芬波加热的问题。用户想知道阿尔芬波加热的基本概念，快阿尔芬波和慢阿尔芬波的传播和吸收特性有何不同，以及它在未来聚变装置中的潜在优势。
-首先，我得回忆一下阿尔芬波的基本知识。阿尔芬波是磁化等离子体中的一种横波，由磁张力驱动。我记得它们在托卡马克等装置中有应用，用于加热和电流驱动。
-接下来，区分快阿尔芬波和慢阿尔芬波。快阿尔芬波应该是指速度较快的那部分，而慢的可能涉及到离子回旋运动。可能在传播特性上，快波需要满足特定的平行相速度条件，而慢波则与离子回旋频率有关。
-关于传播和吸收特性，快阿尔芬波通常传播在较大的半径范围内，可能在梯度较强的区域更容易吸收，转化为热能和电流。而慢阿尔芬波可能在较低速的区域传播，吸收可能涉及更复杂的动理学过程，可能和离子回旋运动有关。
-然后，考虑它们在聚变装置中的潜在优势。阿尔芬波加热的优势可能包括高效的电流驱动，减少对超导线圈的依赖，同时提供非感应加热，可能减少杂质和流扰动的问题。未来装置如ITER可能受益于这种加热方法，因为它可以在高密度下操作，并有助于实现稳态运行。
-现在，我需要把这些点组织成规范的回答，确保涵盖所有部分：核心结论、背景概念、机理分析、工程意义等。可能需要查阅一些资料来确保准确性，比如快波和慢波的传播条件和吸收机制的具体差异。
-最后，要点总结要简洁明了，强调阿尔芬波加热的优势及其在聚变装置中的应用前景。
-&lt;/think&gt;
-### 阿尔芬波加热的基本概念
+          <t>### 阿尔芬波加热的基本概念
 **核心结论**  
 阿尔芬波加热是利用磁化等离子体中的阿尔芬波将能量传递给等离子体粒子的加热方法。
 **背景与概念**  
@@ -8379,7 +7260,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -8405,16 +7286,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>嗯，我现在要回答关于电子伯恩斯坦波（EBW）加热的问题，特别是它与传统电子回旋谐波加热（ECRH）相比在高密度或过密等离子体中的优势。首先，我得理解EBW和ECRH的基本原理，以及它们在不同等离子体条件下的表现。
-电子回旋谐波加热（ECRH）是一种常用的等离子体加热方法，它利用高频电磁波与等离子体中的电子发生共振，将其加热。ECRH通常适用于低到中等密度的等离子体，因为当密度增加时，电子回旋频率降低，需要更高的频率来保持共振。然而，随着密度继续增加，ECRH的有效性可能会受到限制，因为波的传播特性可能会改变，或者波无法有效地传递能量到等离子体中。
-电子伯恩斯坦波（EBW）则是另一种波加热方法，它利用的是电子伯恩斯坦模式的波。这种波在高密度等离子体中更容易传播，因为它们不需要像ECRH那样高的频率来维持共振。EBW可以在更高的密度下有效地传输能量到等离子体，这可能使其在高密度或过密等离子体中更具优势。
-接下来，我需要详细分析EBW的原理。EBW是一种可以同时传播在电子回旋频率和电子声学频率之间的波。与ECRH不同，EBW不需要严格的频率匹配，因为它们能够在较宽的频率范围内传播。这意味着即使在密度变化的情况下，EBW仍然可以有效地将能量传递到等离子体中，而不需要频繁调整频率。
-此外，EBW在高密度等离子体中的传播特性也有所不同。由于波的传播依赖于密度梯度，EBW可能在高密度区域更容易传播，而ECRH可能因为波反射或模式转换而导致能量损失。因此，在高密度条件下，EBW可能更高效地将能量传输到等离子体的核心，从而提高加热效果。
-另一个需要考虑的因素是波的吸收和能量传递机制。ECRH主要通过电子回旋吸收，这在低密度下效果很好，但在高密度下，由于电子运动速度的增加，吸收效率可能下降。而EBW由于其波的传播和吸收机制的不同，可能在高密度下仍然保持较高的吸收效率，从而提供更有效的加热。
-此外，EBW可能在过密等离子体中提供更好的稳定性。过密等离子体可能会导致其他加热方法如ECRH出现波反射或其他不稳定现象，而EBW可能因为其波的模式特性，避免这些问题，从而提供更稳定的加热效果。
-综上所述，EBW在高密度和过密等离子体中相对于ECRH的优势主要体现在更高的传播效率、更好的能量吸收以及更稳定的加热过程。这些优势使得EBW成为一种有潜力的等离子体加热方法，尤其是在未来的聚变装置中，如托卡马克和仿星器，这些装置可能需要在高密度条件下运行以实现高效的聚变反应。
-&lt;/think&gt;
-### 核心结论
+          <t>### 核心结论
 电子伯恩斯坦波（EBW）加热是一种在高密度或过密等离子体中更为有效的等离子体加热方法，相较于传统电子回旋谐波加热（ECRH），其优势体现在更高的传播效率、更好的能量吸收以及更稳定的加热过程。
 ### 背景与概念
 等离子体加热是聚变反应堆研究中的关键环节，电子回旋谐波加热（ECRH）是一种广泛应用的方法，但其效率在高密度条件下会显著降低。电子伯恩斯坦波（EBW）加热则利用了电子伯恩斯坦模式的波，能够在更高的密度下更有效地传输能量到等离子体。
@@ -8432,7 +7304,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -8458,20 +7330,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>好的，我现在需要回答关于未来聚变电站，如DEMO，对等离子体加热与电流驱动系统的总体要求，特别是效率、可靠性、可维护性和与氚增殖包层的兼容性方面。
-首先，我应该明确问题的核心，也就是DEMO等未来聚变电站的需求。这意味着我要考虑实际应用中的各种限制和技术要求。
-核心结论方面，我应该总结出加热与驱动系统必须高效、可靠、易于维护，并且能够与氚增殖包层兼容。这一点需要在回答中突出。
-接下来，背景与概念部分需要解释聚变电站的基本结构，特别是等离子体加热和电流驱动系统的角色。要提到常用的加热方法，如中性束注入、射频波加热，以及电流驱动技术，如偏滤器等离子体自举电流。还要定义关键指标，比如效率（WPE）、可用性、维护性，以及兼容性。
-在原理与推导部分，我需要详细解释每种加热和驱动方法的物理机制，以及它们如何影响效率。例如，中性束注入的效率可能受到能量损失的影响，而射频波加热则需要考虑波的传播和吸收效率。电流驱动部分则需要分析自举电流的产生条件和限制，以及外部驱动的补充作用。
-定量估算部分，我可以引用一些典型参数，比如中性束的效率大约在40%到60%，射频波加热可能在50%到80%之间。同时，系统可用性目标可能设定在90%以上，这需要考虑设备的可靠性和维护周期。
-工程或实验意义方面，我需要指出这些设计对实际装置的影响，比如设备的耐辐射能力、诊断系统的开发、材料选择，以及维护策略。这些都是实际工程中必须考虑的因素。
-比较与拓展部分，我应该比较不同加热和驱动方法的优缺点。例如，中性束注入效率高但成本高，射频波加热成本较低但效率可能受到等离子体参数的限制。偏滤器电流驱动虽然高效，但可能需要复杂的磁轭设计，而外部驱动则需要额外的电源系统支持。
-最后，要点总结需要重申最重要的信息，比如高效率、可靠性、易于维护和兼容性是设计的关键，同时指出未来发展的方向和挑战。
-在整个思考过程中，我需要确保逻辑清晰，各部分内容之间有良好的衔接，并且每个部分都提供足够的细节来支持结论。同时，要注意使用正确的物理术语和单位，避免混淆。如果某些信息不够明确，可能需要做出合理的假设，并在回答中注明。
-现在，我需要将这些思考过程组织成一个结构化的回答，按照用户提供的规范进行。这包括使用小标题、项目符号，以及适当的方程和单位。确保每个部分都覆盖到问题的各个方面，同时保持严谨和客观。
-总的来说，我需要全面分析DEMO等聚变电站对加热与驱动系统的要求，从背景、原理、估算、工程意义、比较到总结，每个部分都要深入且详细，确保回答既全面又有深度。
-&lt;/think&gt;
-### 对DEMO等未来聚变电站加热与电流驱动系统的总体要求
+          <t>### 对DEMO等未来聚变电站加热与电流驱动系统的总体要求
 #### 1. **核心结论**
 未来聚变电站（如DEMO）的等离子体加热与电流驱动系统必须具备高效率（wall-plug efficiency, WPE）、高可靠性、良好的可维护性，并与氚增殖包层实现兼容。
 ---
@@ -8522,7 +7381,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -8548,16 +7407,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>嗯，用户问的是关于不同加热和电流驱动方法的协同效应，具体怎么组合使用NBI、ECRH和ICRH来优化等离子体的温度、密度和电流剖面。首先，我得理解这些方法各自的特点。
-NBI主要是通过注入高能中性束，与等离子体发生核聚变反应，加热离子，同时还能驱动电流。它的优点是离子加热效率高，适合在离子回旋频率附近操作，所以在托卡马克的高密度区域效果好。但是，过强的NBI可能会让边缘温度太高，甚至导致等离子体不稳定，比如边缘局域模（ELMs）的触发。
-ECRH是通过微波或毫米波加热电子，通常用于高密度区域，因为它不容易被等离子体吸收。它还能通过下加热来控制杂质的分布，减少杂质污染。不过，ECRH对密度的限制比较敏感，高密度下效果可能下降。
-ICRH是通过低频波加热离子，适用于较低密度的区域，可以帮助加热离子并驱动电流。它的加热效率可能比NBI低，但适合不同的等离子体条件。
-协同效应方面，可能需要NBI负责主要的离子加热和电流驱动，ECRH处理电子加热和杂质控制，ICRH在低密度区域辅助加热。这样组合的话，可以在不同区域优化温度和电流分布，避免单一方法的不足。
-在设计组合策略时，需要考虑等离子体各区域的特性，比如中心和边缘的密度差异。可能需要动态调整各方法的功率分配，以应对等离子体的变化。此外，还要注意各方法的相互影响，比如NBI可能加剧边缘加热，影响ECRH的效果，所以需要协调它们的功率和频率。
-工程上，可能需要优化波的频率和功率，确保各加热方法的有效性。诊断方面，需要实时监测温度、密度和电流的变化，及时调整策略。这种综合控制不仅能提高聚变效率，还能减少不稳定性，对装置运行非常重要。
-总的来说，协同使用这三种方法，各取所长，互补所短，可以在复杂的等离子体环境中实现更好的控制。不过，具体实施还需要根据实验结果不断调整和优化。
-&lt;/think&gt;
-### 1. **核心结论**  
+          <t>### 1. **核心结论**  
 NBI（中性束注入）、ECRH（电子回旋谐波加热）和ICRH（离子回旋谐波加热）的协同使用可以通过优化功率分配和频率选择，实现对等离子体温度、密度和电流剖面的综合控制，从而提升等离子体性能和稳定性。
 ---
 ### 2. **背景与概念**  
@@ -8610,7 +7460,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -8636,17 +7486,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，我现在需要分析高功率波加热系统中的关键技术部件在长脉冲、强辐射聚变环境下面临的材料和工程挑战。首先，我得明确这些系统包括ECRH和ICRH，它们用于托卡马克装置中，比如ITER。这些系统的关键部件有大功率源、传输线、真空窗和发射天线。每个部件可能面临不同的挑战，我需要逐一分析。
-首先是大功率源，这通常指的是微波源，比如 gyrotrons 或者 klystrons。它们在高频下产生高功率，长时间运行会产生大量的热量，如何有效冷却是个问题。同时，高频微波管的阴极和其他部件可能会受到电子轰击，导致材料疲劳或失效。此外，这些源需要高真空环境，长时间运行可能会有漏气的问题，影响性能。
-接下来是传输线，它们负责将微波从源传输到天线。传输线需要处理高功率，可能会有热载荷，导致结构变形或材料损坏。金属部件可能在高频下产生涡流，导致额外的发热。此外，传输线与真空窗之间的连接处可能在热循环下出现应力，导致密封失效，影响整个系统的真空环境。
-真空窗是一个关键部分，因为它隔离了高真空的聚变装置和大气环境。长脉冲运行意味着真空窗需要承受持续的热载荷，可能导致材料退化甚至破裂。此外，真空窗可能会受到微波的反射，影响传输效率，导致额外的加热。同时，材料的长期稳定性也是问题，因为聚变环境中可能有辐射影响材料性能。
-发射天线负责将微波耦合到等离子体中。在强辐射环境下，天线表面可能会受到等离子体杂质的侵蚀。此外，天线可能需要处理反射波，长时间的高功率反射可能导致天线过热或结构损坏。天线的几何形状和材料选择对于高效耦合也很重要，设计不当会影响加热效果。
-从材料角度来看，这些部件需要耐高温、高强度、高导电性和高导热性的材料。例如，钼和碳纤维增强陶瓷在高温下表现良好，但可能在某些情况下容易破裂。此外，抗氧化性能也很重要，因为高温下材料容易氧化，影响寿命。
-工程设计方面，冷却系统的设计至关重要。高效的冷却可以带走热量，防止部件过热。同时，结构设计需要考虑热膨胀和振动，避免因应力集中导致的部件损坏。接口设计，如真空窗和传输线的连接处，需要确保密封性，防止漏气。
-诊断和监测技术也是必不可少的。实时监测温度、应力和振动可以帮助预测故障，及时进行维护。此外，冗余设计可以提高系统的可靠性，减少因单个部件故障导致整个系统停机的风险。
-最后，未来的发展方向可能包括新型材料的研究，如高温超导材料，以及智能控制系统的发展，以优化运行参数并延长部件寿命。总的来说，这些技术挑战需要多学科的合作，包括材料科学、热力学、电磁学和结构工程，才能找到有效的解决方案。
-&lt;/think&gt;
-### 分析高功率波加热系统（如ECRH、ICRH）中关键技术部件在长脉冲、强辐射聚变环境下面临的材料和工程挑战
+          <t>### 分析高功率波加热系统（如ECRH、ICRH）中关键技术部件在长脉冲、强辐射聚变环境下面临的材料和工程挑战
 #### 核心结论
 高功率波加热系统的关键部件在长脉冲、强辐射条件下面临显著的热、机械和材料挑战，需采用耐高温、抗辐射、高导热和结构稳定的材料，配合高效冷却和精确设计以确保长期可靠性。
 #### 背景与概念
@@ -8746,7 +7586,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -8772,18 +7612,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>好，我现在要详细描述等离子体与壁相互作用（PMI）中的主要物理过程，包括物理溅射、化学溅射、热升华、反射、吸附、再沉积和氢同位素滞留。并说明这些过程如何影响等离子体性能和PFC寿命。嗯，首先，我得弄清楚每个过程的基本概念和它们在PMI中的作用。
-首先，物理溅射。这应该是等离子体中的高能粒子，比如离子或者电子，轰击壁材料，导致材料原子被溅射出来。这些溅射出来的粒子会进入等离子体，改变等离子体的成分，可能增加杂质，影响等离子体的稳定性和能量 confinement。
-接下来是化学溅射。这可能涉及等离子体中的氢同位素与壁材料的化学反应。例如，氘或氚与碳或金属壁反应，生成化合物，这些化合物随后会进入等离子体，可能释放更多的杂质，同时导致壁材料的腐蚀，缩短PFC的寿命。
-热升华，应该是壁材料在高温下直接从固态转化为气态的过程。这种情况下，壁材料的原子或分子进入等离子体，同样会带来杂质，影响等离子体的性能，同时也会消耗壁材料，降低PFC的寿命。
-反射，这可能是指等离子体中的中性粒子或离子被壁反射回等离子体。这部分会影响等离子体的密度分布，可能在边缘区域形成密度的积累，影响边界等离子体的稳定性，可能引发边缘放电问题，比如边缘模式或者等离子体失控。
-吸附，指的是壁材料表面捕获等离子体中的粒子。这个过程可以减少等离子体中的杂质浓度，因为这些粒子被吸附在壁上，而不是留在等离子体中。但是，吸附的物质在后续的等离子体运行中可能重新释放，导致再沉积或其他问题。
-再沉积，是指被溅射或升华的壁材料在其他地方重新沉积，可能是在等离子体中的其他区域或者冷却的PFC表面。这可能导致局部区域的壁材料堆积，影响热传导和结构完整性，同时可能改变等离子体中的杂质分布，影响整体的等离子体行为。
-氢同位素滞留，这涉及到等离子体中的氘、氚等轻元素与壁材料的相互作用，可能包括渗透、吸附和捕获。这些同位素可能在壁中保留较长时间，这不仅会影响等离子体的燃料补充，还可能导致氚的损失，影响聚变反应的效率，同时也可能增加氚的库存管理难度。
-这些过程对等离子体性能的影响包括引入杂质，影响等离子体的稳定性、能量 confinement 和粒子输运。例如，物理和化学溅射带来的杂质会增加辐射损失，降低能量 confinement，从而影响聚变反应的效率。同时，这些过程也会直接影响PFC的寿命，因为溅射和升华导致壁材料的损失，而再沉积和滞留可能导致结构问题和氚的损失。
-接下来，我需要整理这些思考，按照结构化的回答规范来组织内容，确保每个部分都涵盖核心结论、背景与概念、过程分析、影响等各个方面，同时保持逻辑清晰和信息准确。
-&lt;/think&gt;
-**等离子体与壁相互作用（PMI）中的主要物理过程及其影响**
+          <t>**等离子体与壁相互作用（PMI）中的主要物理过程及其影响**
 **1. 核心结论**
 等离子体与壁相互作用（PMI）涉及多种物理过程，如溅射、升华、反射、吸附、再沉积和同位素滞留，这些过程显著影响等离子体性能和第一壁寿命，需综合考虑以优化聚变装置设计。
 ---
@@ -8845,7 +7674,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -8871,14 +7700,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>嗯，今天有个问题需要解决，关于托卡马克偏滤器的热负荷估算。首先，我得理解问题是什么。用户给了总加热功率是100MW，其中50%通过偏滤器排出，也就是50MW。然后，这些功率主要沉积在内外靶板上，总面积是4平方米。那问题就是要算出靶板承受的平均稳态热负荷，还要讨论为什么实际的峰值可能比这个平均值高很多。
-好，首先，我得明确一下什么是热负荷。热负荷通常指的是单位面积上接收到的功率，单位是W/m²。所以，这里总的功率是50MW，面积是4m²，那平均下来应该是50,000,000W / 4m² = 12,500,000 W/m²，也就是1.25e7 W/m²。这应该是平均值。
-但是，用户还问了为什么实际峰值会比这个平均值高。这可能是因为在实际运行中，热量并不是均匀分布在靶板上的。比如，等离子体可能在某些区域集中放电，或者流体运动导致某些点的热流密度特别高。此外，偏滤器的几何形状也可能导致某些区域更容易积累热量，或者冷却系统可能在某些点不够有效，从而导致局部过热。
-再想想，可能还有其他因素，比如等离子体的不稳定状态，比如磁岛或者边缘放电，这些都会导致局部区域的热流密度急剧增加。此外，靶板的材料可能会影响热传导，如果材料导热不好，热量会在局部区域堆积，导致温度上升更快。
-还有，控制系统的响应时间也可能影响峰值热负荷。如果等离子体状态变化很快，而冷却系统反应不够迅速，可能会导致局部过热。这些都是可能的原因。
-所以，总结一下，平均值是1.25e7 W/m²，而实际峰值可能高达平均值的几倍甚至十几倍，主要因为热量分布不均匀，局部区域承受了更大的热流密度。
-&lt;/think&gt;
-### 偏滤器的主要功能
+          <t>### 偏滤器的主要功能
 托卡马克偏滤器的主要功能是通过磁流体动力学（MHD）效应引导和排出等离子体中的杂质、热量及粒子流，同时保护壁面免受高热流的直接冲击。偏滤器在托卡马克装置中扮演着**热排出**、**杂质控制**及**等离子体约束优化**的重要角色。
 ---
 ### 平均稳态热负荷估算
@@ -8933,7 +7755,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -8959,15 +7781,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>嗯，我现在需要分析钨（W）、铍（Be）和碳（C）基材料作为聚变装置第一壁或偏滤器材料的优缺点，并解释为什么ITER最初选择铍，后来改为钨。
-首先，我应该分别了解这三种材料的基本物理和工程特性。钨是一种高熔点金属，铍也是金属，但铍比较轻，碳则通常是石墨形式。
-铍的优点可能包括低原子序数，这有助于减少中子的慢化，适合在聚变反应中使用。同时，铍的中子俘获截面低，所以不会过多吸收中子，而且铍在中子辐照下生成的氚可能有限。但铍的问题是辐照肿胀，也就是在高能粒子的冲击下，材料会发生体积膨胀，这可能会影响结构的稳定性。此外，铍的高温性能可能不如钨，容易在高温下发生蠕变。
-碳基材料，尤其是石墨，优点是高温下非常稳定，不会发生融化，而且可以承受很高的温度。石墨的中子俘获截面也较低，但会随着辐照时间逐渐变脆，发生辐照损伤。此外，石墨中的碳可能会与等离子体中的氢发生化学反应，导致材料的侵蚀。
-钨的优点是非常高的熔点，抗高温性能优异，而且在高温下不容易发生蠕变。钨的高熔点可以承受更高的热负荷，这对聚变装置的高热流区域非常重要。此外，钨的辐照性能相对较好，虽然辐照肿胀问题依然存在，但可能比铍和碳基材料更稳定。但钨的缺点是原子序数高，可能会导致更多的中子慢化，对聚变反应的效率有影响。另外，钨的加工成本可能比较高，因为钨是一种较重的元素，提炼和制造钨部件可能较为复杂和昂贵。
-ITER最初选择铍作为第一壁材料，可能是因为铍的低原子序数和较低的中子俘获截面，有利于聚变反应的中子管理。然而，后续改为钨可能是因为在运行中发现铍在高热负荷和高能粒子辐照下的性能不如预期，特别是辐照肿胀和蠕变的问题导致结构可靠性下降。而钨的高熔点和抗高温性能更适合ITER长期运行的需求，特别是在更高的热负荷和粒子辐照条件下，钨能够提供更好的结构稳定性和寿命。
-总结来说，铍在初始设计中被选中是因为其中子物理性能优异，但后续改为钨是因为在实际运行中发现钨在高温和辐照下的性能更可靠，尽管钨在中子管理方面可能稍逊一筹，但综合性能更符合ITER的需求。
-&lt;/think&gt;
-### 钨（W）、铍（Be）和碳（C）基材料作为聚变装置第一壁或偏滤器材料的优缺点比较
+          <t>### 钨（W）、铍（Be）和碳（C）基材料作为聚变装置第一壁或偏滤器材料的优缺点比较
 #### 钨（W）材料
 - **优点**：
   - 高熔点（3422°C），在极端高温环境下具有优异的稳定性。
@@ -9010,7 +7824,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -9036,14 +7850,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>嗯，用户问的是脱靶运行模式的物理机制以及它对降低偏滤器靶板热负荷和粒子通量的意义，还有实现稳态脱靶运行面临的挑战。首先，我得确定用户的知识背景，应该是聚变等离子体物理或相关工程领域的人，可能在做相关研究或设计。
-脱靶运行模式，我记得是托卡马克装置中的一种偏滤器配置。目标是让等离子体与靶板分离，这样热负荷和粒子通量就能降低。那背后的物理机制是什么呢？应该是通过调整偏滤器的磁拓扑结构，让等离子体在边缘区域形成一个低温、低密度的区域，避免直接撞击靶板。这可能涉及到三维磁效应，比如皮尔斯钉扎或者自组织结构。
-接下来，意义部分。降低热负荷和粒子通量对材料寿命很重要，因为偏滤器材料在高热流下容易损坏。脱靶运行还能减少溅射，延长运行时间，提高聚变装置的效率和经济性。
-挑战方面，我想到的第一个问题是维持稳态。脱靶运行需要精确控制等离子体参数，比如密度和温度，否则容易回到靶板模式。其次，如何避免新的问题，比如等离子体在分离区域的不稳定性或杂质积累。还有，系统的诊断需要非常精确，能够实时监测等离子体的状态，这对诊断技术提出了更高的要求。
-另外，脱靶运行可能依赖于特定的装置配置，比如特殊的偏滤器结构或磁场控制，这可能增加了装置设计的复杂性。同时，操作人员需要掌握更复杂的控制策略，这对运行团队来说也是一个挑战。
-总的来说，脱靶运行模式在理论上很有优势，但在实际应用中需要克服不少技术和控制上的难题。需要进一步研究和实验来验证和优化这些方法，确保长期稳定运行。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 脱靶运行模式通过在偏滤器靶板附近形成一个分离的低温等离子体层，减少了热负荷和粒子通量对靶板的直接冲击。但实现稳态脱靶运行需要克服等离子体稳定性、分离层维持和边界控制等技术挑战。
 ---
 ### 背景与概念  
@@ -9085,7 +7892,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -9111,17 +7918,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>嗯，我现在需要讨论聚变堆第一壁材料（PFC）的腐蚀、迁移和再沉积问题，以及这些过程如何导致混合材料层的形成和氚的共沉积。同时，还要考虑如何通过原位诊断来监测PFC表面状态的演化。让我一步一步地分析这个问题。
-首先，我需要明确什么是PFC材料。PFC是指聚变堆的第一壁材料，通常面临高温、高能粒子轰击等极端条件，这可能导致材料发生腐蚀、迁移和再沉积。这些过程会影响材料的性能，进而影响聚变堆的运行。
-接下来，腐蚀部分。腐蚀主要是由于高能粒子（如氢同位素）与材料表面的相互作用导致的。当氘或氚离子轰击材料时，可能会导致材料中的原子被溅射出来，这种过程叫做溅射。溅射会导致材料逐渐失去质量，即腐蚀。此外，高温和辐照也可能导致材料发生化学反应，进一步引起腐蚀。
-然后是迁移和再沉积。溅射出来的原子或者离子可能会在聚变堆的其他区域重新沉积，形成新的材料层，这就是再沉积。迁移指的是这些原子在聚变堆中的运动，可能在表面扩散或者进入其他材料中。这个过程可能形成混合材料层，因为不同材料的原子会混合在一起。例如，如果PFC材料是金属，而周围的材料是碳基的，那么溅射出的金属原子可能会在碳基材料表面沉积，形成金属-碳的混合层。
-关于氚的共沉积，氚是聚变反应的重要燃料之一，但它也是一个活泼的元素，容易与其他材料发生反应。在再沉积过程中，可能有氚被携带并沉积在材料表面，形成含有氚的共沉积层。这种共沉积层可能会影响聚变堆的性能，比如改变材料的热传导性能，或者在极端情况下，可能释放氚，影响聚变堆的安全性和运行效率。
-接下来，如何通过原位诊断监测PFC表面状态的演化？这里需要考虑几种可能的诊断方法。首先，表面分析技术如俄歇电子能谱（AES）或X射线光电子能谱（XPS）可以用来分析材料表面的组成和结构。这些技术可以在实验室内使用，但是否适合聚变堆的极端环境呢？这可能需要进一步的考虑。
-其次，中子和γ射线诊断技术可以用来检测氚的分布和含量。例如，中子测厚法可以用来监测材料层的厚度变化，而γ射线成像可以提供材料表面的分布情况。此外，微波诊断技术可能用于监测材料表面的温度和状态变化，而激光诱导击穿光谱（LIBS）可以用于检测材料的组成变化。
-不过，这些诊断方法是否适合在聚变堆运行的高温、高辐照环境中使用呢？可能需要开发适应极端环境的传感器和诊断设备。此外，这些方法是否能够实时、快速地监测材料状态的变化，也是一个需要考虑的问题。
-总结一下，PFC材料的腐蚀、迁移和再沉积会导致混合材料层的形成，并且可能伴随氚的共沉积，影响聚变堆的性能和安全。要监测这些变化，需要结合多种诊断技术，可能需要在现有方法的基础上进行改进和优化，以适应聚变堆的运行条件。
-&lt;/think&gt;
-聚变堆第一壁材料（PFC）的腐蚀、迁移和再沉积是一个复杂的过程，影响着聚变堆的性能和安全。以下是对此问题的详细分析和解决方案：
+          <t>聚变堆第一壁材料（PFC）的腐蚀、迁移和再沉积是一个复杂的过程，影响着聚变堆的性能和安全。以下是对此问题的详细分析和解决方案：
 ### 腐蚀、迁移和再沉积的影响
 1. **腐蚀过程**：
    - 高能粒子（如氘、氚离子）轰击PFC材料，导致溅射现象，材料失去质量。
@@ -9152,7 +7949,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -9178,17 +7975,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>嗯，我现在要回答的问题是关于高Z杂质进入聚变等离子体芯部的影响，以及偏滤器在杂质屏蔽和氦排出中的作用，还要讨论杂质输运的物理机制。这看起来是一个比较专业的聚变物理问题，我需要仔细梳理一下。
-首先，高Z杂质，比如钨，对等离子体有什么负面影响呢？我记得高Z杂质的原子序数较高，可能会与等离子体发生强烈的相互作用。可能的影响包括辐射损失增加，因为高Z原子在高温下会辐射大量能量，这会降低等离子体的温度，影响聚变反应的效率。另外，高Z杂质的迁移率较低，容易在芯部积累，导致杂质浓度升高，进一步恶化辐射损失。
-接下来，偏滤器的作用是什么呢？我知道偏滤器是聚变装置中的一个关键部件，用于排出聚变反应产生的氦灰，并且尽量减少杂质进入等离子体芯部。偏滤器通过其结构设计，比如强磁场区域，使得杂质被引导到特定的区域，而不是进入等离子体的核心。这样可以减少杂质对等离子体性能的负面影响。同时，偏滤器还能帮助排出氦，这可能是因为氦的扩散特性较好，偏滤器的结构能够促进氦的排出。
-然后是杂质输运的物理机制。杂质的输运涉及多种物理过程，包括等离子体流、梯度引起的扩散、波动导致的运输等。在高Z杂质的情况下，它们的迁移率较低，可能更容易被特定的运输机制控制，比如径向电场驱动的流输运或者磁流体动力学（MHD）波动引起的运输。这些过程会影响杂质在等离子体中的分布，进而影响整体的等离子体性能。
-在思考这些内容时，我需要确保每个部分都有足够的科学依据。比如，关于高Z杂质的辐射损失，是否真的会导致等离子体的冷却？查阅相关资料，发现确实如此，高Z杂质原子在高温下会释放大量辐射，这会带走等离子体的能量，使温度下降，从而抑制聚变反应。
-关于偏滤器的作用，我需要明确它是如何屏蔽杂质的。偏滤器通常位于等离子体的外围，利用磁场结构引导杂质和不想要的粒子流向特定的收集板，这样就可以减少它们进入等离子体芯部的可能性。而氦的排出可能与偏滤器的几何形状和磁场配置有关，设计良好的偏滤器可以有效促进氦的排出，保持等离子体的清洁。
-在讨论杂质输运的物理机制时，我需要考虑不同的输运模型，比如标准扩散模型、流输运模型以及由于波动引起的非扩散输运。对于高Z杂质来说，可能还涉及到它们与等离子体相互作用的特殊性，比如较重的原子可能更容易被静电场或磁场捕获，从而影响其输运路径。
-此外，我还需要注意杂质浓度梯度的影响。浓度梯度会驱动扩散，而磁场的存在会改变这种扩散的方式，可能形成各向异性的输运特性。波动，如等离子体中的湍流，可能会增强输运，使杂质分布更加不均匀。
-总结一下，我需要分三个主要部分来回答问题：高Z杂质的影响、偏滤器的作用以及杂质输运的机制。每个部分都需要详细阐述，并且结合已知的物理知识和实验结果来支持结论。同时，要注意用规范的语言和结构，确保答案清晰易懂，符合用户的要求。
-&lt;/think&gt;
-### 高Z杂质进入等离子体芯部的不利影响
+          <t>### 高Z杂质进入等离子体芯部的不利影响
 #### 1. **核心结论**
 高Z杂质（如钨）进入等离子体芯部会导致等离子体辐射损失增加、热传导增强以及宏观稳定性降低，进而严重影响聚变反应的持续性和效率。
 #### 2. **背景与概念**
@@ -9245,7 +8032,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -9271,27 +8058,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>好的，我现在要解答的问题是关于液态金属作为偏滤器（PFCs）的潜在优势和面临的主要挑战。液态金属候选包括锂和锡。让我一步步分析。
-首先，核心结论：液态金属偏滤器在聚变装置中具有独特优势，但面临流体动力学、蒸发、材料兼容性和氚提取等挑战。
-背景与概念：PFCs在托卡马克中用于处理等离子体边缘和壁相互作用，包括降低热负荷、减少杂质进入等离子体。液态金属如锂和锡因其高导热性和低杂质特性，被视为潜在的PFC材料。关键参数包括热导率（W/m·K）、蒸气压（Pa）、熔点（°C）和与结构材料的兼容性。
-接下来，优势分析：
-1. 高导热性：液态金属如锂（95 W/m·K）和锡（69 W/m·K）的导热性优于石墨（约150 W/m·K，但常用于结构材料）。这有助于高效散热，降低表面温度，减少热负荷。
-2. 低杂质引入：液态金属在等离子体环境中蒸发或溅射时，释放的杂质较少，保持等离子体清洁，避免性能下降。
-3. 结构自愈性：液态金属可以在运行中重新流动，修复因运行产生的损伤或缺陷，提高使用寿命。
-4. 中子反应特性：锂（^6Li）可以与中子反应生成氚，支持聚变燃料循环；锡对中子的吸收较少，可能减少核反应活性，但需进一步评估。
-然后，主要挑战：
-1. MHD效应：液态金属具有导电性，会在磁场中产生MHD效应，导致流体流动不稳定，可能影响等离子体性能和结构稳定性。需要进行MHD模拟和实验研究。
-2. 蒸发与腐蚀：在高温等离子体环境中，液态金属可能发生蒸发或气化，导致材料损失和杂质进入等离子体。需要评估蒸发速率和采用适当的冷却系统。
-3. 材料兼容性：液态金属可能与结构材料（如不锈钢或钨）发生化学反应或物理侵蚀，影响长期使用和装置可靠性。需要测试不同结构材料的兼容性。
-4. 氚提取与控制：锂在中子辐照下生成氚，需要有效的氚提取和控制系统，避免氚的积累和泄漏，同时确保聚变燃料的自持循环。
-定量估算或示例：
-假设液态锂的表面温度为200°C，环境蒸气压为10^-6 Pa，使用蒸发速率公式，估算蒸发速率。这有助于设计冷却系统和材料保护措施。
-工程或实验意义：液态金属PFCs的研究和应用对聚变装置的性能和可靠性有重要意义。工程设计需要考虑材料选择、冷却系统优化、MHD效应控制和氚管理系统的设计。
-比较与拓展：
-其他候选材料如钨基材料具有高熔点，但导热性不如液态金属，且易引入杂质。液态金属材料在某些方面更优，但在MHD效应和材料兼容性方面需要进一步研究。
-要点总结：液态金属PFCs在聚变装置中有显著优势，但需克服MHD效应、蒸发、材料兼容性和氚控制等挑战。未来研究应侧重实验验证和优化设计，以评估其在实际装置中的可行性。
-&lt;/think&gt;
-### 液态金属作为PFCs的潜在优势和挑战
+          <t>### 液态金属作为PFCs的潜在优势和挑战
 #### 核心结论
 液态金属（如锂、锡）作为偏滤器（PFCs）在聚变装置中具有优异的热性能和杂质控制潜力，但面临复杂的流动稳定性、材料兼容性、氚提取和蒸发损失等挑战。
 #### 背景与概念
@@ -9330,7 +8097,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -9356,19 +8123,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，我现在需要讨论DEMO反应堆的偏滤器设计和材料选择上需要哪些超越ITER的革新。首先，我应该回忆一下偏滤器在托卡马克中的作用，主要是用于排出等离子体中的杂质和热量，同时处理高能粒子流带来的热负荷。
-DEMO的目标是比ITER更接近商用，所以它会面临更高的热负荷和更强烈的中子辐照。ITER的热负荷可能在每平方米几百千瓦左右，而DEMO可能会高几个数量级，达到每平方米几兆瓦甚至更高。中子辐照也会更严重，因为DEMO的运行时间更长，功率更高，产生的中子更多，对材料的辐照损伤会更显著。
-在设计上，我想DEMO可能需要更高效的热排出系统。可能需要采用主动冷却结构，比如使用液态金属冷却或者更好的传热材料。同时，结构设计可能需要更复杂的几何形状，以优化流道，提高冷却效率，避免热点的产生。
-材料方面，ITER可能使用的材料如W（钨）或者合金，但在DEMO中，这些材料可能不足以应对更高的热负荷和辐照。因此，可能需要开发新的耐高温、高辐照的材料。比如，添加某些微量元素的合金，或者陶瓷基复合材料，这些材料可能在高温下强度更好，辐照损伤更小。另外，材料的抗氧化性能也很重要，因为高温下材料容易氧化，影响使用寿命。
-系统集成也是一个挑战。偏滤器不仅要处理高热流，还要与等离子体控制、诊断系统、维护系统等集成。因此，设计时需要考虑整体的兼容性和可维护性。可能需要模块化设计，便于更换和维修。
-此外，还需要考虑中子辐照带来的材料肿胀、性能退化等问题。可能需要进行更深入的辐照实验，了解材料在不同辐照剂量下的表现，从而选择最适合的材料。
-总结一下，DEMO的偏滤器设计和材料选择需要在以下几个方面超越ITER：
-1. 高效热排出系统：更高的冷却能力和结构优化。
-2. 耐用材料：能够承受更高热负荷和辐照损伤的新材料。
-3. 系统集成：与其他系统兼容，便于维护和操作。
-可能需要进一步研究和实验，特别是材料的辐照性能和热力学性能，以确保DEMO的长期稳定运行。
-&lt;/think&gt;
-为了应对DEMO反应堆中偏滤器面临的挑战，设计和材料选择需要在以下几个方面进行革新：
+          <t>为了应对DEMO反应堆中偏滤器面临的挑战，设计和材料选择需要在以下几个方面进行革新：
 1. **高效热排出系统**：
    - **主动冷却结构**：采用液态金属冷却或其他高效传热材料，提高冷却效率。
    - **优化几何设计**：复杂的流道设计，确保均匀散热，避免热点。
@@ -9387,7 +8142,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -9413,16 +8168,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>好吧，我现在要解决的问题是解释PFCs上的瞬态热事件，比如ELMs和破裂，如何导致材料熔化、蒸发和开裂，以及如何设计PFCs以提高其耐受性。首先，我得弄清楚PFCs是什么，ELMs又是什么。
-PFCs，全称是Primary First Wall，是托卡马克装置中直接与高温等离子体接触的部分。它们不仅要承受极高的温度，还要承受等离子体产生的各种瞬态热事件，比如边缘局部模态（ELMs）。ELMs是一种瞬时的高热流现象，发生在托卡马克的边界区域，当等离子体边界不稳定时，会突然释放大量能量，导致PFCs表面温度急剧上升。
-接下来，我需要理解这些瞬态热事件如何导致材料的熔化、蒸发和开裂。当ELMs发生时，PFCs表面会受到非常高的热流密度，可能在短时间内达到数百万瓦每平方米。这种剧烈的加热会导致材料温度迅速升高，超过其熔点，从而引起局部熔化。如果热量继续集中，材料可能会进一步蒸发。同时，快速的温度变化会导致材料内部产生热应力，当应力超过材料的极限时，就会发生开裂。
-现在，思考如何设计PFCs来提高耐受性。首先，可能需要选择熔点高、导热性能好的材料，这样即使在高热流下，也能更好地分散热量，避免局部过热。比如 tungsten 是一种常用材料，因为它熔点高，但在某些情况下可能会脆性断裂，所以可能需要与其他材料结合使用，如铜，以提高导热性。
-其次，结构设计也很重要。可以采用多层结构，将高熔点材料作为外层，内部有高导热材料，这样可以迅速将热量导出，避免积累。另外，优化冷却系统，比如使用更高效的冷却回路，增加冷却剂的流速，或者采用先进冷却技术如液态金属冷却，可能有助于更有效地带走热量。
-表面处理也是一个方面。如果表面有纹理或特殊涂层，可能改变等离子体的行为，减少热流密度。例如，表面微结构可能促进等离子体的稳定，或者在ELMs发生时分散热流，减少局部过热的风险。
-另外，监测和控制也很关键。实时监测PFCs的温度和应力，可以在异常事件发生时及时调整等离子体参数，降低热负荷。同时，控制ELMs的频率和强度，比如通过射频波或其他控制手段，减少它们对PFCs的影响。
-总的来说，设计PFCs需要综合考虑材料选择、结构优化、冷却系统、表面处理和监测控制等多个方面，以提高其对瞬态热事件的耐受性，从而确保聚变装置的安全和可靠性。
-&lt;/think&gt;
-### 瞬态热事件对PFCs材料的影响
+          <t>### 瞬态热事件对PFCs材料的影响
 1. **核心结论**
 瞬态热事件如ELMs和破裂通过极高的局部热流密度导致PFCs材料的熔化、蒸发和开裂，严重威胁聚变装置的安全运行。
 2. **背景与概念**
@@ -9463,7 +8209,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -9489,15 +8235,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，我现在需要讨论PFCs产生的灰尘对聚变装置安全运行的潜在风险，以及如何监测和控制这些灰尘。首先，我得理解PFCs是什么，它们在托卡马克中的作用，以及为什么会产生灰尘。
-PFCs是第一壁的防护部件，用来吸收等离子体的高热流。在聚变反应中，等离子体温度极高，所以PFCs很容易受到溅射和侵蚀，导致材料颗粒脱落，也就是灰尘。这些灰尘会对装置造成严重威胁，比如爆炸、氚扩散和冷却剂通道堵塞。
-接下来，我需要分析这些风险的具体表现。首先是爆炸风险。等离子体中的高能粒子可能会点燃碳颗粒，引发爆炸。其次是氚扩散。碳颗粒可能吸附氚，导致氚在装置内扩散，增加安全风险。最后是冷却剂通道堵塞。如果灰尘进入冷却系统，可能会堵塞通道，导致过热甚至损坏设备。
-然后，我要思考如何监测和控制这些灰尘。监测方面，可能需要使用气溶胶检测器来监测气相中的颗粒浓度，或者用核聚变分析来检测氚的含量。控制方面，可以通过优化材料、改善几何结构和使用吹扫系统来减少灰尘的产生。此外，设计有效的排尘系统，比如喷嘴或过滤器，也能帮助清除现有的灰尘。
-在具体措施上，我应该建议使用非碳材料，如 tungsten 或 beryllium，因为它们产生的碳颗粒较少。改进PFCs的几何设计，比如增加凸起或凹槽，可以引导颗粒排出，减少堆积。此外，吹扫系统可以使用气体或磁场来清除颗粒，降低它们在装置内积累的可能性。
-我还需要考虑可能的监测和控制方案的优缺点。比如，非碳材料虽然减少碳颗粒，但可能更难制造或成本更高。改进几何设计可能增加复杂性，需要更精确的制造工艺。吹扫系统则需要额外的资源，如气体供应和控制系统，可能增加装置的复杂性。
-最后，我需要总结这些措施，强调综合运用这些方法可以有效控制灰尘水平，提高聚变装置的安全性和可靠性。
-&lt;/think&gt;
-### 1. 核心结论
+          <t>### 1. 核心结论
 PFCs（等离子体与壁相互作用部件）产生的灰尘（dust）主要由碳颗粒组成，其在聚变装置中可能引发爆炸、氚扩散及冷却剂通道堵塞等安全隐患。通过优化PFC材料、设计吹扫系统、安装气溶胶检测器等措施，可有效监测和控制装置内灰尘水平。
 ---
 ### 2. 背景与概念
@@ -9594,7 +8332,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -9620,16 +8358,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于14 MeV的D-T聚变中子与材料相互作用的主要物理过程，特别是原子位移级联和嬗变反应，尤其是He和H的产生。同时，还要比较这种现象与裂变堆中子辐照效应的不同之处。这个问题看起来挺复杂的，但我想我可以一步步拆解来分析。
-首先，我需要明确D-T聚变中子的能量和来源。D-T聚变通常发生在托卡马克等聚变装置中，产生的中子能量为14 MeV，这比裂变堆中的中子能量要高得多。因为裂变堆中的中子通常是热中子，能量大约在0.025 eV左右。这个能量差异肯定会对材料相互作用产生不同的影响。
-接下来，我要考虑中子进入材料后的主要物理过程。中子与材料中原子核的相互作用主要有两种方式：弹性散射和非弹性散射。对于重核材料，比如钢或钨，中子在弹性散射中会传递较高的动量，导致靶核获得较大的动能，从而引发原子位移级联。而对于轻核材料，比如铍，中子可能在非弹性散射中产生单个原子位移，因为它们较轻，容易被弹出晶格位置。
-然后是嬗变反应，特别是He和H的产生。中子与材料中的原子核发生核反应，生成新的同位素。在D-T聚变中，中子的能量很高，容易引发高能核反应。例如，中子与硅-28反应可能生成磷-31和氦核，或者与铁-56反应生成钴-59和氢核。这些反应会产生He和H，累积后会导致材料性能的变化，比如肿胀和脆化。
-接下来，我需要比较这两种辐照效应的不同。裂变堆中的中子能量较低，通常分布在热中子区（~0.025 eV）到快中子区（~1 MeV），而聚变堆中的中子能量是14 MeV，属于超快中子区。这导致聚变中子的溅射阈值更高，能够产生更多的原子位移，导致更严重的材料损伤。此外，聚变中子的平均自由程更短，意味着它们在材料中的穿透深度更小，集中在表面附近，这也增加了材料的表面损伤风险。
-另外，聚变中子引发的嬗变反应速率通常高于裂变堆，因为它们的高能量更容易打破束缚核的力。因此，He和H的生成率更高，材料更容易发生肿胀和辐照蠕变。
-我还想到，用户可能是在设计聚变装置时考虑材料选择，所以需要明确不同材料在不同辐照条件下的表现。例如，轻核材料在聚变辐照下可能更适合，因为它们较少产生位移损伤，但在裂变辐照下可能更容易产生嬗变产物。
-总结一下，我的思考过程包括：理解问题背景，分析中子与材料的相互作用过程，比较两种辐照效应的区别，最后考虑这些分析对聚变装置设计的意义。这样可以帮助用户更好地理解材料在聚变环境中的行为，从而做出更合适的选择。
-&lt;/think&gt;
-### 1. **核心结论**  
+          <t>### 1. **核心结论**  
 14 MeV D-T聚变中子与材料相互作用的主要物理过程包括原子位移级联和嬗变反应（如生成He和H）。这些过程与裂变堆中子辐照效应的显著区别在于聚变中子的高能量导致更高的原子位移效率和更显著的轻元素生成。
 ---
 ### 2. **背景与概念**  
@@ -9681,7 +8410,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -9707,13 +8436,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>嗯，用户问的是辐照引起的材料肿胀和辐照蠕变的微观机制，以及它们对聚变堆部件的影响。首先，我得回忆一下这些现象的基本原理。辐照肿胀通常是因为在材料中植入了大量He气泡，而辐照蠕变可能涉及到点缺陷的运动或He气泡的迁移。
-用户可能是一位聚变工程的学生或者研究人员，他们需要理解这些现象如何影响部件的尺寸稳定性和结构完整性。这可能涉及到材料的选择、设计以及维护策略。
-接下来，我需要分解这两个现象。对于辐照肿胀，高能粒子在材料中产生缺陷，然后捕获He原子形成气泡。这些气泡聚集会导致材料体积膨胀，影响几何尺寸。而辐照蠕变则是因为辐照产生的缺陷导致材料在无外力作用下发生变形，这可能破坏结构完整性。
-我还需要考虑材料中的位错和其他缺陷结构如何移动，以及这些移动如何导致材料变形。这可能涉及到辐照条件下材料的微观结构变化。
-最后，要确保回答结构清晰，使用用户要求的格式，每个部分都要涵盖背景、原理、影响等，同时保持语言严谨客观。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 辐照引起的材料肿胀和辐照蠕变是核聚变堆材料在高能粒子辐照下常见的损伤现象。肿胀由氦气泡形成和积累引起，而辐照蠕变则是辐照诱导的点缺陷和气泡迁移导致的材料变形。这些现象会降低聚变堆部件的尺寸稳定性和结构完整性，影响其长期运行性能。
 ---
 ### 背景与概念  
@@ -9755,7 +8478,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -9781,13 +8504,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>嗯，我现在需要回答关于氦脆的问题，特别是为什么氦脆在高温下更显著，以及这对聚变堆结构材料的温度上限有什么影响。首先，我应该明确氦脆是什么。氦脆是指在某些金属材料中，氦原子的积累导致材料脆性增加的现象。这通常发生在高温环境下，比如核反应堆或聚变堆中。
-接下来，我需要了解氦脆为什么会发生在高温下。这可能与金属在高温下的微观结构变化有关。高温通常会导致金属中的位错运动和扩散过程增加，这可能有助于氦原子在材料中的聚集。此外，高温下金属的晶格结构可能会变得更加不稳定，使得氦原子更容易被捕获或聚集在晶格缺陷处。
-然后，我需要思考氦脆对聚变堆结构材料工作温度上限的影响。聚变堆的工作环境通常涉及高温和高辐射，这会导致材料中积累大量氦原子。如果温度过高，氦脆效应会加剧，导致材料变脆，容易断裂，这对聚变堆的安全运行构成了威胁。因此，聚变堆的结构材料需要在较低的温度范围内工作，以避免氦脆的发生。
-另外，可能还有其他因素影响氦脆，比如材料的类型、氦的浓度以及辐照条件等。不同材料对氦的敏感性可能不同，因此在选择聚变堆结构材料时，需要考虑这些因素。同时，材料的微观结构设计，比如引入纳米级的强化相，可能有助于缓解氦脆效应。
-最后，我需要总结一下我的思考：氦脆在高温下更为显著，主要是因为高温促进了氦原子在材料中的扩散和聚集，导致材料变脆。这对聚变堆的结构材料工作温度提出了限制，需要在设计时考虑材料的耐高温和抗氦脆性能，以确保堆的安全运行。
-&lt;/think&gt;
-### 核心结论
+          <t>### 核心结论
 氦脆现象在高温下更为显著，因为高温加速了氦原子在金属晶格中的扩散和聚集。这限制了聚变堆结构材料的工作温度上限，通常要求低于约400°C，以避免材料脆化。
 ---
 ### 背景与概念
@@ -9836,7 +8553,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -9862,14 +8579,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>嗯，用户问的是关于低活化材料（LAMs）的问题，特别是在聚变能开发中的应用。我需要先理解什么是LAMs，以及它们为什么重要。接着，以RAFM为例，说明成分设计和活化元素的限制。
-首先，低活化材料主要是指在聚变反应中，材料受到中子辐照后产生的放射性较低。这很重要，因为聚变装置中的中子辐照会导致材料活化，产生放射性同位素，这对维护和废料处理带来挑战。
-背景方面，聚变反应堆尤其是托卡马克，如ITER和未来的DEMO，需要使用低活化材料来减少运行和退役时的辐射风险。材料中的特定元素，如Cr、Ni、Mo，容易捕获中子，生成长半衰期的放射性同位素，这些元素的控制是关键。
-接下来，RAFM是一种低活化钢，通过调整合金成分来减少这些活化元素。例如，Cr的含量通常控制在8%以下，以减少55Mn的活化。此外，使用高纯度原料去除Mo等杂质元素，进一步降低活化。
-工程意义方面，使用LAMs可以简化装置的维护，降低退役成本，同时提高装置的安全性和经济性。这也是未来聚变能大规模应用的重要前提。
-总结来说，用户可能是在学习聚变材料或设计相关装置，需要了解LAMs的基本概念、应用背景以及具体材料的成分设计。回答时要结构清晰，分点说明，用专业术语但保持易懂。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 低活化材料（Low Activation Materials, LAMs）是指在聚变中子辐照下产生的放射性水平较低的材料，是聚变能开发中不可或缺的关键材料。低活化铁素体/马氏体钢（Reduced Activation Ferritic/Martensitic steel, RAFM）通过限制关键活化元素的含量，显著降低了辐照后的放射性，是聚变堆候选材料之一。
 ---
 ### 背景与概念  
@@ -9911,7 +8621,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -9937,16 +8647,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>嗯，今天用户提了一个关于聚变堆候选结构材料的比较问题，我需要详细分析一下RAFM钢、ODS钢、钒基合金和碳化硅复合材料这几种材料的优缺点。首先，我得明确比较的几个方面：辐照性能、力学性能、工作温度、与冷却剂/增殖剂的兼容性，以及制造工艺。
-辐照性能方面，RAFM钢和ODS钢在高能中子辐照下都有较好的稳定性，因为它们都是合金，且添加了如钨这样的元素来增强性能。而钒基合金在这方面可能稍逊一筹，不过在高温下表现更好。碳化硅复合材料因为轻元素的缘故，辐照损伤相对较少，这点是个优势。
-力学性能方面，RAFM钢的高温蠕变强度好，ODS钢也有类似的优势。钒基合金在高温下的塑性和韧性不错，适合作为高温结构材料。碳化硅复合材料的高温力学性能好，不过脆性较大，这可能是个缺点。
-工作温度窗口上，RAFM钢通常在600°C以下，ODS钢可以到800°C，钒基合金适合在高温下使用，到800-1000°C，而碳化硅可以在更高的温度下工作，1200°C以上，但脆性问题可能限制其应用。
-与冷却剂/增殖剂的兼容性，RAFM钢和ODS钢与水和氦气都有不错的兼容性，适合各种冷却系统。钒基合金与水反应可能有问题，但与氦气相容性好。碳化硅对水基冷却剂可能腐蚀，但与氦气和液态金属相容。
-制造工艺方面，RAFM钢和ODS钢的生产相对成熟，成本较低，适合大规模应用。钒基合金因为难熔性，制造难度较高，成本也贵。碳化硅复合材料的生产复杂，成本高，大规模应用可能有挑战。
-总体来看，每种材料都有其适用场景。RAFM钢和ODS钢适合中等温度，辐照性能好，适合传统冷却系统。钒基合金适合高温，但制造成本高。碳化硅复合材料在高温下表现最好，但脆性问题和制造成本是障碍。
-在选择材料时，需要根据聚变堆的具体设计、工作条件和经济性来综合考虑。比如，如果温度要求高，可能选择碳化硅或钒基合金；如果更注重制造成本，可能选择RAFM钢或ODS钢。同时，材料在辐照下的性能也很重要，因为聚变反应会产生大量中子，影响材料的使用寿命。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 不同聚变堆候选结构材料在辐照性能、力学性能、工作温度窗口、与冷却剂/增殖剂兼容性以及制造工艺等方面各有优劣，RAFM钢和ODS钢适合中低温服役环境，钒基合金和碳化硅（SiC/SiC）复合材料适合高温环境。
 ---
 ### 背景与概念  
@@ -9998,7 +8699,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -10024,18 +8725,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>好吧，我现在需要解决的问题是关于聚变中子源缺失对材料研发的影响，以及如何利用现有设施模拟这种环境。作为一个刚开始接触这个领域的人来说，这个问题有点复杂，但我会尽力一步步分析。
-首先，我得理解聚变中子源是什么，以及它们在材料研发中的作用。聚变反应，比如氘氚反应，会产生高能中子。这些中子对材料的影响很大，因为它们会导致材料发生辐照损伤，比如晶体结构的变化、缺陷的产生等。所以，聚变中子源对测试和开发耐辐照材料至关重要。
-但现在，问题指出缺乏聚变中子源，这给材料研发带来了挑战。也就是说，现有的设施可能不足以模拟聚变环境中的中子辐照。那么，为什么会缺乏呢？可能是因为聚变反应堆还没有被大规模建设，或者现有的实验装置无法提供足够的中子通量和能量分布。
-接下来，我需要了解现有辐照设施有哪些，它们是如何模拟聚变中子环境的，以及这些模拟的局限性是什么。根据我所知道的，现有的设施包括裂变反应堆、离子束装置和散裂中子源。
-裂变反应堆产生中子的机制与聚变不同。裂变堆中的中子主要是由铀-235等核燃料裂变产生的，能量范围较广，但能量分布与聚变反应堆中的中子不同。聚变反应堆中的中子能量更高，主要集中在14MeV左右，而裂变堆中的中子能量较低，且能量分布更宽。因此，用裂变堆来模拟聚变中子辐照环境可能在中子能量和通量上无法完全匹配。
-离子束装置通常是用来产生高能离子轰击材料的，从而模拟辐照损伤。但这些离子通常是单一的，如氦离子或氢离子，它们的轰击能量和聚变中子不同。而且，离子束装置提供的辐照通量可能也与聚变反应堆中的不同。此外，离子束装置通常在较高温度下运行，而聚变材料可能需要在特定温度范围内测试。
-散裂中子源是通过高能质子轰击重核靶（如钨）产生的中子。这些中子的能量分布与聚变反应堆的中子不同，散裂中子源的中子能量可能更宽泛，且中子通量可能不如聚变反应堆高。此外，散裂中子源的运行方式通常是脉冲式的，这可能与聚变反应堆连续的中子辐照环境不同。
-那么，这些模拟方法的局限性是什么呢？裂变堆的主要局限性在于中子能量较低，能量分布不同，且可能缺乏足够的中子通量来模拟聚变环境。离子束装置的主要问题在于它们只能模拟特定类型的辐照损伤，无法全面反映中子辐照的影响。散裂中子源的问题在于中子能量分布不同，通量可能不足，以及脉冲运行与实际聚变环境的连续性不符。
-另外，我还应该考虑这些方法在实际应用中的可行性。例如，裂变堆虽然存在能量匹配问题，但其可用性强，可以进行长期辐照实验。而散裂中子源可能适合进行材料的结构变化研究，但不适用于长期辐照测试。
-综上所述，缺乏聚变中子源对材料研发的影响主要在于无法准确模拟聚变环境中的辐照条件。现有的模拟方法各有优缺点，但都无法完全复制聚变中子辐照环境。因此，为了克服这些挑战，可能需要结合多种辐照设施，进行多方面的测试和分析，同时加速聚变反应堆的建设，以提供真实的辐照环境进行材料测试。
-&lt;/think&gt;
-### 当前缺乏聚变中子源对聚变材料研发和认证带来的挑战
+          <t>### 当前缺乏聚变中子源对聚变材料研发和认证带来的挑战
 1. **核心结论**
    聚变中子源的缺失导致无法准确模拟聚变环境中的辐照条件，对材料研发和认证带来重大挑战。现有辐照设施虽能部分模拟，但各有局限性。
 2. **背景与概念**
@@ -10061,7 +8751,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -10087,14 +8777,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于辐照如何改变材料的韧脆转变温度（DBTT），以及这对聚变堆结构部件的影响。首先，我需要理解辐照效应和DBTT的基本概念。
-辐照效应指的是材料在高能粒子辐照下发生的一系列变化，可能导致材料性能退化。DBTT是材料从韧性变为脆性转变的温度，低于这个温度材料容易脆断。
-接下来，考虑辐照如何影响DBTT。高能粒子（如中子和离子）轰击材料时，会在晶格中产生缺陷，如空位和间隙原子，这些缺陷会导致材料硬化和脆化。由于缺口处更容易积累这些缺陷，缺口附近的强度增加，导致韧脆转变温度上升。这种变化会让材料在低温下更容易断裂，从而降低结构完整性。
-再来看聚变堆结构部件，尤其是启停和异常工况时，温度变化剧烈，容易导致热应力。如果材料的DBTT提高，材料在较低温度下变得脆性，可能在启停过程中因温度变化而发生脆性断裂，影响装置的安全运行。
-最后，需要考虑如何缓解这一问题。可能的措施包括选用耐辐照材料，优化结构设计以减少应力集中，以及采用先进材料处理技术提高材料的抗辐照性能。此外，定期监测材料状态，确保其在安全范围内运行也是必要的。
-综上所述，辐照效应导致DBTT升高，增加聚变堆结构部件在特定工况下的断裂风险，需要通过材料选择和设计优化等手段来应对。
-&lt;/think&gt;
-### 1. 核心结论
+          <t>### 1. 核心结论
 辐照通过引入缺陷和改变材料微观结构，显著提高材料的韧脆转变温度（DBTT），降低其韧性，从而对聚变堆结构部件的结构完整性造成不利影响。
 ---
 ### 2. 背景与概念
@@ -10139,7 +8822,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -10165,15 +8848,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，这个问题涉及到核聚变反应堆中的包层设计，特别是液态金属包层和结构材料之间的腐蚀与相容性问题。作为刚接触这个领域的学生，我需要先理解什么是液态金属包层，以及RAFM钢是什么。
-首先，液态金属包层通常使用铅锂合金（PbLi）作为冷却剂，因为它具有良好的热性能和中子慢化能力。然而，液态金属在高温下容易与结构材料发生反应，导致腐蚀问题。RAFM钢（Reduced Activation Ferritic/Martensitic steel）是一种被广泛研究的结构材料，因为它具有良好的高温强度和低活化特性。
-接下来，我需要了解液态金属与结构材料之间的腐蚀机制。可能的原因包括溶解腐蚀、电化学腐蚀以及机械损伤如流动加速腐蚀（FAC）。腐蚀会导致材料性能下降，甚至结构失效，这对核聚变反应堆的安全性构成威胁。
-为了缓解这些问题，材料选择、涂层技术和液态金属化学控制都是可行的方法。在材料选择方面，可能需要寻找与液态金属兼容性更好的钢种。涂层技术可以形成一个保护层，防止金属直接接触液态金属。此外，控制液态金属中的杂质浓度，比如去除氧气和水，可以减少腐蚀的发生。
-我还记得，氧和水是导致腐蚀的重要因素，因为它们会引发氧化反应。因此，液态金属的纯度管理至关重要。在涂层方面，可能需要选择具有良好热稳定性和化学稳定性的材料，如氧化物或陶瓷涂层。
-此外，涂层与基体材料的结合强度也是一个重要考虑因素，以防止涂层脱落。在选择液态金属时，除了PbLi合金，可能还需要探索其他合金成分，看看是否有更优的相容性。
-总结一下，腐蚀和相容性问题主要源于化学反应和物理损伤，解决方案需要综合材料科学、涂层技术和化学控制等多个领域的知识。在实际应用中，还需要通过实验验证这些方法的有效性，并优化工艺参数以达到最佳效果。
-&lt;/think&gt;
-**核心结论**：  
+          <t>**核心结论**：  
 液态金属（如铅锂）与结构材料（如RAFM钢）之间的腐蚀和相容性问题主要源于化学反应和物理损伤，可通过优化材料选择、涂层技术和化学控制来缓解。
 ---
 ### **背景与概念**  
@@ -10222,7 +8897,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -10248,20 +8923,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>好吧，我现在要仔细想一想用户的问题。用户问的是先进制造技术，特别是增材制造或3D打印，在聚变部件，尤其是复杂形状或多材料部件中的应用前景和挑战。另外，这些技术如何影响材料的微观结构和性能。
-首先，我得理解什么是增材制造。增材制造，也就是3D打印，是一种通过逐层添加材料来制造物体的技术。这与传统的减材制造不同，后者是从原材料中切割或雕刻出形状。增材制造的优势在于它可以制造传统方法难以实现的复杂结构，这对于聚变装置来说可能非常重要。
-聚变装置，尤其是托卡马克类型，比如国际热核实验堆ITER，其内部结构非常复杂，包括磁线圈、真空室、屏蔽结构等。这些部件通常需要承受极端的温度、高能粒子的冲击以及复杂的电磁环境。因此，制造这些部件需要高度的精确性和材料性能的优化。
-接下来，我要考虑增材制造在聚变部件中的应用前景。首先，复杂几何形状。聚变装置内部可能需要特定的冷却通道、支撑结构等，这些用传统方法可能难以实现，但增材制造可以轻松构造。其次，多材料部件，比如耐辐照材料和结构材料的结合，增材制造可以通过多材料打印技术实现，这可能减少接缝，提高整体性能。
-然后是挑战。首先是材料性能。增材制造过程中，材料的微观结构可能发生变化，比如晶体结构、孔隙率等，这会影响材料的强度、韧性和耐辐照性能。因此，如何保证增材制造的材料与传统制造的材料性能相当甚至更优是一个关键问题。
-其次是工艺控制。在极端工作环境下，聚变部件的制造需要极高的精确性和重复性。增材制造过程中，温度梯度、层与层之间的结合强度等因素都可能影响最终部件的性能，因此需要严格控制制造过程中的参数。
-还有成本和规模化生产的问题。虽然增材制造在原型制造和小批量生产中表现优异，但对于大型聚变装置来说，可能需要大量的部件，这时候增材制造的成本和时间效率是否能跟得上，也是一个挑战。
-接下来，思考增材制造对材料微观结构和性能的影响。增材制造通常涉及高能量束（激光或电子束）熔化粉末或线材，这会导致材料的快速加热和冷却，从而可能形成不同的晶体结构，比如更细小的晶粒，这可能提高材料的强度和韧性。但另一方面，快速冷却也可能导致微观应力和孔隙的形成，这可能降低材料的性能。
-另外，增材制造允许在材料内部构造复杂的冷却通道，这可以提高部件的冷却效率，从而延长部件寿命。这对于聚变装置中的第一壁等关键部件来说非常重要，因为它们需要承受极高的热负荷。
-再考虑工程或实验意义。应用增材制造技术可以显著缩短聚变装置部件的制造周期，减少材料浪费，同时提高部件的复杂性和性能。这对于未来聚变能的商业化应用具有重要意义。不过，这也需要对增材制造的材料性能进行深入研究和测试，以确保其在极端环境下的可靠性。
-最后，比较与拓展。增材制造与其他先进制造技术相比，如精密铸造、粉末冶金等，可能在复杂结构和多材料结合方面更具优势。但每种技术都有其适用的场景和局限性，可能需要根据具体部件的需求来选择最合适的技术。
-总结一下，增材制造在聚变部件制造中有很大的潜力，尤其是在复杂形状和多材料部件方面，但同时也面临材料性能、工艺控制和成本等方面的挑战。未来需要在这些方面进行深入研究和开发，以推动增材制造在聚变装置中的应用。
-&lt;/think&gt;
-### 1. **核心结论**  
+          <t>### 1. **核心结论**  
 增材制造（3D打印）在聚变部件制造中具有显著应用前景，尤其是在复杂几何形状和多材料部件方面，但需克服材料性能、工艺控制和成本等挑战。
 ---
 ### 2. **背景与概念**  
@@ -10302,7 +8964,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -10328,17 +8990,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>好的，我现在要回答关于聚变堆中除了结构材料之外，还需要哪些关键功能材料，以及它们各自面临的材料科学挑战。首先，我需要明确聚变堆的整体结构和各个部分的功能。聚变堆的核心是产生聚变反应的等离子体，外围则有各种系统支持这个过程。
-首先，诊断窗口的耐辐照光学材料。我知道在聚变堆中，诊断设备需要实时监测等离子体的状态，比如温度、密度等。这些诊断通常使用各种光学或热学方法，窗口材料需要能够透过这些诊断信号，同时承受聚变环境中强烈的辐射。因此，光学材料需要具备高透过率和抗辐照性能，但辐照可能导致材料结构变化，影响光学性能。
-接下来是用于绝缘的陶瓷材料。聚变堆中的磁体系统，特别是超导磁体，需要在低温环境中运行，陶瓷材料常用于支撑和绝缘这些系统。这些材料需要在极端低温下保持机械强度和绝缘性能，同时还要应对辐照的影响，避免性能下降。
-热沉材料，如铜合金，用于吸收和传导等离子体中的热量。聚变反应会产生大量能量，需要高效的热管理。铜合金虽然导热性好，但在高热负荷和辐照条件下，可能会发生性能退化，如微裂纹形成或组织变化，影响其长期稳定性。
-还有氚增殖材料，这对实现聚变堆的自持反应至关重要。材料需要在高温和高辐照条件下高效增殖氚，同时具备足够的热稳定性和抗辐照性能。目前常用的材料如Li2ZrO3和Li4SiO4，但它们在极端条件下的稳定性仍需进一步研究。
-辐射屏蔽材料也是关键，用于减少中子和高能粒子对人体和设备的影响。这些材料需要有高的中子捕获能力和足够的力学性能，同时在长期辐照下保持稳定。常用材料如铅和混凝土，但铅在极端条件下的行为可能需要进一步优化。
-此外，还有超导材料，用于制造强磁场，这对约束等离子体至关重要。超导材料需要在极低温下保持超导状态，并且在辐照环境下不发生退化。开发能在辐照下维持性能的超导材料是当前的研究重点。
-最后，先进包层材料，用于实现高效能量转换和氚循环。这些材料需要在高温、高辐照和强烈热冲击下稳定工作，这对材料的热性能、抗辐照性能和抗侵蚀能力提出了很高的要求。
-综上所述，每种功能材料都需要在特定条件下保持性能，同时克服辐照、极端温度和高热负荷带来的挑战。未来的研究需要结合实验、理论和模拟，开发出性能更优的新材料，以满足聚变堆的实际需求。
-&lt;/think&gt;
-### 聚变堆中的关键功能材料及其材料科学挑战
+          <t>### 聚变堆中的关键功能材料及其材料科学挑战
 #### 1. **核心结论**
 聚变堆除了结构材料外，还需要多种功能材料，包括耐辐照光学材料、绝缘陶瓷材料、高效热沉材料、氚增殖材料、辐射屏蔽材料、超导材料及先进包层材料，这些材料均面临独特的辐照损伤、极端环境适应性和长期稳定性等挑战。
 ---
@@ -10468,7 +9120,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -10494,20 +9146,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>嗯，今天老师布置了一个关于D-T聚变堆中氚自持必要性的问题，还有关于氚增殖的基本核反应原理，以及氚增殖比TBR的相关内容。我得好好想想怎么回答这个问题。首先，我得回忆一下D-T聚变反应的基本原理。
-D-T聚变，也就是氘和氚的聚变反应，生成氦-4和一个中子，并释放大量能量。这个反应的温度要求很高，通常需要在1亿摄氏度以上的等离子体中进行。但是，氚的供应问题一直是个难题，因为氚在自然界中非常稀少，而且它是放射性元素，半衰期大约12.3年。所以，如果聚变堆长期运行，氚的消耗速度会很快，必须找到一种持续的氚供应方式。
-氚自持的意思应该是聚变堆自己能够生成足够的氚来维持反应，而不需要外部不断补充。这听起来很重要，因为如果不能自持，氚的成本会很高，而且供应不稳定，可能会影响聚变堆的长期运行和商业化。
-接下来是氚增殖的基本核反应原理。我好像记得有几种反应，主要是中子与锂-6和锂-7的反应。中子打到锂-6上，会生成氚、氦-4和两个中子，对吧？而中子打到锂-7上，则生成氚、氦-4和一个中子。这两种反应都涉及到锂，因为锂在自然界中比较丰富，所以用锂来生产氚是一个可行的方法。
-那氚增殖比TBR是什么呢？应该是生成的氚与消耗的氚的比率。如果TBR等于1，说明生成的氚刚好等于消耗的，达到平衡。但实际中，TBR必须大于1，因为可能还会有氚的损失，比如泄漏到材料中或者被其他过程消耗。所以，TBR必须显著大于1，才能确保氚的自持。
-不过，这里有个问题，为什么TBR必须显著大于1，而不仅仅是稍微大一点呢？是不是因为实际运行中会有各种损失和效率问题？比如，中子在反应堆中的吸收效率可能不是100%，或者生成的氚可能有一部分没有被有效地收集回来。这些都会导致TBR需要更大的值来补偿这些损失，从而确保整体的氚供应是稳定的。
-另外，我还得考虑TBR对聚变堆设计的影响。如果TBR太小，可能需要更多的锂材料，或者更复杂的增殖系统，这会增加堆的设计难度和成本。因此，设计一个高效的氚增殖系统，提高TBR，是聚变堆实现商业化的重要因素。
-现在，我得把这些思路整理成一个结构化的回答，按照老师要求的格式来写。首先，核心结论要简明扼要，说明氚自持的重要性。然后，背景与概念部分要解释D-T反应和氚的稀缺性。接着，详细解释氚增殖的反应原理，然后定义TBR，并解释为什么它必须大于1。
-在原理与推导部分，我会列出相关的核反应方程，说明每个反应生成的氚量和中子数。然后，讨论TBR的计算公式，以及实际中为什么必须大于1的原因，比如中子损失和氚损失。
-定量估算部分，我可以举一个例子，假设一个聚变堆每秒消耗一定量的氚，而增殖系统生成更多的氚，计算TBR的值，并说明它必须大于1。这可能帮助读者更直观地理解。
-工程或实验意义方面，强调高效氚增殖系统的重要性，以及优化设计对降低成本和提高稳定性的帮助。比较与拓展部分，可以讨论其他可能的氚增殖方法，比如使用不同锂同位素或者其他元素，但目前来看，锂基的方法是最可行的。
-最后，要点总结要重申最关键的信息，比如氚自持的必要性、TBR必须大于1的原因，以及高效设计的重要性。这样整个回答就会结构清晰，内容全面，符合老师的要求了。
-&lt;/think&gt;
-### 阐述D-T聚变堆中氚自持的必要性以及氚增殖的基本原理
+          <t>### 阐述D-T聚变堆中氚自持的必要性以及氚增殖的基本原理
 #### 核心结论
 在D-T聚变堆中，氚的自持是实现可持续聚变反应的关键，因为氚在自然界中极其稀少且具有放射性。通过中子与锂-6和锂-7的核反应生成氚，可以实现氚的自给自足，而氚增殖比（TBR）必须显著大于1以补偿各种损失。
 ---
@@ -10561,7 +9200,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -10587,17 +9226,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>好的，我现在要比较固态和液态金属增殖剂包层在六个方面的优缺点。首先，我得回顾这两种包层的基本概念和设计目的。
-固态包层，比如HCPB和WCCB，通常使用固态材料，如铍和碳化硅作为增殖剂。这些材料在高温下稳定性较好，适合在较高温度下工作。而液态金属包层，如DCLL和WCLL，使用液态金属，如液态锂或锂铅合金，作为增殖剂，这类材料具有良好的流动性，能够更有效地吸收中子并传递热量。
-在氚增殖性能方面，液态金属包层可能有更好的增殖效率，因为液态金属的流动性和中子吸收能力较好。而固态包层的增殖效率可能稍低，但材料稳定性更高。
-氚提取方式上，固态包层可能需要物理手段，如机械破碎，来提取氚，而液态金属包层可以通过化学方法提取，效率更高，但系统可能更复杂。
-热工水力特性方面，液态金属包层由于流动性好，传热性能更好，但材料可能更难加工，且对结构材料的兼容性需要考虑。固态包层在材料兼容性和加工上可能更简单，但传热效率较低，可能需要更多的冷却系统设计。
-材料兼容性方面，液态金属与结构材料可能有腐蚀或反应问题，需要使用特殊材料，增加了成本和复杂性。而固态包层的材料兼容性较好，适合现有的材料技术。
-安全性方面，液态金属可能面临泄漏和流动控制的问题，增加了安全风险。固态包层在这方面可能更安全，但需要应对材料在极端条件下的性能问题。
-工程复杂度方面，液态金属包层由于需要循环流动系统，设计和维护更复杂，成本较高。而固态包层的结构简单，维护方便，但可能需要更大的尺寸和更高的运行温度。
-接下来，我需要逐一分析这些方面，结合各包层的具体设计，明确其优缺点，并确保结论的合理性。同时，要注意各部分的逻辑连贯，确保比较全面且准确。
-&lt;/think&gt;
-### 1. 核心结论  
+          <t>### 1. 核心结论  
 液态金属增殖剂包层（如DCLL）在氚增殖效率、热工水力特性方面更具优势，而固态增殖剂包层（如HCPB）在材料兼容性、安全性和工程复杂度上更具优势。
 ---
 ### 2. 背景与概念  
@@ -10682,7 +9311,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -10708,16 +9337,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>好，现在我来详细分析一下关于ITER实验包层模块（TBM）的问题。首先，我需要理解TBM的目标和主要内容。根据问题描述，ITER测试的TBM类型和从这些实验中获得的关键数据和经验，以支持DEMO包层的设计。这些问题都需要我回顾ITER的相关信息。
-首先，TBM的主要目标是测试下一代核聚变反应堆所需的氚增殖、热管理以及材料性能。具体来说，氚自给是一个关键目标，因为ITER本身并不具备氚的完全自给能力，所以TBM需要在这方面有所突破。其次，包层材料在高能中子和热负荷下的长期稳定性必须得到验证，以确保未来聚变堆的可靠运行。最后，热管理系统的设计和效率也是测试的重点，以确保包层能够有效散热，维持稳定的运行条件。
-接下来，主要内容包括设计、制造、安装和测试各种TBM原型，以及对实验结果的分析和反馈。这意味着ITER团队需要考虑不同的设计和技术，以确保全面的数据收集和验证。
-关于ITER测试的TBM类型，有三种主要的候选方案：基于固体 breeding blanket（比如Li4SiO4或Li2ZrO3）、基于液态金属（如Li或LiPb）以及基于气体（如He或He/CO2）的设计。每种类型都有其独特的优缺点，例如固体设计的稳定性和材料兼容性，液态金属的高效热传递和氚提取能力，以及气体系统的低活化性和易于维护。
-在获得关键数据和经验方面，有几个方面需要重点关注。首先是氚增殖效率和自给率，这直接影响聚变堆的可持续性。其次是材料的耐久性，特别是面对高能中子辐照和热机械应力时的性能。热管理系统的效果也至关重要，需要确保有效的散热和系统稳定性。
-从工程角度来看，TBM的成功将直接影响DEMO包层的设计和制造工艺。ITER测试的材料和系统将为DEMO提供实际的数据支持，帮助优化设计，提高可靠性和效率。此外，实验中获得的经验将指导未来的材料研发、系统集成和运行维护策略。
-在比较不同TBM设计时，固体、液态和气体方案各有优劣。固体方案在辐照稳定性和氚保留方面表现较好，但传热效率较低，可能需要更复杂的冷却系统。液态金属具有优异的导热性能和氚提取能力，但存在流动不稳定性的问题，且材料兼容性需进一步验证。气体方案则以低活化和易于维护为特点，但在氚增殖效率和热管理方面可能不如其他方案。
-总结来说，ITER的TBM测试是DEMO设计的重要基石。通过测试不同的概念，可以获得关键的实验数据和经验，从而优化包层设计，确保其在高能中子和极端热环境下的长期稳定性和效率。
-&lt;/think&gt;
-### ITER实验包层模块（TBM）计划的目标和主要内容
+          <t>### ITER实验包层模块（TBM）计划的目标和主要内容
 #### 1. **核心结论**
 ITER的实验包层模块（TBM）计划旨在测试氚增殖、热管理和材料耐受性，为未来的DEMO聚变堆提供关键数据和经验。
 #### 2. **背景与概念**
@@ -10741,7 +9361,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -10767,13 +9387,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>好的，我现在要回答关于中子倍增剂在氚增殖包层中的作用和必要性，以及使用铍作为倍增剂存在的材料和安全问题，还有是否有替代材料方案的问题。首先，我需要明确中子倍增剂的作用，这涉及到聚变反应和氚的增殖过程。
-中子倍增剂的主要作用是将聚变产生的中子能量降低，使它们能够被包层中的氚增殖材料有效利用。铍是一种常用的倍增剂，因为它对中子有很高的散射截面，能够有效减速中子。这有助于提高氚增殖效率，确保聚变反应的持续进行。
-接下来，我需要考虑使用铍作为倍增剂带来的材料和安全问题。首先，铍的辐照肿胀问题，高能中子的长期辐照会导致材料肿胀，影响包层的结构完整性。其次，铍在高温和辐照条件下的机械性能下降，可能导致材料失效。此外，铍金属的毒性也是一个重大问题，无论是粉尘还是蒸气都对人体和环境有严重危害，这增加了处理和废物管理的难度。
-然后，我应该探讨替代材料的可能性。替代材料需要具备良好的中子减速性能，同时在辐照和高温下的稳定性更好，且毒性较低或无毒。可能的替代材料包括钛、锆、铪等，这些金属具有较高的中子散射能力，并且辐照性能优于铍。碳化硅（SiC）和碳纤维复合材料（CFRC）也是选项，它们不仅具有优良的辐照性能，还具有高熔点和良好的热稳定性，适合作为结构材料。
-最后，我需要综合这些信息，提出一个全面的回答，涵盖铍的作用、存在的问题以及替代材料的选择和理由。这需要在结构上清晰，逻辑上连贯，确保每个部分都有足够的依据和解释。
-&lt;/think&gt;
-### 中子倍增剂在氚增殖包层中的作用和必要性
+          <t>### 中子倍增剂在氚增殖包层中的作用和必要性
 **核心结论**：中子倍增剂（如铍）在氚增殖包层中起关键作用，通过减速聚变中子，提高氚增殖效率，同时解决氚自给问题，维持聚变反应的可持续性。
 **背景与概念**：在聚变反应堆中，尤其是托卡马克装置，氘氚（D-T）聚变反应释放出大量高能中子（约14 MeV）。这些中子需要被适当减速，以便在后续的核反应中生产氚。氚增殖包层通常由锂陶瓷材料构成，这些材料在吸收中子后会裂变生成氚。然而，直接利用高能中子会导致裂变效率低下，因此需要中子倍增剂来降低中子能量，使其更易于被锂陶瓷吸收。
 **原理与推导**：中子倍增剂通过与高能中子发生弹性或非弹性散射，逐步降低中子的能量。铍（Be）因其对中子的高散射截面和低吸收特性，成为常用的倍增剂。反应过程如下：
@@ -10820,7 +9434,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -10846,16 +9460,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>嗯，用户问的是关于HCPB包层的氚提取系统，包括原理、流程以及主要技术挑战。首先，我需要确认HCPB是什么，HCPB应该是氦冷 Pebble Bed，也就是使用氦气冷却的颗粒堆，这种结构常用于聚变反应堆的包层。
-接下来，氚提取系统的基本原理是什么？我知道，在聚变反应中，中子会和锂发生核反应，生成氚。所以，包层材料需要有足够的锂来捕捉中子并生成氚。HCPB通常使用锂化陶瓷颗粒，比如Li4SiO4或Li2ZrO3，这些材料在高温下能够释放氚。
-然后，氚是如何被提取出来的？我记得有个过程叫做“吹扫”，也就是用气体把氚吹出来。具体来说，氦气作为冷却剂，同时也会携带氚，通过吸附和解吸的过程。温度的变化会影响氚的吸附，高温下释放，低温下吸附。这可能涉及到一个循环系统，可能需要外部冷却设备，比如液氮冷却的冷阱，来捕获氚。
-现在，详细描述工艺流程。首先，HCPB包层在聚变反应中产生氚，然后用氦气作为载体将氚输送到收集系统。在收集系统中，可能有一个吸附床，当温度降低时，氚会被吸附在材料上，这样就可以从氦气中分离出来。然后，再升高温度，将氚从吸附床中释放出来，形成氚气体，供外部使用。
-然后，面临的技术挑战有哪些？氚的渗透是个大问题，HCPB的结构可能比较紧密，但中子通量很高，所以氚的生成量可能很大，如何有效地收集这些氚是一个挑战。提取效率也是一个关键因素，必须确保足够的效率，否则无法维持聚变反应所需的氚供应。
-另外，材料在高温下的稳定性也很重要，包层材料在长时间的高温和高辐射环境下是否会老化，影响氚的释放和收集。还有系统设计中的温度控制，需要精确控制各个部分的温度，以确保氚的正确释放和吸附。此外，系统的可靠性和寿命也至关重要，长时间运行的系统必须稳定，不能频繁出现故障。
-再想一想，可能还需要考虑氚的安全问题，因为氚是一种放射性物质，处理过程中必须确保安全，防止泄漏。此外，系统的成本和复杂性也是挑战，设计一个高效的氚提取系统可能会增加整体装置的复杂性，需要在性能和成本之间找到平衡。
-总结一下，HCPB包层的氚提取系统涉及生成、吹扫、收集等多个步骤，每个步骤都有其技术和工程上的难点。需要在材料选择、温度控制、系统设计等多个方面进行优化，才能实现高效、可靠和安全的氚提取。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 固态增殖剂包层（HCPB）的氚提取系统通过氦气吹扫和分阶段冷却实现氚的分离与收集。其主要技术挑战包括氚渗透效率、提取过程中的气体分离纯度以及系统长期运行的稳定性。
 ---
 ### 背景与概念  
@@ -10899,7 +9504,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -10925,14 +9530,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>嗯，我需要详细分析液态金属增殖剂包层中的氚提取技术，特别是真空渗透和气体吹扫的方法。首先，我要理解背景，液态金属如PbLi用于核聚变反应堆的增殖剂，因为它们能有效地生成氚。但是液态金属中氚的提取效率是个大问题，因为氚会溶解在其中。
-首先，真空渗透法。这是利用分压差来促使氚从液态金属中扩散出来。当周围压力降低时，氚的溶解度也会降低，从而促使氚从液态金属中释放出来。但问题在于，液态金属的表面张力大，流动性能差，这会影响气体的传递和扩散，导致提取效率不高。另外，液态金属在高温下会活化，容易与水或其他杂质反应，带来安全风险。
-接下来是气体吹扫法。这种方法通过在液态金属中通入惰性气体，如氦气，增加气液接触面积，促进氚的解析。氦气的高密度和低溶解度有利于高效吹扫。但同样，液态金属的高粘度和高密度会降低气体的扩散效率，可能需要施加压力来维持气体流动，这会增加系统的复杂性。
-然后是技术挑战。高效提取的关键在于如何提高气液接触效率。可能需要改进结构设计，比如增加换热面积或优化流动路径。另外，液态金属的腐蚀性也是一个问题，因为它们在高温下会腐蚀包层材料，影响长期运行的可靠性。此外，氚的高放射性要求所有设备必须具备极高的密封性能，防止泄漏，这对工程实现提出了很高的要求。
-在实际工程中，可能需要结合多种方法，比如真空渗透和吹扫同时使用，或者采用化学吸附的方式。还可以考虑提高操作温度，以降低液态金属的粘度，从而提高气体的扩散效率。但温度过高又会加剧材料的腐蚀问题，所以需要在效率和材料性能之间找到平衡。
-最后，未来可能的发展方向包括开发新型的氚提取材料和工艺，比如使用多孔介质或膜分离技术，以提高提取效率。此外，改进液态金属的性能，比如通过合金化降低其粘度和表面张力，也可能是一个有效的途径。总之，氚提取技术在液态金属包层中的应用面临诸多挑战，需要在材料、工艺和设计等多方面进行综合优化。
-&lt;/think&gt;
-### **液态金属增殖剂包层中的氚提取技术分析**
+          <t>### **液态金属增殖剂包层中的氚提取技术分析**
 #### **核心结论**
 液态金属增殖剂包层（如PbLi DCLL）中的氚提取主要依赖真空渗透和气体吹扫技术。真空渗透利用分压差驱动氚析出，而气体吹扫通过吹扫气体增加气液接触面积。工程实现面临液态金属高粘度、高表面张力和腐蚀性等挑战，需优化结构设计和材料选择以提高效率。
 ---
@@ -10993,7 +9591,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -11019,15 +9617,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于聚变堆氚工厂的主要组成部分及其功能，以及相关的关键技术和安全挑战。首先，我得确定用户可能是一位聚变能领域的研究人员或者学生，他们可能在学习或工作中需要深入了解氚工厂的结构和挑战。
-核心结论需要简洁明了，所以我会先概述氚工厂的重要性及其关键系统。接下来，背景与概念部分，我需要解释氚在聚变中的作用，以及氚工厂的基本任务，比如补充氚、处理杂质和安全存储。
-然后是原理与推导，这部分要详细描述每个系统的工作原理。比如，燃料清理系统如何去除杂质，可能需要介绍捕获器和离子泵的工作机制。同位素分离系统则涉及氢同位素分离技术，比如蒸馏或化学交换法。
-储存和输运系统方面，我需要讨论金属储氚罐的工作原理，以及如何在极端条件下安全输运氚。精准衡算系统则需要说明监测氚存量的技术，以及数据采集和分析的重要性。
-接下来是关键技术和安全挑战。这里我得列举氚增殖效率低、氚安全储存难、同位素分离能耗高、以及系统故障导致的安全风险。这些都是当前研究中的难点，需要详细说明每一点的影响和可能的解决方案。
-最后，工程或实验意义部分，要指出这些系统对聚变装置设计和运行的影响，比如如何优化材料选择、提高效率和确保安全。比较与拓展部分，可以简要提到其他氚供应方案，如核电厂提取，但目前聚变堆氚自持是主流方向。
-总结时，我会重申氚工厂的重要性和面临的挑战，强调其对聚变能发展的影响。整个思考过程中，我需要确保逻辑清晰，涵盖所有关键点，并用简洁的语言表达，让用户能够快速理解氚工厂的复杂性和重要性。
-&lt;/think&gt;
-### 聚变堆氚工厂的主要组成部分及其功能
+          <t>### 聚变堆氚工厂的主要组成部分及其功能
 #### 核心结论
 聚变堆氚工厂是实现核聚变能自持运行的关键系统，包含燃料清理、同位素分离、氚储存和输运以及氚的精确衡算四大主要功能，面临氚的高放射性、低丰度及极端储存条件等关键技术与安全挑战。
 #### 背景与概念
@@ -11073,7 +9663,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -11099,17 +9689,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，今天遇到了一个关于聚变堆氚清单的问题。我得先理清楚问题到底是什么，然后一步步解决。
-首先，用户问的是影响聚变堆整体氚清单的主要因素，包括包层滞留、PFC滞留、燃料循环系统滞留等。然后还要解释为什么最小化氚清单对安全性和经济性至关重要。看起来这是一个涉及聚变堆设计和氚管理的问题。
-我记得氚是聚变反应中的关键燃料，但它是放射性的，半衰期挺短的，大约12.3年。而且在聚变堆中，氚的循环利用效率很高，但还是会有一些损失，比如滞留在结构材料中或者燃料循环系统里。所以，分析这些滞留的原因和影响因素，然后解释为何减少这些滞留对聚变堆的运行很重要。
-首先，得理解什么是氚清单。氚清单是指聚变堆中氚的总存量，包括正在使用的和储存的。而滞留指的是氚在系统中的累积，这部分氚无法被有效利用，可能带来安全风险和经济负担。
-接下来，分析主要因素。首先是包层滞留，包层材料（如Li）在高温和高能中子辐照下会发生氚的滞留。这个滞留量可能与中子通量、材料厚度以及氚的释放机制有关。然后是PFC滞留，PFC（主要面向等离子体的部件，如 divertor）在高温和高能粒子冲击下，可能吸收氚。这部分滞留可能与材料的选择、表面温度、等离子体条件有关。最后是燃料循环系统的滞留，这部分涉及到系统中氚的循环效率，如果系统有泄漏或效率不高，也会导致氚的滞留。
-然后，为什么最小化氚清单重要呢？从安全性来说，氚是放射性的，滞留在系统中的氚如果发生泄漏，可能会带来辐射风险。此外，氚的管理和回收需要专门的设施，这可能会影响聚变堆的整体安全性。从经济性来看，氚资源比较匮乏，生产成本高，如果有很多氚滞留在系统中无法回收，会增加运营成本，降低经济性。此外，氚的循环效率直接影响到聚变堆的运行时间和经济可行性。
-现在，把这些思路整理成结构化的回答，按照用户给的规范来写。首先，核心结论，然后背景与概念，接着分析原理，定量估算，工程意义，比较与拓展，最后要点总结。
-可能需要假设一些典型参数，比如中子通量、材料厚度、释放系数等，来估算滞留量。同时，比较不同滞留因素的影响，指出哪个因素占主导地位。
-总的来说，回答需要涵盖各个因素的具体影响机制，给出定量估算，说明其对安全性和经济性的具体影响，最后总结出最小化氚清单的重要性。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 影响聚变堆氚清单的主要因素包括包层滞留、PFC（面向等离子体组件）滞留和燃料循环系统滞留。最小化氚清单对聚变堆的安全性和经济性至关重要，因为它能降低氚的潜在泄漏风险和资源消耗，同时提高燃料循环效率。
 ---
 ### 背景与概念  
@@ -11177,7 +9757,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -11203,19 +9783,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>嗯，今天有个问题需要讨论，就是关于实现DEMO氚自持（TBR &gt; 1.1 或更高）所面临的综合性挑战。用户指出了几个关键因素：包层覆盖率、中子泄漏、结构材料吸收、增殖剂富集度，以及氚提取和处理过程中的损失。作为聚变等离子体物理与工程专家，我需要详细分析这些问题，给出一个结构化的答案。
-首先，我得明确核心结论，也就是DEMO实现氚自持的主要挑战是什么。然后按照用户给的答题规范，分成七个部分来组织答案。接下来，我需要逐一分析每个因素，看看它们各自的影响和如何综合起来导致挑战。
-包层覆盖率，这显然是关键的。覆盖率越高，捕获的中子越多，生成的氚就越多。覆盖率不足的话，TBR自然就下降。那覆盖率如何计算呢？可能涉及包层的设计，比如环向和纵向的覆盖情况，还有结构材料的布局。
-中子泄漏也是个大问题。泄漏出去的中子无法参与氚的生成，反而增加屏蔽的需求，还可能引起其他问题。要分析泄漏的主要途径，可能是包层间隙或结构材料中的泄漏。中子的泄漏率计算可能涉及到几何因素和材料的中子吸收截面。
-结构材料吸收，这又是一个损失中子的因素。结构材料中的中子被捕获，无法用于增殖。这可能需要选择低吸收的结构材料，比如使用低活化钢或其他复合材料，但这样成本和工艺可能提高。
-增殖剂富集度，富集度越高，中子被吸收生成氚的概率越大。富集度不足可能导致TBR不够，所以可能需要高富集度的锂同位素。但富集过程本身需要资源和能源，成本可能很高。
-氚提取和处理过程中的损失，这部分损失可能包括化学处理中的损失、储存过程中的损失以及运输过程中的损失。这些环节的效率直接影响最终的氚产量。可能需要优化提取工艺，减少损失，提高回收率。
-接下来，我得将这些因素综合起来，分析它们对TBR的影响。例如，包层覆盖率和增殖剂富集度直接影响反应的效率，而中子泄漏和结构材料吸收则减少可用中子的数量。氚提取和处理的损失则影响最终的氚产量，这些都必须纳入综合考虑。
-在工程和实验意义上，可能需要提高包层覆盖率，优化结构设计，选择合适的材料，提高增殖剂的富集度，改进氚处理工艺等。这些措施可以共同提升TBR，帮助DEMO实现氚自持。
-最后，比较与拓展部分，可能需要讨论不同设计方案的优缺点，比如全陶瓷包层和模块化设计的比较。不同设计方案在成本、复杂度和效率上各有优劣，需要根据具体情况选择合适的设计。
-总的来说，实现氚自持是一个复杂的系统工程，需要在多个方面进行优化和协调。每个因素都可能影响最终的TBR，必须综合考虑，找到一个平衡点，才能使DEMO成功实现氚自持。
-&lt;/think&gt;
-### 核心结论
+          <t>### 核心结论
 DEMO实现氚自持（TBR &gt; 1.1 或更高）面临多重复杂挑战，包括中子捕获效率、增殖剂循环处理、结构材料设计以及氚提取损失等综合因素，需通过优化包层设计、提高增殖剂富集度和改进氚处理工艺来解决。
 ---
 ### 背景与概念
@@ -11262,7 +9830,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -11288,17 +9856,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>嗯，用户的问题是关于氚在聚变电厂内的安全约束和管理策略，包括多重屏障、滞留物去除、事故缓解措施等，确保氚的释放远低于法规限值。我需要按照之前的指示来组织答案，但首先得理清楚这个问题涉及的关键点。
-首先，氚作为一种放射性物质，它的危险性主要在于其半衰期和对人体的影响。氚的半衰期约为12.3年，会通过辐射对细胞造成损伤。在聚变电厂中，氚被用作燃料，因此如何安全地管理它是一个关键问题。
-接下来，我得考虑多重屏障的设计。通常，聚变装置会有内部屏障、中间屏障和最终屏障。内部屏障可能包括燃料循环系统和真空室，中间屏障可能是保护性吹扫系统，而最终屏障则是厂房的安全壳。这些屏障需要确保在正常运行和事故情况下都能有效隔离氚。
-然后是氚的滞留物去除。在聚变反应中，氚可能会以气体、沉积物或溶胶的形式存在。需要定期清除这些滞留物，以防止积累和潜在的释放。可能的方法包括物理吹扫、化学捕获或高温解吸等。
-事故缓解措施也是关键。事故可能包括设备故障、泄漏或极端事件如失水事故。这些情况下，需要有紧急响应系统，比如自动停堆、隔离系统和高效的过滤系统。此外，监测系统必须实时检测氚的浓度，一旦超过设定阈值立即启动警报和应急程序。
-为了确保氚的释放远低于法规限值，设计时需要考虑多重屏障的可靠性、系统的冗余以及事故条件下的应对能力。法规限值通常以贝克雷每平方米（Bq/m²）或小时平均浓度为单位，因此需要精确的计算和模型来评估各种情况下的释放量，确保即使在最坏情况下，释放量也在允许范围内。
-此外，可能需要进行风险评估和事故模拟，以识别潜在的弱点并优化管理策略。这可能涉及使用概率风险评估（PRA）方法，分析不同事故场景的可能性及其对氚释放的影响。
-最后，我需要确保答案结构符合规范，包含核心结论、背景、原理分析、定量估算、工程意义、比较拓展和总结。但用户现在的问题并没有数值条件，所以可能不需要详细的计算，而是更多地依赖于机制分析和策略描述。
-总的来说，我需要系统地阐述氚的安全管理策略，从屏障设计到事故缓解，再到法规遵守，确保逻辑清晰、结构合理，并且涵盖所有关键点。
-&lt;/think&gt;
-### 核心结论  
+          <t>### 核心结论  
 氚在聚变电厂内的安全约束和管理策略依赖于多重屏障设计、滞留物清除系统以及事故缓解措施，确保氚的释放远低于法规限值（例如，美国法规限值为 $10^6$ Bq/m² 年释放量）。  
 ---
 ### 背景与概念  
@@ -11399,7 +9957,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -11425,16 +9983,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>嗯，这个问题是要比较NbTi和Nb3Sn这两种低温超导材料在聚变磁体中的性能，以及为什么ITER的环向场和中心螺线管会采用Nb3Sn导体。作为聚变等离子体物理与工程的专家，我需要先回顾这两种材料的特性。
-首先，我要回想一下临界电流密度(Jc)的概念。NbTi的Jc在高场下会迅速下降，而Nb3Sn则在更高的磁场下仍有较高的Jc。这可能是因为Nb3Sn的结构不同，或者其临界磁场更高。我需要确认具体的数值，比如NbTi的Jc大约在5-10 kA/cm²，而Nb3Sn则在10-20 kA/cm²以上，特别是在高磁场环境下。
-接着是临界磁场(Bc)，NbTi的Bc大约在15-20 T，而Nb3Sn则可以达到20-30 T以上。考虑到ITER需要的磁场强度很高，特别是环向场和中心螺线管，可能需要更高的临界磁场，所以Nb3Sn更适合。
-然后是应变敏感性，NbTi对机械应变比较敏感，容易导致性能下降，而Nb3Sn在这方面表现更好。这可能意味着在制造过程中，Nb3Sn的处理更容易，或者在运行中更稳定，不易因为应力而失效。
-制造成本方面，Nb3Sn的制造工艺复杂，涉及到Nb和Sn的反应，可能需要高温处理，所以成本较高。而NbTi则相对简单，成本较低。但是考虑到材料的性能，即使成本高，如果性能更好，可能还是值得投资。
-为什么ITER会采用Nb3Sn？可能是因为ITER的磁体需要在高磁场和高温（相对低温来说）下运行，而Nb3Sn的高Jc和高Bc使其更适合这样的环境。此外，ITER的目标是实现长时间的稳态运行，这可能需要更稳定的材料，而Nb3Sn在应变和稳定性方面可能表现更好。
-不过，我可能需要查阅具体的数据来确认这些点，比如具体的Jc和Bc数值，以及制造工艺的成本比较。可能还要考虑Nb3Sn在制造过程中的挑战，比如反应过程中的控制和材料的稳定性。
-总结一下，Nb3Sn在临界电流密度、临界磁场和应变敏感性上都优于NbTi，尽管制造成本更高，但为了满足ITER的高磁场需求和长期运行的稳定性，选择Nb3Sn是合理的。
-&lt;/think&gt;
-### 比较分析NbTi和Nb₃Sn低温超导材料在聚变磁体应用中的主要性能特点和制造成本
+          <t>### 比较分析NbTi和Nb₃Sn低温超导材料在聚变磁体应用中的主要性能特点和制造成本
 #### 1. **核心结论**
 ITER的环向场（TF）和中心螺线管（CS）磁体采用Nb₃Sn导体，主要是因为其在高磁场和高温（相对低温）环境下的优异性能，尽管制造成本较高。
 #### 2. **背景与概念**
@@ -11453,7 +10002,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -11479,17 +10028,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>好吧，我现在得解释一下CICC的设计原理以及它在聚变装置中的应用优势，还要分析它在热工水力和电磁力学方面遇到的挑战。我对CICC不是很了解，所以得先弄清楚什么是CICC。CICC应该是某种电缆的名称，可能和超导体有关，因为聚变装置通常使用超导磁体。
-首先，CICC可能指的是“Composite Internal Conductor Cable”，或者类似的复合内部导体电缆。既然是用于聚变装置，尤其是像ITER这样的大型装置，那它应该具备高载流能力，因为这些磁体需要产生强大的磁场来约束等离子体。高载流能力意味着在高温或高压下仍能有效传导电流，可能涉及超导材料。
-接下来，良好的稳定性和机械强度也很重要。聚变装置的运行环境非常苛刻，电磁力和机械应力都会很大。所以，CICC需要有足够的结构来承受这些应力，同时保持稳定的性能，防止热机械故障的发生。
-在设计上，CICC可能采用了多层结构，内部是超导体，外部有多种绝缘层和支撑结构。这样的结构可以提高导电性能，同时提供良好的热传导，便于冷却系统的工作。冷却系统对于超导体来说至关重要，因为超导材料需要在极低的温度下才能工作，所以设计中可能有液氮或其他冷却剂的流动通道。
-说到热工水力挑战，我想到的是冷却系统的效率和热流管理。如果电流过大，可能会导致局部过热，影响超导体的性能，甚至引发故障。因此，设计时需要确保冷却系统能够及时带走热量，维持合适的温度梯度。这可能涉及到流体动力学的计算，以确保冷却剂的流动效率和散热效果。
-电磁力学方面的挑战可能包括电磁力的分布和应力的管理。在高电流密度下，电磁力可能非常大，导致导体变形或损坏。设计时需要计算这些力，并确保结构能够承受这些应力，可能需要使用高强度的材料，并优化结构以分散应力。
-另外，材料的选择也很关键。CICC可能使用了特定的超导材料，如高温超导体或低温超导体，每种材料都有其优缺点，需要根据具体应用环境来选择。同时，材料的兼容性也很重要，确保各个层之间的界面不会产生额外的应力或热损失。
-在实际应用中，CICC的设计还需要考虑制造工艺的可行性。复杂的多层结构可能需要高精度的制造技术，材料的选择也需要考虑到加工成本和难度。
-总结一下，CICC的设计需要综合考虑电、热、机械等多个方面的因素，平衡性能与成本，确保在极端环境下的可靠运行。这可能涉及到多物理场的建模和仿真，以验证设计的可行性和优化各个参数。
-&lt;/think&gt;
-### 管内电缆导体（CICC）的设计原理及其应用优势
+          <t>### 管内电缆导体（CICC）的设计原理及其应用优势
 #### 核心结论
 CICC（管内电缆导体）是一种高性能超导电缆，广泛应用于大型聚变磁体中，具有高载流能力、良好的稳定性和机械强度，但也面临热工水力和电磁力学方面的挑战。
 #### 背景与概念
@@ -11517,7 +10056,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -11543,15 +10082,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>嗯，我现在要讨论高温超导材料，特别是REBCO，在聚变磁体中的应用潜力。用户还提到了HTS磁体相对于LTS的优势，以及CFS公司的突破性进展。
-首先，高温超导材料与低温超导材料相比，最大的优势肯定是运行温度更高，这样制冷成本更低。HTS的工作温度通常在液氮温度，也就是77K左右，而LTS需要更低的温度，比如4K或更低。液氮比液氦更容易获得，成本也更低，这肯定是个大优势。
-然后，磁场强度方面，HTS材料的临界磁场更高，这意味着在相同条件下，可以产生更强的磁场。这对于聚变反应堆来说非常重要，因为更强的磁场可以更好地约束等离子体，提高反应效率。
-还有，设计更紧凑。HTS材料在相同磁场下可以有更高的电流密度，所以磁体的体积可以更小，整体设计更紧凑。这对于托卡马克这类装置来说，空间利用更高效，结构设计也更灵活。
-再来看CFS公司的突破。他们可能在材料性能、工程应用、制冷技术等方面有所突破。比如，REBCO带材的性能提升，临界电流更高，临界磁场更好，这样磁体性能更优。工程应用方面，可能开发了新型的HTS磁体结构，更适合聚变装置的需求。制冷技术上，可能开发了高效的制冷系统，降低成本，提高可靠性。
-不过，HTS磁体也面临一些挑战。材料的稳定性和可靠性需要进一步验证，运行中的动态行为可能需要更深入的研究。制造成本目前较高，大规模应用可能受限，未来需要优化制造工艺，降低成本。
-总结一下，HTS在聚变磁体中的优势很明显，特别是在制冷成本、磁场强度和设计紧凑性上。而CFS公司的突破可能集中在材料性能、工程应用和制冷技术上，推动HTS磁体在聚变装置中的应用。当然，这些突破还需要进一步验证和推广。
-&lt;/think&gt;
-### 高温超导（HTS）材料在聚变磁体中的潜力
+          <t>### 高温超导（HTS）材料在聚变磁体中的潜力
 #### 1. 核心结论
 高温超导（HTS）材料如REBCO（稀土钡铜氧化物）在聚变磁体中具有显著潜力，主要优势在于更高的运行温度、更强的磁场和更紧凑的设计，有望显著降低制冷成本并提高装置性能。
 ---
@@ -11591,7 +10122,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -11617,17 +10148,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>嗯，这个问题是关于ITER的大型低温系统的，我需要详细描述它的主要组成部分、功能，以及温度水平和制冷功率。同时，还要分析运行中面临的挑战，比如动态热负荷。
-首先，了解ITER的低温系统是为了冷却超导磁体和其他设备，确保它们在超导状态下工作。主要组成包括氦制冷机、液氮预冷系统、低温分配系统和过冷氦循环。这些部分各自有不同的功能。
-氦制冷机是核心，提供冷量，分为冷头部分和压缩机部分。冷头使用膨胀机或节流阀来降温，压缩机则负责循环氦气。温度要达到1.4K，制冷功率约50MW。
-液氮预冷系统作为预冷阶段，将氦气从环境温度降到70K，使用液氮作为冷源，节省能量。
-低温分配系统负责将冷量分配到各设备，维持温度稳定，避免振动，保持氦气过冷状态。
-过冷氦循环则进一步降低温度到1.4K以下，过冷度通常为0.3-0.5K，提升冷却效率。
-运行挑战方面，动态热负荷是关键问题。ITER脉冲式运行会产生周期性热波动，尤其是磁体和校正线圈的耗散功率，可能导致局部温度波动。瞬态热负荷可能影响超导性能，需要精确控制和快速响应的控制系统。
-此外，系统复杂性也是一大挑战，涉及多个子系统，需要协调运行，确保稳定性和可靠性。氦气的泄漏风险和长期运行的维护也是一个问题，需要可靠的设计和监控机制。
-总结下来，设计和运行ITER的低温系统需要综合考虑热管理、系统集成、控制策略和材料选择，以应对这些挑战。
-&lt;/think&gt;
-### ITER大型低温系统的主要组成和功能
+          <t>### ITER大型低温系统的主要组成和功能
 #### 1. 核心结论
 ITER的低温系统由氦制冷机、液氮预冷系统、低温分配系统和过冷氦循环组成，需将超导磁体冷却至1.4 K，总制冷功率约50 MW，面临动态热负荷、系统复杂性和维护挑战。
 ---
@@ -11668,7 +10189,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -11694,15 +10215,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>嗯，我现在要解决的问题是关于超导磁体的失超现象，解释它的发生机制和潜在危害，以及聚变装置中常用的失超检测技术和保护策略。
-首先，我需要明确什么是失超现象。超导磁体在正常工作时处于超导状态，电阻为零。如果发生失超，电阻会突然增加，导致大量焦耳热的产生，可能损坏磁体甚至整个装置。
-接下来，我要分析失超的发生机制。可能的原因有很多，比如局部温度升高、磁场或电流波动、杂质进入等。这些因素会导致某些区域的超导体失去超导特性，进而影响整个磁体。
-然后，潜在的危害包括热损伤和机械应力。热损伤是因为失超时产生的热量无法及时散去，导致温度升高，可能破坏材料结构。机械应力是因为电流在失超时突然变化，产生电磁力，可能造成结构损坏。
-关于检测技术和保护策略，我需要列举几种常用的方法。例如，电压监测和超导线的电阻监测可以帮助及时发现失超。保护策略包括快速放电、使用淬火加热器等，这些方法可以在失超发生后迅速采取措施，减少损坏。
-在推导过程中，我需要考虑具体的工作条件，如电流变化率和磁场强度等参数，这些都会影响失超的发生和应对措施的有效性。同时，我还需要引用相关的公式和理论，如欧姆定律，来说明热量产生的机制。
-最后，我需要总结这些技术如何协同工作，确保超导磁体的安全运行，避免重大事故的发生。
-&lt;/think&gt;
-### 什么是超导磁体的失超（quench）现象？
+          <t>### 什么是超导磁体的失超（quench）现象？
 **核心结论**  
 超导磁体的失超是指超导体在受到扰动后失去超导特性，电阻骤然升高的现象。这种转变可能导致磁体迅速加热，甚至损坏装置。
 #### **背景与概念**
@@ -11778,7 +10291,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -11804,15 +10317,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>嗯，用户问的是关于大型高场超导聚变磁体在制造和装配过程中的主要工程挑战，特别是像ITER的TF线圈这样的装置。首先，我得先理解用户的问题背景。用户可能是一位聚变物理或工程领域的学生，或者是刚进入该领域的研究人员，想要了解ITER这样的装置在制造过程中遇到的具体困难。
-接下来，我需要分解问题，看看用户提到了哪些具体挑战：导体接头、绕组精度、绝缘、支撑结构、电磁力处理。这些确实是制造过程中的关键点，但可能还有其他因素需要考虑。例如，冷却系统、振动控制、装配过程中的精度维持等。
-然后，我要逐一分析每个挑战。导体接头部分，超导材料在极端低温下工作，接头必须保证低电阻，否则会引发局部加热，影响性能。绕组精度方面，ITER的线圈非常大，绕制时需要极高的精度，否则可能在运行时产生应力，影响结构完整性。绝缘材料需要在低温和强电磁环境下保持性能，同时还要有足够的机械强度，这相当有挑战性。
-支撑结构设计必须能够承受巨大的电磁力，这些力在设备运行时可能达到兆牛级别，设计不当会导致结构变形甚至失效。电磁力处理方面，除了结构设计，还需要通过优化电流分布和磁场形状来减小电磁力，这涉及到复杂的数值模拟和实验验证。
-此外，冷却系统的设计和可靠性也是关键，因为超导磁体需要在液氦温度下运行，任何冷却故障都会导致失超，造成严重后果。装配过程中的振动控制和质量保证也是不可忽视的，特别是在处理如此庞大的结构时，稍有不慎就可能导致不可逆的损坏。
-现在，我要把这些思考整理成一个连贯的回答，确保涵盖所有主要挑战，并提供相应的技术难点和解决方案。同时，要使用用户提供的答题规范，分点论述，每部分都要有明确的结构和内容，避免遗漏重要信息。
-最后，我需要确保语言清晰，逻辑严谨，符合学术规范，同时让读者能够理解每个挑战的重要性和应对措施。这可能涉及到引用一些已有的研究或工程实践，以增强回答的可信度。
-&lt;/think&gt;
-### 大型、高场超导聚变磁体的制造与装配挑战
+          <t>### 大型、高场超导聚变磁体的制造与装配挑战
 #### 1. 核心结论  
 大型、高场超导聚变磁体（如ITER托卡马克的TF线圈）的制造与装配面临多重复杂工程挑战，包括高精度绕制、超低温绝缘性能、巨大电磁力的承受与平衡、导体接头的低电阻特性以及整体结构的稳定性。
 ---
@@ -11871,7 +10376,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -11897,14 +10402,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>好的，我现在需要回答关于ITER的中心螺线管（CS）的关键作用，以及为什么采用分模块设计，同时讨论其结构和运行面临的挑战。作为聚变等离子体物理与工程的专家，我得详细分析这些问题。
-首先，中心螺线管CS的关键作用。等离子体在托卡马克中的电流驱动是维持等离子体稳定和加热的关键因素。CS通过外部电磁感应来驱动等离子体电流。这涉及到法拉第电磁感应定律，CS的通断会产生变化的磁场，从而在等离子体中感应电动势，进而驱动电流。
-接下来，为什么CS采用分模块设计。这可能与制造和工程上的考虑有关。ITER的CS非常庞大，单个线圈可能难以制造，因此分成多个模块，每个模块可以独立制造和测试，然后组装起来。此外，分模块设计可能允许在运行中独立控制各部分，提高灵活性和安全性，比如在故障发生时，可以单独断开某个模块而不是整个系统。
-关于结构和运行的挑战，尺寸和重量是一个大问题。CS的巨大尺寸需要强大的支撑结构，同时材料的选择必须考虑到高温、高磁场和辐射环境的影响。此外，CS的运行会产生巨大的电磁力，需要确保结构能够承受这些力，同时避免振动和位移导致的损害。冷却系统也是一个挑战，CS需要高效的冷却以防止过热，这涉及到复杂的流体动力学和热管理。
-还有一个是精确控制电流和磁场的问题。由于CS在产生变化磁场时，任何不精确都可能影响等离子体的稳定性，因此控制系统的精度和可靠性至关重要。此外，维护和诊断也是一个挑战，因为CS位于ITER装置的中心，维护困难，诊断设备需要能够实时监测CS的状态，确保其正常运行。
-综上所述，CS在ITER中起着关键的等离子体电流驱动和维持作用，分模块设计提供了制造和操作的便利，但也带来了制造、结构支撑、电磁力、热管理、控制系统、维护和诊断等多方面的挑战。这些都需要在设计和运行过程中仔细考虑和解决。
-&lt;/think&gt;
-### ITER中心螺线管的关键作用及其设计挑战
+          <t>### ITER中心螺线管的关键作用及其设计挑战
 #### 核心结论
 ITER的中心螺线管（CS）通过电磁感应驱动和维持等离子体电流，采用分模块设计以解决制造和运行难题，同时面临巨大的结构、电磁和热管理挑战。
 #### 背景与概念
@@ -11934,7 +10432,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -11960,16 +10458,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>嗯，我现在得讨论聚变堆中超导磁体的辐射屏蔽的重要性，特别是中子和伽马射线对超导材料，特别是绝缘材料的损伤效应，以及如何设计有效的屏蔽系统来保护磁体。
-首先，聚变堆里的超导磁体很关键，因为它们负责产生强磁场来约束等离子体。但聚变反应会产生大量中子和伽马射线，这些辐射会对磁体造成损害，影响它们的性能，甚至导致故障。
-中子和伽马射线的损伤效应可能包括辐射硬化、材料脆化、性能下降以及绝缘材料的介电性能退化。这些效应会导致磁体的超导性能下降，电阻增加，甚至可能引发失超现象，影响整个聚变堆的稳定运行。
-所以，设计有效的屏蔽系统非常重要。屏蔽系统的主要目标是减少辐射对磁体的照射。可能需要多重屏蔽结构，首先是中子屏蔽层，其次是伽马屏蔽层，再加上可能的反射层。材料选择方面，中子屏蔽可能需要高原子序数的材料，比如铅或铁，而伽马屏蔽则需要高密度、高原子序数的材料，比如钨或钽。
-同时，屏蔽设计还必须考虑到聚变堆的整体布局，确保屏蔽层的位置、厚度和材料不会对其他系统造成过多负担或干扰。
-可能还需要考虑屏蔽层对磁场的影响，确保磁体的性能不会因为屏蔽层的存在而显著降低。
-此外，可能需要进行详细的辐射传输模拟和热分析，以优化屏蔽设计，确保在屏蔽效率和工程可行性的平衡点。
-总的来说，设计有效的屏蔽系统需要综合考虑多种因素，包括辐射类型、材料性能、工程布局和磁场影响等，以保护超导磁体免受辐射损伤，确保聚变堆的安全和高效运行。
-&lt;/think&gt;
-### 超导磁体辐射屏蔽的重要性
+          <t>### 超导磁体辐射屏蔽的重要性
 **核心结论**：超导磁体的辐射屏蔽是聚变堆设计中的关键环节，需综合考虑中子和伽马射线的损伤效应，并通过合理的屏蔽材料和结构设计来保护磁体，确保其长期稳定运行。
 #### 背景与概念
 在聚变堆中，超导磁体用于产生强磁场以约束高温等离子体。然而，聚变反应会产生大量中子和伽马射线，这些辐射对超导材料及其绝缘层有显著的损伤效应。因此，设计有效的辐射屏蔽系统至关重要，以保护磁体免受辐射损伤，维持其超导性能。
@@ -12012,7 +10501,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -12038,19 +10527,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>好，我现在要解决的是关于未来商业聚变堆中超导磁体系统成本降低的可能途径。这个问题涉及到材料选择、导体设计、制造工艺和系统集成等多个方面，每个方面都需要深入分析和探讨。
-首先，我需要明确当前超导磁体系统的主要成本构成。材料成本是一个重要因素，尤其是超导材料和绝缘材料。此外，导体的制造工艺复杂，涉及多步骤的处理，这也增加了成本。系统集成部分，包括磁体系统的整体设计和维护，也是成本的重要组成部分。
-接下来，从材料选择的角度来看，目前广泛使用的超导材料是Nb3Sn和高温超导体（HTS）。Nb3Sn虽然性能稳定，但制造成本较高，而HTS虽然成本较高，但有潜力降低整体系统成本。因此，寻找更经济的超导材料或优化现有材料的制造工艺是一个重要的方向。
-在导体设计方面，导体的结构直接影响到其性能和成本。传统的圆缆导体结构复杂，制造成本高。而新型的复合材料结构，如带状或块状结构，可以简化制造工艺，降低成本。同时，优化导体的几何形状，提高其电流承载能力，也可以减少所需导体的总量，从而降低成本。
-制造工艺方面，现有工艺复杂，步骤多，成本高。改进制造工艺，例如采用自动化生产，可以提高生产效率，降低成本。此外，简化制造步骤，减少材料浪费，也是降低成本的有效途径。
-在系统集成方面，磁体系统的整体设计和维护成本也是一笔不小的开支。优化磁体系统的结构设计，提高其可靠性和可维护性，可以降低维护成本。同时，采用模块化设计，使系统更容易组装和维修，也是降低成本的一个方向。
-综上所述，降低超导磁体系统成本的可能途径包括：优化超导材料的选择和制造工艺，改进导体设计以提高性能和降低成本，简化制造工艺以提高生产效率，以及优化系统集成设计以降低整体维护和运营成本。
-现在，我需要逐一分析这些途径，并结合具体的实施方法，探讨其可行性和潜在效果。同时，还需要考虑这些改进措施对聚变装置性能的影响，确保成本降低的同时，不影响磁体系统的性能和可靠性。
-在实施过程中，可能会遇到一些挑战。例如，寻找更经济的超导材料可能需要进行大量的研发和测试，而优化导体设计和制造工艺也可能面临技术上的难题。此外，系统集成的优化需要综合考虑多个因素，确保各个子系统的协调工作。
-因此，为了实现成本的有效降低，需要在材料、设计、制造和系统集成等多个方面进行综合考虑和协同优化。同时，还需要加强研发，推动技术创新，以实现成本与性能的双重提升。
-总的来说，降低超导磁体系统成本是一个系统性的工程，需要从多个角度入手，进行深入研究和实践，才能实现目标。
-&lt;/think&gt;
-降低未来商业聚变堆中超导磁体系统成本的关键途径可以从材料选择、导体设计、制造工艺和系统集成等方面进行探讨。以下是对这些方面的详细分析：
+          <t>降低未来商业聚变堆中超导磁体系统成本的关键途径可以从材料选择、导体设计、制造工艺和系统集成等方面进行探讨。以下是对这些方面的详细分析：
 ### 1. 材料选择
 **背景与概念：**
 超导磁体系统主要使用Nb3Sn和高温超导体（HTS）作为超导材料。这些材料的性能和成本直接影响磁体系统的整体成本。
@@ -12120,7 +10597,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -12146,17 +10623,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>好的，我现在要解答的问题是关于仿星器磁体系统设计的挑战以及如何应对这些挑战。首先，我需要理解仿星器和托卡马克在磁体系统上的主要区别。仿星器的磁体系统比托卡马克更复杂和三维化，这可能涉及到更多的线圈和更复杂的磁场结构。这样的设计带来了哪些特殊挑战呢？
-首先，我想到材料和制造上的挑战。仿星器的线圈可能需要更复杂的形状和更精确的制造工艺。托卡马克的线圈相对简单，而仿星器的线圈可能更弯曲，三维结构更复杂，这会增加制造难度。此外，超导材料在复杂形状下的性能可能受到影响，比如应力和变形可能导致超导临界温度下降，甚至出现失超的情况。
-接下来，结构应力分析也是一个挑战。三维化的磁体系统可能在不同的载荷条件下承受更大的应力。常规的结构分析方法可能不够，需要更复杂的计算工具，比如有限元分析，来精确评估各个线圈的应力分布情况。如何优化结构设计以降低应力，同时满足磁场的需求，是一个需要解决的问题。
-控制和校正也是一个重要方面。仿星器的磁场需要精确控制，以确保等离子体的稳定性和约束性能。由于磁场的复杂性，可能需要更多的控制线圈，并开发更精确的反馈控制系统，这增加了控制的复杂性。此外，在运行过程中，磁场可能会发生变化，需要有效的诊断和实时校正机制。
-然后是冷却和维护的问题。超导磁体需要在极低温度下运行，而复杂化的线圈可能增加冷却系统的复杂性。如何确保冷却剂能够有效覆盖所有线圈，同时避免泄漏和其他故障，是一个需要解决的问题。维护方面，由于结构复杂，维修和更换线圈可能更加困难，需要设计易于维护的结构。
-现在，关于如何利用先进的计算工具和制造技术来应对这些挑战。材料科学方面，研发更高强度、更好导电性的超导材料，可以在不影响性能的情况下，提高线圈的承受能力。在制造技术上，采用3D打印技术可以制造复杂的形状，保证高精度，同时通过模拟制造过程，优化工艺参数，减少缺陷。
-计算工具方面，多物理场耦合仿真可以同时考虑磁场、电流分布、温度变化和结构应力，提供更全面的分析。这对于优化设计和预测潜在问题非常重要。有限元分析在结构力学中的应用，可以更精确地评估各个部分的应力，帮助设计更稳健的结构。先进算法的优化工具可以用来优化线圈的形状和布局，以达到最佳的磁场性能，同时降低材料用量和成本。
-制造技术的进步，如智能机器人和自动化系统，可以提高制造精度和效率，减少人为误差。数字化设计和虚拟样机的使用，可以在实际制造之前进行多次模拟和优化，降低试错成本。
-总结一下，仿星器的磁体系统确实面临许多挑战，但通过先进的材料、制造技术和计算工具，我们可以逐步克服这些问题，推动仿星器技术的发展。
-&lt;/think&gt;
-仿星器的磁体系统设计面临多重复杂挑战，但利用先进的技术和工具可以有效应对这些挑战。以下是逐步解决方案：
+          <t>仿星器的磁体系统设计面临多重复杂挑战，但利用先进的技术和工具可以有效应对这些挑战。以下是逐步解决方案：
 ### 1. **材料与制造挑战**
    - **材料性能**：开发更高强度和更好导电性的超导材料，如高温超导体（HTS），以提高线圈的稳定性和可靠性。
    - **制造工艺**：采用3D打印技术，制造复杂形状的超导线圈，确保高精度和复杂结构的一次成型。使用计算机辅助设计（CAD）进行精确建模，优化线圈设计，减少材料浪费。

</xml_diff>